<commit_message>
feat: Update IPP Excel template for improved functionality
</commit_message>
<xml_diff>
--- a/public/assets/file/Template IPP.xlsx
+++ b/public/assets/file/Template IPP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\core\public\assets\file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88228A04-1A8E-47FF-8B5D-D3CD159DCBEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73DFC3D9-D14E-46E1-884B-8665C0D4D4D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -205,7 +205,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="43">
+  <borders count="44">
     <border>
       <left/>
       <right/>
@@ -679,11 +679,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="132">
+  <cellXfs count="130">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -815,113 +824,9 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="5" fillId="3" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="5" fillId="3" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="3" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="6" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -943,27 +848,129 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="17" fontId="6" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="17" fontId="6" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="17" fontId="6" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="5" fillId="3" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="3" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="5" fillId="3" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1259,7 +1266,7 @@
   <dimension ref="A1:BU1000"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="AA4" sqref="AA4:AC4"/>
+      <selection activeCell="U9" sqref="U9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1273,229 +1280,134 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:73" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="76" t="s">
+      <c r="A1" s="104" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="59"/>
-      <c r="F1" s="59"/>
-      <c r="G1" s="59"/>
-      <c r="H1" s="59"/>
-      <c r="I1" s="59"/>
-      <c r="J1" s="59"/>
-      <c r="K1" s="59"/>
-      <c r="L1" s="59"/>
-      <c r="M1" s="59"/>
-      <c r="N1" s="59"/>
-      <c r="O1" s="59"/>
-      <c r="P1" s="59"/>
-      <c r="Q1" s="59"/>
-      <c r="R1" s="59"/>
-      <c r="S1" s="59"/>
-      <c r="T1" s="59"/>
-      <c r="U1" s="59"/>
-      <c r="V1" s="59"/>
-      <c r="W1" s="59"/>
-      <c r="X1" s="59"/>
-      <c r="Y1" s="59"/>
-      <c r="Z1" s="59"/>
-      <c r="AA1" s="59"/>
-      <c r="AB1" s="59"/>
-      <c r="AC1" s="59"/>
-      <c r="AD1" s="59"/>
-      <c r="AE1" s="59"/>
-      <c r="AF1" s="59"/>
-      <c r="AG1" s="59"/>
-      <c r="AH1" s="59"/>
-      <c r="AI1" s="59"/>
-      <c r="AJ1" s="59"/>
-      <c r="AK1" s="59"/>
-      <c r="AL1" s="59"/>
-      <c r="AM1" s="59"/>
-      <c r="AN1" s="59"/>
-      <c r="AO1" s="59"/>
-      <c r="AP1" s="59"/>
-      <c r="AQ1" s="59"/>
-      <c r="AR1" s="59"/>
-      <c r="AS1" s="59"/>
-      <c r="AT1" s="59"/>
-      <c r="AU1" s="59"/>
-      <c r="AV1" s="59"/>
-      <c r="AW1" s="59"/>
-      <c r="AX1" s="59"/>
-      <c r="AY1" s="59"/>
-      <c r="AZ1" s="59"/>
-      <c r="BA1" s="60"/>
+      <c r="B1" s="92"/>
+      <c r="C1" s="92"/>
+      <c r="D1" s="92"/>
+      <c r="E1" s="92"/>
+      <c r="F1" s="92"/>
+      <c r="G1" s="92"/>
+      <c r="H1" s="92"/>
+      <c r="I1" s="92"/>
+      <c r="J1" s="92"/>
+      <c r="K1" s="92"/>
+      <c r="L1" s="92"/>
+      <c r="M1" s="92"/>
+      <c r="N1" s="92"/>
+      <c r="O1" s="92"/>
+      <c r="P1" s="92"/>
+      <c r="Q1" s="92"/>
+      <c r="R1" s="92"/>
+      <c r="S1" s="92"/>
+      <c r="T1" s="92"/>
+      <c r="U1" s="92"/>
+      <c r="V1" s="92"/>
+      <c r="W1" s="92"/>
+      <c r="X1" s="92"/>
+      <c r="Y1" s="92"/>
+      <c r="Z1" s="92"/>
+      <c r="AA1" s="92"/>
+      <c r="AB1" s="92"/>
+      <c r="AC1" s="92"/>
+      <c r="AD1" s="92"/>
+      <c r="AE1" s="92"/>
+      <c r="AF1" s="92"/>
+      <c r="AG1" s="92"/>
+      <c r="AH1" s="92"/>
+      <c r="AI1" s="92"/>
+      <c r="AJ1" s="92"/>
+      <c r="AK1" s="92"/>
+      <c r="AL1" s="92"/>
+      <c r="AM1" s="92"/>
+      <c r="AN1" s="92"/>
+      <c r="AO1" s="92"/>
+      <c r="AP1" s="92"/>
+      <c r="AQ1" s="92"/>
+      <c r="AR1" s="92"/>
+      <c r="AS1" s="92"/>
+      <c r="AT1" s="92"/>
+      <c r="AU1" s="92"/>
+      <c r="AV1" s="92"/>
+      <c r="AW1" s="92"/>
+      <c r="AX1" s="92"/>
+      <c r="AY1" s="92"/>
+      <c r="AZ1" s="92"/>
+      <c r="BA1" s="105"/>
     </row>
     <row r="2" spans="1:73" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="77" t="s">
+      <c r="A2" s="106" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="62"/>
-      <c r="C2" s="62"/>
-      <c r="D2" s="62"/>
-      <c r="E2" s="62"/>
-      <c r="F2" s="62"/>
-      <c r="G2" s="62"/>
-      <c r="H2" s="62"/>
-      <c r="I2" s="62"/>
-      <c r="J2" s="62"/>
-      <c r="K2" s="62"/>
-      <c r="L2" s="62"/>
-      <c r="M2" s="62"/>
-      <c r="N2" s="62"/>
-      <c r="O2" s="62"/>
-      <c r="P2" s="62"/>
-      <c r="Q2" s="62"/>
-      <c r="R2" s="62"/>
-      <c r="S2" s="62"/>
-      <c r="T2" s="62"/>
-      <c r="U2" s="62"/>
-      <c r="V2" s="62"/>
-      <c r="W2" s="62"/>
-      <c r="X2" s="62"/>
-      <c r="Y2" s="62"/>
-      <c r="Z2" s="62"/>
-      <c r="AA2" s="62"/>
-      <c r="AB2" s="62"/>
-      <c r="AC2" s="62"/>
-      <c r="AD2" s="62"/>
-      <c r="AE2" s="62"/>
-      <c r="AF2" s="62"/>
-      <c r="AG2" s="62"/>
-      <c r="AH2" s="62"/>
-      <c r="AI2" s="62"/>
-      <c r="AJ2" s="62"/>
-      <c r="AK2" s="62"/>
-      <c r="AL2" s="62"/>
-      <c r="AM2" s="62"/>
-      <c r="AN2" s="62"/>
-      <c r="AO2" s="62"/>
-      <c r="AP2" s="62"/>
-      <c r="AQ2" s="62"/>
-      <c r="AR2" s="62"/>
-      <c r="AS2" s="62"/>
-      <c r="AT2" s="62"/>
-      <c r="AU2" s="62"/>
-      <c r="AV2" s="62"/>
-      <c r="AW2" s="62"/>
-      <c r="AX2" s="62"/>
-      <c r="AY2" s="62"/>
-      <c r="AZ2" s="62"/>
-      <c r="BA2" s="63"/>
+      <c r="B2" s="79"/>
+      <c r="C2" s="79"/>
+      <c r="D2" s="79"/>
+      <c r="E2" s="79"/>
+      <c r="F2" s="79"/>
+      <c r="G2" s="79"/>
+      <c r="H2" s="79"/>
+      <c r="I2" s="79"/>
+      <c r="J2" s="79"/>
+      <c r="K2" s="79"/>
+      <c r="L2" s="79"/>
+      <c r="M2" s="79"/>
+      <c r="N2" s="79"/>
+      <c r="O2" s="79"/>
+      <c r="P2" s="79"/>
+      <c r="Q2" s="79"/>
+      <c r="R2" s="79"/>
+      <c r="S2" s="79"/>
+      <c r="T2" s="79"/>
+      <c r="U2" s="79"/>
+      <c r="V2" s="79"/>
+      <c r="W2" s="79"/>
+      <c r="X2" s="79"/>
+      <c r="Y2" s="79"/>
+      <c r="Z2" s="79"/>
+      <c r="AA2" s="79"/>
+      <c r="AB2" s="79"/>
+      <c r="AC2" s="79"/>
+      <c r="AD2" s="79"/>
+      <c r="AE2" s="79"/>
+      <c r="AF2" s="79"/>
+      <c r="AG2" s="79"/>
+      <c r="AH2" s="79"/>
+      <c r="AI2" s="79"/>
+      <c r="AJ2" s="79"/>
+      <c r="AK2" s="79"/>
+      <c r="AL2" s="79"/>
+      <c r="AM2" s="79"/>
+      <c r="AN2" s="79"/>
+      <c r="AO2" s="79"/>
+      <c r="AP2" s="79"/>
+      <c r="AQ2" s="79"/>
+      <c r="AR2" s="79"/>
+      <c r="AS2" s="79"/>
+      <c r="AT2" s="79"/>
+      <c r="AU2" s="79"/>
+      <c r="AV2" s="79"/>
+      <c r="AW2" s="79"/>
+      <c r="AX2" s="79"/>
+      <c r="AY2" s="79"/>
+      <c r="AZ2" s="79"/>
+      <c r="BA2" s="80"/>
     </row>
     <row r="3" spans="1:73" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="V3" s="130" t="s">
+      <c r="V3" s="71" t="s">
         <v>28</v>
       </c>
-      <c r="W3" s="126"/>
-      <c r="X3" s="126"/>
-      <c r="Y3" s="126"/>
-      <c r="Z3" s="126"/>
-      <c r="AA3" s="126"/>
-      <c r="AB3" s="126"/>
-      <c r="AC3" s="126"/>
-      <c r="AD3" s="126"/>
-      <c r="AE3" s="126"/>
-      <c r="AF3" s="126"/>
-      <c r="AG3" s="126"/>
-      <c r="AH3" s="126"/>
-      <c r="AI3" s="126"/>
-      <c r="AJ3" s="126"/>
-      <c r="AK3" s="126"/>
-      <c r="AL3" s="126"/>
-      <c r="AM3" s="126"/>
-      <c r="AN3" s="126"/>
-      <c r="AO3" s="126"/>
-      <c r="AP3" s="126"/>
-      <c r="AQ3" s="126"/>
-      <c r="AR3" s="126"/>
-      <c r="AS3" s="126"/>
-      <c r="AT3" s="126"/>
-      <c r="AU3" s="126"/>
-      <c r="AV3" s="126"/>
-      <c r="AW3" s="126"/>
-      <c r="AX3" s="126"/>
-      <c r="AY3" s="126"/>
-      <c r="AZ3" s="126"/>
-      <c r="BA3" s="126"/>
-      <c r="BB3" s="126"/>
-      <c r="BC3" s="126"/>
-      <c r="BD3" s="126"/>
-      <c r="BE3" s="126"/>
-      <c r="BF3" s="126"/>
-      <c r="BG3" s="126"/>
-      <c r="BH3" s="126"/>
-      <c r="BI3" s="126"/>
-      <c r="BJ3" s="126"/>
-      <c r="BK3" s="126"/>
-      <c r="BL3" s="126"/>
-      <c r="BM3" s="126"/>
-      <c r="BN3" s="126"/>
-      <c r="BO3" s="126"/>
-      <c r="BP3" s="126"/>
-      <c r="BQ3" s="126"/>
-      <c r="BR3" s="126"/>
-      <c r="BS3" s="126"/>
-      <c r="BT3" s="126"/>
-      <c r="BU3" s="127"/>
+      <c r="BA3" s="129"/>
+      <c r="BU3" s="55"/>
     </row>
     <row r="4" spans="1:73" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="126"/>
-      <c r="C4" s="126"/>
-      <c r="D4" s="126"/>
-      <c r="E4" s="126"/>
-      <c r="F4" s="126"/>
-      <c r="G4" s="126"/>
-      <c r="H4" s="126"/>
-      <c r="I4" s="126"/>
-      <c r="J4" s="126"/>
-      <c r="K4" s="126"/>
-      <c r="L4" s="126"/>
-      <c r="M4" s="126"/>
-      <c r="N4" s="126"/>
-      <c r="O4" s="126"/>
-      <c r="P4" s="126"/>
-      <c r="Q4" s="126"/>
-      <c r="R4" s="126"/>
-      <c r="S4" s="126"/>
-      <c r="T4" s="126"/>
-      <c r="U4" s="126"/>
-      <c r="V4" s="126"/>
-      <c r="W4" s="128" t="s">
+      <c r="W4" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="X4" s="129"/>
-      <c r="Z4" s="126"/>
-      <c r="AA4" s="131"/>
-      <c r="AB4" s="131"/>
-      <c r="AC4" s="131"/>
-      <c r="AD4" s="126"/>
-      <c r="AE4" s="126"/>
-      <c r="AF4" s="126"/>
-      <c r="AG4" s="126"/>
-      <c r="AH4" s="126"/>
-      <c r="AI4" s="126"/>
-      <c r="AJ4" s="126"/>
-      <c r="AK4" s="126"/>
-      <c r="AL4" s="126"/>
-      <c r="AM4" s="126"/>
-      <c r="AN4" s="126"/>
-      <c r="AO4" s="126"/>
-      <c r="AP4" s="126"/>
-      <c r="AQ4" s="126"/>
-      <c r="AR4" s="126"/>
-      <c r="AS4" s="126"/>
-      <c r="AT4" s="126"/>
-      <c r="AU4" s="126"/>
-      <c r="AV4" s="126"/>
-      <c r="AW4" s="126"/>
-      <c r="AX4" s="126"/>
-      <c r="AY4" s="126"/>
-      <c r="AZ4" s="126"/>
-      <c r="BA4" s="127"/>
+      <c r="AA4" s="72"/>
+      <c r="AB4" s="72"/>
+      <c r="AC4" s="72"/>
+      <c r="BA4" s="55"/>
     </row>
     <row r="5" spans="1:73" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1"/>
@@ -1553,10 +1465,10 @@
       <c r="BA5" s="4"/>
     </row>
     <row r="6" spans="1:73" ht="6" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="78"/>
-      <c r="B6" s="79"/>
-      <c r="C6" s="79"/>
-      <c r="D6" s="79"/>
+      <c r="A6" s="107"/>
+      <c r="B6" s="108"/>
+      <c r="C6" s="108"/>
+      <c r="D6" s="108"/>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
@@ -1608,13 +1520,13 @@
       <c r="BA6" s="6"/>
     </row>
     <row r="7" spans="1:73" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="80" t="s">
+      <c r="A7" s="109" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="62"/>
-      <c r="C7" s="62"/>
-      <c r="D7" s="62"/>
-      <c r="E7" s="62"/>
+      <c r="B7" s="79"/>
+      <c r="C7" s="79"/>
+      <c r="D7" s="79"/>
+      <c r="E7" s="79"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
@@ -1848,10 +1760,10 @@
       <c r="BA10" s="9"/>
     </row>
     <row r="11" spans="1:73" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="81"/>
-      <c r="B11" s="65"/>
-      <c r="C11" s="65"/>
-      <c r="D11" s="65"/>
+      <c r="A11" s="110"/>
+      <c r="B11" s="111"/>
+      <c r="C11" s="111"/>
+      <c r="D11" s="111"/>
       <c r="E11" s="12"/>
       <c r="F11" s="12"/>
       <c r="G11" s="12"/>
@@ -1903,187 +1815,187 @@
       <c r="BA11" s="13"/>
     </row>
     <row r="12" spans="1:73" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="84" t="s">
+      <c r="A12" s="91" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="59"/>
-      <c r="C12" s="59"/>
-      <c r="D12" s="59"/>
-      <c r="E12" s="59"/>
-      <c r="F12" s="59"/>
-      <c r="G12" s="59"/>
-      <c r="H12" s="59"/>
-      <c r="I12" s="59"/>
-      <c r="J12" s="59"/>
-      <c r="K12" s="59"/>
-      <c r="L12" s="59"/>
-      <c r="M12" s="59"/>
-      <c r="N12" s="59"/>
-      <c r="O12" s="59"/>
-      <c r="P12" s="59"/>
-      <c r="Q12" s="94"/>
-      <c r="R12" s="96" t="s">
+      <c r="B12" s="92"/>
+      <c r="C12" s="92"/>
+      <c r="D12" s="92"/>
+      <c r="E12" s="92"/>
+      <c r="F12" s="92"/>
+      <c r="G12" s="92"/>
+      <c r="H12" s="92"/>
+      <c r="I12" s="92"/>
+      <c r="J12" s="92"/>
+      <c r="K12" s="92"/>
+      <c r="L12" s="92"/>
+      <c r="M12" s="92"/>
+      <c r="N12" s="92"/>
+      <c r="O12" s="92"/>
+      <c r="P12" s="92"/>
+      <c r="Q12" s="93"/>
+      <c r="R12" s="97" t="s">
         <v>10</v>
       </c>
-      <c r="S12" s="59"/>
-      <c r="T12" s="94"/>
-      <c r="U12" s="82" t="s">
+      <c r="S12" s="92"/>
+      <c r="T12" s="93"/>
+      <c r="U12" s="112" t="s">
         <v>11</v>
       </c>
-      <c r="V12" s="83"/>
-      <c r="W12" s="83"/>
-      <c r="X12" s="83"/>
-      <c r="Y12" s="83"/>
-      <c r="Z12" s="83"/>
-      <c r="AA12" s="83"/>
-      <c r="AB12" s="83"/>
-      <c r="AC12" s="83"/>
-      <c r="AD12" s="83"/>
-      <c r="AE12" s="83"/>
-      <c r="AF12" s="83"/>
-      <c r="AG12" s="83"/>
-      <c r="AH12" s="83"/>
-      <c r="AI12" s="83"/>
-      <c r="AJ12" s="83"/>
-      <c r="AK12" s="83"/>
-      <c r="AL12" s="83"/>
-      <c r="AM12" s="83"/>
-      <c r="AN12" s="83"/>
-      <c r="AO12" s="83"/>
-      <c r="AP12" s="83"/>
-      <c r="AQ12" s="83"/>
-      <c r="AR12" s="83"/>
-      <c r="AS12" s="83"/>
-      <c r="AT12" s="83"/>
-      <c r="AU12" s="108"/>
-      <c r="AV12" s="107" t="s">
+      <c r="V12" s="113"/>
+      <c r="W12" s="113"/>
+      <c r="X12" s="113"/>
+      <c r="Y12" s="113"/>
+      <c r="Z12" s="113"/>
+      <c r="AA12" s="113"/>
+      <c r="AB12" s="113"/>
+      <c r="AC12" s="113"/>
+      <c r="AD12" s="113"/>
+      <c r="AE12" s="113"/>
+      <c r="AF12" s="113"/>
+      <c r="AG12" s="113"/>
+      <c r="AH12" s="113"/>
+      <c r="AI12" s="113"/>
+      <c r="AJ12" s="113"/>
+      <c r="AK12" s="113"/>
+      <c r="AL12" s="113"/>
+      <c r="AM12" s="113"/>
+      <c r="AN12" s="113"/>
+      <c r="AO12" s="113"/>
+      <c r="AP12" s="113"/>
+      <c r="AQ12" s="113"/>
+      <c r="AR12" s="113"/>
+      <c r="AS12" s="113"/>
+      <c r="AT12" s="113"/>
+      <c r="AU12" s="114"/>
+      <c r="AV12" s="115" t="s">
         <v>12</v>
       </c>
-      <c r="AW12" s="59"/>
-      <c r="AX12" s="59"/>
-      <c r="AY12" s="59"/>
-      <c r="AZ12" s="59"/>
-      <c r="BA12" s="60"/>
+      <c r="AW12" s="92"/>
+      <c r="AX12" s="92"/>
+      <c r="AY12" s="92"/>
+      <c r="AZ12" s="92"/>
+      <c r="BA12" s="105"/>
     </row>
     <row r="13" spans="1:73" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="85"/>
-      <c r="B13" s="86"/>
-      <c r="C13" s="86"/>
-      <c r="D13" s="86"/>
-      <c r="E13" s="86"/>
-      <c r="F13" s="86"/>
-      <c r="G13" s="86"/>
-      <c r="H13" s="86"/>
-      <c r="I13" s="86"/>
-      <c r="J13" s="86"/>
-      <c r="K13" s="86"/>
-      <c r="L13" s="86"/>
-      <c r="M13" s="86"/>
-      <c r="N13" s="86"/>
-      <c r="O13" s="86"/>
-      <c r="P13" s="86"/>
-      <c r="Q13" s="95"/>
-      <c r="R13" s="97"/>
-      <c r="S13" s="86"/>
-      <c r="T13" s="95"/>
-      <c r="U13" s="88" t="s">
+      <c r="A13" s="94"/>
+      <c r="B13" s="95"/>
+      <c r="C13" s="95"/>
+      <c r="D13" s="95"/>
+      <c r="E13" s="95"/>
+      <c r="F13" s="95"/>
+      <c r="G13" s="95"/>
+      <c r="H13" s="95"/>
+      <c r="I13" s="95"/>
+      <c r="J13" s="95"/>
+      <c r="K13" s="95"/>
+      <c r="L13" s="95"/>
+      <c r="M13" s="95"/>
+      <c r="N13" s="95"/>
+      <c r="O13" s="95"/>
+      <c r="P13" s="95"/>
+      <c r="Q13" s="96"/>
+      <c r="R13" s="98"/>
+      <c r="S13" s="95"/>
+      <c r="T13" s="96"/>
+      <c r="U13" s="117" t="s">
         <v>13</v>
       </c>
-      <c r="V13" s="89"/>
-      <c r="W13" s="89"/>
-      <c r="X13" s="89"/>
-      <c r="Y13" s="89"/>
-      <c r="Z13" s="89"/>
-      <c r="AA13" s="89"/>
-      <c r="AB13" s="89"/>
-      <c r="AC13" s="89"/>
-      <c r="AD13" s="89"/>
-      <c r="AE13" s="89"/>
-      <c r="AF13" s="89"/>
-      <c r="AG13" s="89"/>
-      <c r="AH13" s="90"/>
-      <c r="AI13" s="88" t="s">
+      <c r="V13" s="118"/>
+      <c r="W13" s="118"/>
+      <c r="X13" s="118"/>
+      <c r="Y13" s="118"/>
+      <c r="Z13" s="118"/>
+      <c r="AA13" s="118"/>
+      <c r="AB13" s="118"/>
+      <c r="AC13" s="118"/>
+      <c r="AD13" s="118"/>
+      <c r="AE13" s="118"/>
+      <c r="AF13" s="118"/>
+      <c r="AG13" s="118"/>
+      <c r="AH13" s="119"/>
+      <c r="AI13" s="117" t="s">
         <v>14</v>
       </c>
-      <c r="AJ13" s="89"/>
-      <c r="AK13" s="89"/>
-      <c r="AL13" s="89"/>
-      <c r="AM13" s="89"/>
-      <c r="AN13" s="89"/>
-      <c r="AO13" s="89"/>
-      <c r="AP13" s="89"/>
-      <c r="AQ13" s="89"/>
-      <c r="AR13" s="89"/>
-      <c r="AS13" s="89"/>
-      <c r="AT13" s="89"/>
-      <c r="AU13" s="109"/>
-      <c r="AV13" s="86"/>
-      <c r="AW13" s="86"/>
-      <c r="AX13" s="86"/>
-      <c r="AY13" s="86"/>
-      <c r="AZ13" s="86"/>
-      <c r="BA13" s="87"/>
+      <c r="AJ13" s="118"/>
+      <c r="AK13" s="118"/>
+      <c r="AL13" s="118"/>
+      <c r="AM13" s="118"/>
+      <c r="AN13" s="118"/>
+      <c r="AO13" s="118"/>
+      <c r="AP13" s="118"/>
+      <c r="AQ13" s="118"/>
+      <c r="AR13" s="118"/>
+      <c r="AS13" s="118"/>
+      <c r="AT13" s="118"/>
+      <c r="AU13" s="120"/>
+      <c r="AV13" s="95"/>
+      <c r="AW13" s="95"/>
+      <c r="AX13" s="95"/>
+      <c r="AY13" s="95"/>
+      <c r="AZ13" s="95"/>
+      <c r="BA13" s="116"/>
     </row>
     <row r="14" spans="1:73" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="91" t="s">
+      <c r="B14" s="85" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="92"/>
-      <c r="D14" s="92"/>
-      <c r="E14" s="92"/>
-      <c r="F14" s="92"/>
-      <c r="G14" s="92"/>
-      <c r="H14" s="92"/>
-      <c r="I14" s="92"/>
-      <c r="J14" s="92"/>
-      <c r="K14" s="92"/>
-      <c r="L14" s="92"/>
-      <c r="M14" s="92"/>
-      <c r="N14" s="92"/>
-      <c r="O14" s="92"/>
-      <c r="P14" s="92"/>
-      <c r="Q14" s="93"/>
-      <c r="R14" s="98">
+      <c r="C14" s="86"/>
+      <c r="D14" s="86"/>
+      <c r="E14" s="86"/>
+      <c r="F14" s="86"/>
+      <c r="G14" s="86"/>
+      <c r="H14" s="86"/>
+      <c r="I14" s="86"/>
+      <c r="J14" s="86"/>
+      <c r="K14" s="86"/>
+      <c r="L14" s="86"/>
+      <c r="M14" s="86"/>
+      <c r="N14" s="86"/>
+      <c r="O14" s="86"/>
+      <c r="P14" s="86"/>
+      <c r="Q14" s="87"/>
+      <c r="R14" s="99">
         <v>0.7</v>
       </c>
-      <c r="S14" s="99"/>
-      <c r="T14" s="100"/>
-      <c r="U14" s="110"/>
-      <c r="V14" s="111"/>
-      <c r="W14" s="111"/>
-      <c r="X14" s="111"/>
-      <c r="Y14" s="111"/>
-      <c r="Z14" s="111"/>
-      <c r="AA14" s="111"/>
-      <c r="AB14" s="111"/>
-      <c r="AC14" s="111"/>
-      <c r="AD14" s="111"/>
-      <c r="AE14" s="111"/>
-      <c r="AF14" s="111"/>
-      <c r="AG14" s="111"/>
-      <c r="AH14" s="112"/>
-      <c r="AI14" s="110"/>
-      <c r="AJ14" s="111"/>
-      <c r="AK14" s="111"/>
-      <c r="AL14" s="111"/>
-      <c r="AM14" s="111"/>
-      <c r="AN14" s="111"/>
-      <c r="AO14" s="111"/>
-      <c r="AP14" s="111"/>
-      <c r="AQ14" s="111"/>
-      <c r="AR14" s="111"/>
-      <c r="AS14" s="111"/>
-      <c r="AT14" s="111"/>
-      <c r="AU14" s="113"/>
-      <c r="AV14" s="114"/>
-      <c r="AW14" s="115"/>
-      <c r="AX14" s="115"/>
-      <c r="AY14" s="115"/>
-      <c r="AZ14" s="115"/>
-      <c r="BA14" s="116"/>
+      <c r="S14" s="100"/>
+      <c r="T14" s="101"/>
+      <c r="U14" s="58"/>
+      <c r="V14" s="59"/>
+      <c r="W14" s="59"/>
+      <c r="X14" s="59"/>
+      <c r="Y14" s="59"/>
+      <c r="Z14" s="59"/>
+      <c r="AA14" s="59"/>
+      <c r="AB14" s="59"/>
+      <c r="AC14" s="59"/>
+      <c r="AD14" s="59"/>
+      <c r="AE14" s="59"/>
+      <c r="AF14" s="59"/>
+      <c r="AG14" s="59"/>
+      <c r="AH14" s="60"/>
+      <c r="AI14" s="58"/>
+      <c r="AJ14" s="59"/>
+      <c r="AK14" s="59"/>
+      <c r="AL14" s="59"/>
+      <c r="AM14" s="59"/>
+      <c r="AN14" s="59"/>
+      <c r="AO14" s="59"/>
+      <c r="AP14" s="59"/>
+      <c r="AQ14" s="59"/>
+      <c r="AR14" s="59"/>
+      <c r="AS14" s="59"/>
+      <c r="AT14" s="59"/>
+      <c r="AU14" s="61"/>
+      <c r="AV14" s="62"/>
+      <c r="AW14" s="63"/>
+      <c r="AX14" s="63"/>
+      <c r="AY14" s="63"/>
+      <c r="AZ14" s="63"/>
+      <c r="BA14" s="64"/>
     </row>
     <row r="15" spans="1:73" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="15"/>
@@ -2109,7 +2021,7 @@
       <c r="U15" s="49"/>
       <c r="AH15" s="47"/>
       <c r="AI15" s="49"/>
-      <c r="AU15" s="105"/>
+      <c r="AU15" s="56"/>
       <c r="AV15" s="20"/>
       <c r="AW15" s="20"/>
       <c r="AX15" s="20"/>
@@ -2135,19 +2047,19 @@
       <c r="O16" s="45"/>
       <c r="P16" s="45"/>
       <c r="Q16" s="45"/>
-      <c r="R16" s="72"/>
-      <c r="S16" s="62"/>
-      <c r="T16" s="73"/>
+      <c r="R16" s="102"/>
+      <c r="S16" s="79"/>
+      <c r="T16" s="103"/>
       <c r="U16" s="49"/>
       <c r="AH16" s="47"/>
       <c r="AI16" s="49"/>
-      <c r="AU16" s="105"/>
-      <c r="AV16" s="104"/>
-      <c r="AW16" s="62"/>
-      <c r="AX16" s="62"/>
-      <c r="AY16" s="62"/>
-      <c r="AZ16" s="62"/>
-      <c r="BA16" s="63"/>
+      <c r="AU16" s="56"/>
+      <c r="AV16" s="78"/>
+      <c r="AW16" s="79"/>
+      <c r="AX16" s="79"/>
+      <c r="AY16" s="79"/>
+      <c r="AZ16" s="79"/>
+      <c r="BA16" s="80"/>
     </row>
     <row r="17" spans="1:53" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="15"/>
@@ -2167,80 +2079,80 @@
       <c r="O17" s="45"/>
       <c r="P17" s="45"/>
       <c r="Q17" s="45"/>
-      <c r="R17" s="72"/>
-      <c r="S17" s="62"/>
-      <c r="T17" s="73"/>
+      <c r="R17" s="102"/>
+      <c r="S17" s="79"/>
+      <c r="T17" s="103"/>
       <c r="U17" s="49"/>
       <c r="AH17" s="47"/>
       <c r="AI17" s="49"/>
-      <c r="AU17" s="105"/>
-      <c r="AV17" s="104"/>
-      <c r="AW17" s="62"/>
-      <c r="AX17" s="62"/>
-      <c r="AY17" s="62"/>
-      <c r="AZ17" s="62"/>
-      <c r="BA17" s="63"/>
+      <c r="AU17" s="56"/>
+      <c r="AV17" s="78"/>
+      <c r="AW17" s="79"/>
+      <c r="AX17" s="79"/>
+      <c r="AY17" s="79"/>
+      <c r="AZ17" s="79"/>
+      <c r="BA17" s="80"/>
     </row>
     <row r="18" spans="1:53" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="69" t="s">
+      <c r="B18" s="88" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="70"/>
-      <c r="D18" s="70"/>
-      <c r="E18" s="70"/>
-      <c r="F18" s="70"/>
-      <c r="G18" s="70"/>
-      <c r="H18" s="70"/>
-      <c r="I18" s="70"/>
-      <c r="J18" s="70"/>
-      <c r="K18" s="70"/>
-      <c r="L18" s="70"/>
-      <c r="M18" s="70"/>
-      <c r="N18" s="70"/>
-      <c r="O18" s="70"/>
-      <c r="P18" s="70"/>
-      <c r="Q18" s="71"/>
-      <c r="R18" s="74">
+      <c r="C18" s="89"/>
+      <c r="D18" s="89"/>
+      <c r="E18" s="89"/>
+      <c r="F18" s="89"/>
+      <c r="G18" s="89"/>
+      <c r="H18" s="89"/>
+      <c r="I18" s="89"/>
+      <c r="J18" s="89"/>
+      <c r="K18" s="89"/>
+      <c r="L18" s="89"/>
+      <c r="M18" s="89"/>
+      <c r="N18" s="89"/>
+      <c r="O18" s="89"/>
+      <c r="P18" s="89"/>
+      <c r="Q18" s="90"/>
+      <c r="R18" s="121">
         <v>0.1</v>
       </c>
-      <c r="S18" s="75"/>
-      <c r="T18" s="73"/>
-      <c r="U18" s="117"/>
-      <c r="V18" s="118"/>
-      <c r="W18" s="118"/>
-      <c r="X18" s="118"/>
-      <c r="Y18" s="118"/>
-      <c r="Z18" s="118"/>
-      <c r="AA18" s="118"/>
-      <c r="AB18" s="118"/>
-      <c r="AC18" s="118"/>
-      <c r="AD18" s="118"/>
-      <c r="AE18" s="118"/>
-      <c r="AF18" s="118"/>
-      <c r="AG18" s="118"/>
-      <c r="AH18" s="119"/>
-      <c r="AI18" s="117"/>
-      <c r="AJ18" s="118"/>
-      <c r="AK18" s="118"/>
-      <c r="AL18" s="118"/>
-      <c r="AM18" s="118"/>
-      <c r="AN18" s="118"/>
-      <c r="AO18" s="118"/>
-      <c r="AP18" s="118"/>
-      <c r="AQ18" s="118"/>
-      <c r="AR18" s="118"/>
-      <c r="AS18" s="118"/>
-      <c r="AT18" s="118"/>
-      <c r="AU18" s="120"/>
-      <c r="AV18" s="121"/>
-      <c r="AW18" s="122"/>
-      <c r="AX18" s="122"/>
-      <c r="AY18" s="122"/>
-      <c r="AZ18" s="122"/>
-      <c r="BA18" s="123"/>
+      <c r="S18" s="122"/>
+      <c r="T18" s="103"/>
+      <c r="U18" s="65"/>
+      <c r="V18" s="66"/>
+      <c r="W18" s="66"/>
+      <c r="X18" s="66"/>
+      <c r="Y18" s="66"/>
+      <c r="Z18" s="66"/>
+      <c r="AA18" s="66"/>
+      <c r="AB18" s="66"/>
+      <c r="AC18" s="66"/>
+      <c r="AD18" s="66"/>
+      <c r="AE18" s="66"/>
+      <c r="AF18" s="66"/>
+      <c r="AG18" s="66"/>
+      <c r="AH18" s="67"/>
+      <c r="AI18" s="65"/>
+      <c r="AJ18" s="66"/>
+      <c r="AK18" s="66"/>
+      <c r="AL18" s="66"/>
+      <c r="AM18" s="66"/>
+      <c r="AN18" s="66"/>
+      <c r="AO18" s="66"/>
+      <c r="AP18" s="66"/>
+      <c r="AQ18" s="66"/>
+      <c r="AR18" s="66"/>
+      <c r="AS18" s="66"/>
+      <c r="AT18" s="66"/>
+      <c r="AU18" s="68"/>
+      <c r="AV18" s="81"/>
+      <c r="AW18" s="82"/>
+      <c r="AX18" s="82"/>
+      <c r="AY18" s="82"/>
+      <c r="AZ18" s="82"/>
+      <c r="BA18" s="83"/>
     </row>
     <row r="19" spans="1:53" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="15"/>
@@ -2260,19 +2172,19 @@
       <c r="O19" s="45"/>
       <c r="P19" s="45"/>
       <c r="Q19" s="45"/>
-      <c r="R19" s="72"/>
-      <c r="S19" s="62"/>
-      <c r="T19" s="73"/>
+      <c r="R19" s="102"/>
+      <c r="S19" s="79"/>
+      <c r="T19" s="103"/>
       <c r="U19" s="49"/>
       <c r="AH19" s="47"/>
       <c r="AI19" s="49"/>
-      <c r="AU19" s="105"/>
-      <c r="AV19" s="104"/>
-      <c r="AW19" s="62"/>
-      <c r="AX19" s="62"/>
-      <c r="AY19" s="62"/>
-      <c r="AZ19" s="62"/>
-      <c r="BA19" s="63"/>
+      <c r="AU19" s="56"/>
+      <c r="AV19" s="78"/>
+      <c r="AW19" s="79"/>
+      <c r="AX19" s="79"/>
+      <c r="AY19" s="79"/>
+      <c r="AZ19" s="79"/>
+      <c r="BA19" s="80"/>
     </row>
     <row r="20" spans="1:53" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="15"/>
@@ -2292,19 +2204,19 @@
       <c r="O20" s="45"/>
       <c r="P20" s="45"/>
       <c r="Q20" s="45"/>
-      <c r="R20" s="72"/>
-      <c r="S20" s="62"/>
-      <c r="T20" s="73"/>
+      <c r="R20" s="102"/>
+      <c r="S20" s="79"/>
+      <c r="T20" s="103"/>
       <c r="U20" s="49"/>
       <c r="AH20" s="47"/>
       <c r="AI20" s="49"/>
-      <c r="AU20" s="105"/>
-      <c r="AV20" s="104"/>
-      <c r="AW20" s="62"/>
-      <c r="AX20" s="62"/>
-      <c r="AY20" s="62"/>
-      <c r="AZ20" s="62"/>
-      <c r="BA20" s="63"/>
+      <c r="AU20" s="56"/>
+      <c r="AV20" s="78"/>
+      <c r="AW20" s="79"/>
+      <c r="AX20" s="79"/>
+      <c r="AY20" s="79"/>
+      <c r="AZ20" s="79"/>
+      <c r="BA20" s="80"/>
     </row>
     <row r="21" spans="1:53" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="15"/>
@@ -2330,7 +2242,7 @@
       <c r="U21" s="49"/>
       <c r="AH21" s="47"/>
       <c r="AI21" s="49"/>
-      <c r="AU21" s="105"/>
+      <c r="AU21" s="56"/>
       <c r="AV21" s="25"/>
       <c r="AW21" s="18"/>
       <c r="AX21" s="18"/>
@@ -2362,7 +2274,7 @@
       <c r="U22" s="49"/>
       <c r="AH22" s="47"/>
       <c r="AI22" s="49"/>
-      <c r="AU22" s="105"/>
+      <c r="AU22" s="56"/>
       <c r="AV22" s="25"/>
       <c r="AW22" s="18"/>
       <c r="AX22" s="18"/>
@@ -2374,62 +2286,62 @@
       <c r="A23" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="B23" s="69" t="s">
+      <c r="B23" s="88" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="70"/>
-      <c r="D23" s="70"/>
-      <c r="E23" s="70"/>
-      <c r="F23" s="70"/>
-      <c r="G23" s="70"/>
-      <c r="H23" s="70"/>
-      <c r="I23" s="70"/>
-      <c r="J23" s="70"/>
-      <c r="K23" s="70"/>
-      <c r="L23" s="70"/>
-      <c r="M23" s="70"/>
-      <c r="N23" s="70"/>
-      <c r="O23" s="70"/>
-      <c r="P23" s="70"/>
-      <c r="Q23" s="71"/>
-      <c r="R23" s="74">
+      <c r="C23" s="89"/>
+      <c r="D23" s="89"/>
+      <c r="E23" s="89"/>
+      <c r="F23" s="89"/>
+      <c r="G23" s="89"/>
+      <c r="H23" s="89"/>
+      <c r="I23" s="89"/>
+      <c r="J23" s="89"/>
+      <c r="K23" s="89"/>
+      <c r="L23" s="89"/>
+      <c r="M23" s="89"/>
+      <c r="N23" s="89"/>
+      <c r="O23" s="89"/>
+      <c r="P23" s="89"/>
+      <c r="Q23" s="90"/>
+      <c r="R23" s="121">
         <v>0.1</v>
       </c>
-      <c r="S23" s="75"/>
-      <c r="T23" s="73"/>
-      <c r="U23" s="117"/>
-      <c r="V23" s="118"/>
-      <c r="W23" s="118"/>
-      <c r="X23" s="118"/>
-      <c r="Y23" s="118"/>
-      <c r="Z23" s="118"/>
-      <c r="AA23" s="118"/>
-      <c r="AB23" s="118"/>
-      <c r="AC23" s="118"/>
-      <c r="AD23" s="118"/>
-      <c r="AE23" s="118"/>
-      <c r="AF23" s="118"/>
-      <c r="AG23" s="118"/>
-      <c r="AH23" s="119"/>
-      <c r="AI23" s="117"/>
-      <c r="AJ23" s="118"/>
-      <c r="AK23" s="118"/>
-      <c r="AL23" s="118"/>
-      <c r="AM23" s="118"/>
-      <c r="AN23" s="118"/>
-      <c r="AO23" s="118"/>
-      <c r="AP23" s="118"/>
-      <c r="AQ23" s="118"/>
-      <c r="AR23" s="118"/>
-      <c r="AS23" s="118"/>
-      <c r="AT23" s="118"/>
-      <c r="AU23" s="120"/>
-      <c r="AV23" s="121"/>
-      <c r="AW23" s="122"/>
-      <c r="AX23" s="122"/>
-      <c r="AY23" s="122"/>
-      <c r="AZ23" s="122"/>
-      <c r="BA23" s="123"/>
+      <c r="S23" s="122"/>
+      <c r="T23" s="103"/>
+      <c r="U23" s="65"/>
+      <c r="V23" s="66"/>
+      <c r="W23" s="66"/>
+      <c r="X23" s="66"/>
+      <c r="Y23" s="66"/>
+      <c r="Z23" s="66"/>
+      <c r="AA23" s="66"/>
+      <c r="AB23" s="66"/>
+      <c r="AC23" s="66"/>
+      <c r="AD23" s="66"/>
+      <c r="AE23" s="66"/>
+      <c r="AF23" s="66"/>
+      <c r="AG23" s="66"/>
+      <c r="AH23" s="67"/>
+      <c r="AI23" s="65"/>
+      <c r="AJ23" s="66"/>
+      <c r="AK23" s="66"/>
+      <c r="AL23" s="66"/>
+      <c r="AM23" s="66"/>
+      <c r="AN23" s="66"/>
+      <c r="AO23" s="66"/>
+      <c r="AP23" s="66"/>
+      <c r="AQ23" s="66"/>
+      <c r="AR23" s="66"/>
+      <c r="AS23" s="66"/>
+      <c r="AT23" s="66"/>
+      <c r="AU23" s="68"/>
+      <c r="AV23" s="81"/>
+      <c r="AW23" s="82"/>
+      <c r="AX23" s="82"/>
+      <c r="AY23" s="82"/>
+      <c r="AZ23" s="82"/>
+      <c r="BA23" s="83"/>
     </row>
     <row r="24" spans="1:53" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="15"/>
@@ -2455,7 +2367,7 @@
       <c r="U24" s="49"/>
       <c r="AH24" s="47"/>
       <c r="AI24" s="49"/>
-      <c r="AU24" s="105"/>
+      <c r="AU24" s="56"/>
       <c r="AV24" s="27"/>
       <c r="AW24" s="20"/>
       <c r="AX24" s="20"/>
@@ -2487,7 +2399,7 @@
       <c r="U25" s="49"/>
       <c r="AH25" s="47"/>
       <c r="AI25" s="49"/>
-      <c r="AU25" s="105"/>
+      <c r="AU25" s="56"/>
       <c r="AV25" s="27"/>
       <c r="AW25" s="27"/>
       <c r="AX25" s="20"/>
@@ -2513,80 +2425,80 @@
       <c r="O26" s="20"/>
       <c r="P26" s="20"/>
       <c r="Q26" s="53"/>
-      <c r="R26" s="72"/>
-      <c r="S26" s="62"/>
-      <c r="T26" s="73"/>
+      <c r="R26" s="102"/>
+      <c r="S26" s="79"/>
+      <c r="T26" s="103"/>
       <c r="U26" s="49"/>
       <c r="AH26" s="47"/>
       <c r="AI26" s="49"/>
-      <c r="AU26" s="105"/>
-      <c r="AV26" s="104"/>
-      <c r="AW26" s="62"/>
-      <c r="AX26" s="62"/>
-      <c r="AY26" s="62"/>
-      <c r="AZ26" s="62"/>
-      <c r="BA26" s="63"/>
+      <c r="AU26" s="56"/>
+      <c r="AV26" s="78"/>
+      <c r="AW26" s="79"/>
+      <c r="AX26" s="79"/>
+      <c r="AY26" s="79"/>
+      <c r="AZ26" s="79"/>
+      <c r="BA26" s="80"/>
     </row>
     <row r="27" spans="1:53" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="B27" s="69" t="s">
+      <c r="B27" s="88" t="s">
         <v>22</v>
       </c>
-      <c r="C27" s="70"/>
-      <c r="D27" s="70"/>
-      <c r="E27" s="70"/>
-      <c r="F27" s="70"/>
-      <c r="G27" s="70"/>
-      <c r="H27" s="70"/>
-      <c r="I27" s="70"/>
-      <c r="J27" s="70"/>
-      <c r="K27" s="70"/>
-      <c r="L27" s="70"/>
-      <c r="M27" s="70"/>
-      <c r="N27" s="70"/>
-      <c r="O27" s="70"/>
-      <c r="P27" s="70"/>
-      <c r="Q27" s="71"/>
-      <c r="R27" s="74">
+      <c r="C27" s="89"/>
+      <c r="D27" s="89"/>
+      <c r="E27" s="89"/>
+      <c r="F27" s="89"/>
+      <c r="G27" s="89"/>
+      <c r="H27" s="89"/>
+      <c r="I27" s="89"/>
+      <c r="J27" s="89"/>
+      <c r="K27" s="89"/>
+      <c r="L27" s="89"/>
+      <c r="M27" s="89"/>
+      <c r="N27" s="89"/>
+      <c r="O27" s="89"/>
+      <c r="P27" s="89"/>
+      <c r="Q27" s="90"/>
+      <c r="R27" s="121">
         <v>0.1</v>
       </c>
-      <c r="S27" s="75"/>
-      <c r="T27" s="73"/>
-      <c r="U27" s="117"/>
-      <c r="V27" s="118"/>
-      <c r="W27" s="118"/>
-      <c r="X27" s="118"/>
-      <c r="Y27" s="118"/>
-      <c r="Z27" s="118"/>
-      <c r="AA27" s="118"/>
-      <c r="AB27" s="118"/>
-      <c r="AC27" s="118"/>
-      <c r="AD27" s="118"/>
-      <c r="AE27" s="118"/>
-      <c r="AF27" s="118"/>
-      <c r="AG27" s="118"/>
-      <c r="AH27" s="119"/>
-      <c r="AI27" s="117"/>
-      <c r="AJ27" s="118"/>
-      <c r="AK27" s="118"/>
-      <c r="AL27" s="118"/>
-      <c r="AM27" s="118"/>
-      <c r="AN27" s="118"/>
-      <c r="AO27" s="118"/>
-      <c r="AP27" s="118"/>
-      <c r="AQ27" s="118"/>
-      <c r="AR27" s="118"/>
-      <c r="AS27" s="118"/>
-      <c r="AT27" s="118"/>
-      <c r="AU27" s="120"/>
-      <c r="AV27" s="124"/>
-      <c r="AW27" s="124"/>
-      <c r="AX27" s="124"/>
-      <c r="AY27" s="124"/>
-      <c r="AZ27" s="124"/>
-      <c r="BA27" s="125"/>
+      <c r="S27" s="122"/>
+      <c r="T27" s="103"/>
+      <c r="U27" s="65"/>
+      <c r="V27" s="66"/>
+      <c r="W27" s="66"/>
+      <c r="X27" s="66"/>
+      <c r="Y27" s="66"/>
+      <c r="Z27" s="66"/>
+      <c r="AA27" s="66"/>
+      <c r="AB27" s="66"/>
+      <c r="AC27" s="66"/>
+      <c r="AD27" s="66"/>
+      <c r="AE27" s="66"/>
+      <c r="AF27" s="66"/>
+      <c r="AG27" s="66"/>
+      <c r="AH27" s="67"/>
+      <c r="AI27" s="65"/>
+      <c r="AJ27" s="66"/>
+      <c r="AK27" s="66"/>
+      <c r="AL27" s="66"/>
+      <c r="AM27" s="66"/>
+      <c r="AN27" s="66"/>
+      <c r="AO27" s="66"/>
+      <c r="AP27" s="66"/>
+      <c r="AQ27" s="66"/>
+      <c r="AR27" s="66"/>
+      <c r="AS27" s="66"/>
+      <c r="AT27" s="66"/>
+      <c r="AU27" s="68"/>
+      <c r="AV27" s="69"/>
+      <c r="AW27" s="69"/>
+      <c r="AX27" s="69"/>
+      <c r="AY27" s="69"/>
+      <c r="AZ27" s="69"/>
+      <c r="BA27" s="70"/>
     </row>
     <row r="28" spans="1:53" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="15"/>
@@ -2612,7 +2524,7 @@
       <c r="U28" s="49"/>
       <c r="AH28" s="47"/>
       <c r="AI28" s="49"/>
-      <c r="AU28" s="105"/>
+      <c r="AU28" s="56"/>
       <c r="AV28" s="28"/>
       <c r="AW28" s="27"/>
       <c r="AX28" s="20"/>
@@ -2638,19 +2550,19 @@
       <c r="O29" s="20"/>
       <c r="P29" s="20"/>
       <c r="Q29" s="53"/>
-      <c r="R29" s="72"/>
-      <c r="S29" s="62"/>
-      <c r="T29" s="73"/>
+      <c r="R29" s="102"/>
+      <c r="S29" s="79"/>
+      <c r="T29" s="103"/>
       <c r="U29" s="49"/>
       <c r="AH29" s="47"/>
       <c r="AI29" s="49"/>
-      <c r="AU29" s="105"/>
-      <c r="AV29" s="104"/>
-      <c r="AW29" s="62"/>
-      <c r="AX29" s="62"/>
-      <c r="AY29" s="62"/>
-      <c r="AZ29" s="62"/>
-      <c r="BA29" s="63"/>
+      <c r="AU29" s="56"/>
+      <c r="AV29" s="78"/>
+      <c r="AW29" s="79"/>
+      <c r="AX29" s="79"/>
+      <c r="AY29" s="79"/>
+      <c r="AZ29" s="79"/>
+      <c r="BA29" s="80"/>
     </row>
     <row r="30" spans="1:53" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="29"/>
@@ -2699,7 +2611,7 @@
       <c r="AR30" s="48"/>
       <c r="AS30" s="48"/>
       <c r="AT30" s="48"/>
-      <c r="AU30" s="106"/>
+      <c r="AU30" s="57"/>
       <c r="AV30" s="30"/>
       <c r="AW30" s="35"/>
       <c r="AX30" s="36"/>
@@ -2725,12 +2637,12 @@
       <c r="O31" s="30"/>
       <c r="P31" s="30"/>
       <c r="Q31" s="31"/>
-      <c r="R31" s="67">
+      <c r="R31" s="127">
         <f>+R14+R18+R23+R27</f>
         <v>0.99999999999999989</v>
       </c>
-      <c r="S31" s="56"/>
-      <c r="T31" s="68"/>
+      <c r="S31" s="74"/>
+      <c r="T31" s="128"/>
       <c r="U31" s="38"/>
       <c r="V31" s="36"/>
       <c r="W31" s="36"/>
@@ -2758,12 +2670,12 @@
       <c r="AS31" s="30"/>
       <c r="AT31" s="30"/>
       <c r="AU31" s="39"/>
-      <c r="AV31" s="101"/>
-      <c r="AW31" s="56"/>
-      <c r="AX31" s="56"/>
-      <c r="AY31" s="56"/>
-      <c r="AZ31" s="56"/>
-      <c r="BA31" s="57"/>
+      <c r="AV31" s="84"/>
+      <c r="AW31" s="74"/>
+      <c r="AX31" s="74"/>
+      <c r="AY31" s="74"/>
+      <c r="AZ31" s="74"/>
+      <c r="BA31" s="75"/>
     </row>
     <row r="32" spans="1:53" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A32" s="40"/>
@@ -2826,54 +2738,54 @@
       <c r="C33" s="45"/>
       <c r="D33" s="45"/>
       <c r="E33" s="45"/>
-      <c r="F33" s="55" t="s">
+      <c r="F33" s="77" t="s">
         <v>23</v>
       </c>
-      <c r="G33" s="56"/>
-      <c r="H33" s="56"/>
-      <c r="I33" s="56"/>
-      <c r="J33" s="56"/>
-      <c r="K33" s="56"/>
-      <c r="L33" s="56"/>
-      <c r="M33" s="56"/>
-      <c r="N33" s="56"/>
-      <c r="O33" s="56"/>
-      <c r="P33" s="56"/>
-      <c r="Q33" s="56"/>
-      <c r="R33" s="56"/>
-      <c r="S33" s="57"/>
-      <c r="T33" s="55" t="s">
+      <c r="G33" s="74"/>
+      <c r="H33" s="74"/>
+      <c r="I33" s="74"/>
+      <c r="J33" s="74"/>
+      <c r="K33" s="74"/>
+      <c r="L33" s="74"/>
+      <c r="M33" s="74"/>
+      <c r="N33" s="74"/>
+      <c r="O33" s="74"/>
+      <c r="P33" s="74"/>
+      <c r="Q33" s="74"/>
+      <c r="R33" s="74"/>
+      <c r="S33" s="75"/>
+      <c r="T33" s="77" t="s">
         <v>24</v>
       </c>
-      <c r="U33" s="56"/>
-      <c r="V33" s="56"/>
-      <c r="W33" s="56"/>
-      <c r="X33" s="56"/>
-      <c r="Y33" s="56"/>
-      <c r="Z33" s="56"/>
-      <c r="AA33" s="56"/>
-      <c r="AB33" s="56"/>
-      <c r="AC33" s="56"/>
-      <c r="AD33" s="56"/>
-      <c r="AE33" s="56"/>
-      <c r="AF33" s="56"/>
-      <c r="AG33" s="57"/>
-      <c r="AH33" s="55" t="s">
+      <c r="U33" s="74"/>
+      <c r="V33" s="74"/>
+      <c r="W33" s="74"/>
+      <c r="X33" s="74"/>
+      <c r="Y33" s="74"/>
+      <c r="Z33" s="74"/>
+      <c r="AA33" s="74"/>
+      <c r="AB33" s="74"/>
+      <c r="AC33" s="74"/>
+      <c r="AD33" s="74"/>
+      <c r="AE33" s="74"/>
+      <c r="AF33" s="74"/>
+      <c r="AG33" s="75"/>
+      <c r="AH33" s="77" t="s">
         <v>25</v>
       </c>
-      <c r="AI33" s="56"/>
-      <c r="AJ33" s="56"/>
-      <c r="AK33" s="56"/>
-      <c r="AL33" s="56"/>
-      <c r="AM33" s="56"/>
-      <c r="AN33" s="56"/>
-      <c r="AO33" s="56"/>
-      <c r="AP33" s="56"/>
-      <c r="AQ33" s="56"/>
-      <c r="AR33" s="56"/>
-      <c r="AS33" s="56"/>
-      <c r="AT33" s="56"/>
-      <c r="AU33" s="57"/>
+      <c r="AI33" s="74"/>
+      <c r="AJ33" s="74"/>
+      <c r="AK33" s="74"/>
+      <c r="AL33" s="74"/>
+      <c r="AM33" s="74"/>
+      <c r="AN33" s="74"/>
+      <c r="AO33" s="74"/>
+      <c r="AP33" s="74"/>
+      <c r="AQ33" s="74"/>
+      <c r="AR33" s="74"/>
+      <c r="AS33" s="74"/>
+      <c r="AT33" s="74"/>
+      <c r="AU33" s="75"/>
       <c r="AV33" s="45"/>
       <c r="AW33" s="45"/>
       <c r="AX33" s="45"/>
@@ -2887,48 +2799,48 @@
       <c r="C34" s="20"/>
       <c r="D34" s="20"/>
       <c r="E34" s="20"/>
-      <c r="F34" s="58"/>
-      <c r="G34" s="59"/>
-      <c r="H34" s="59"/>
-      <c r="I34" s="59"/>
-      <c r="J34" s="59"/>
-      <c r="K34" s="59"/>
-      <c r="L34" s="59"/>
-      <c r="M34" s="59"/>
-      <c r="N34" s="59"/>
-      <c r="O34" s="59"/>
-      <c r="P34" s="59"/>
-      <c r="Q34" s="59"/>
-      <c r="R34" s="59"/>
-      <c r="S34" s="60"/>
-      <c r="T34" s="58"/>
-      <c r="U34" s="59"/>
-      <c r="V34" s="59"/>
-      <c r="W34" s="59"/>
-      <c r="X34" s="59"/>
-      <c r="Y34" s="59"/>
-      <c r="Z34" s="59"/>
-      <c r="AA34" s="59"/>
-      <c r="AB34" s="59"/>
-      <c r="AC34" s="59"/>
-      <c r="AD34" s="59"/>
-      <c r="AE34" s="59"/>
-      <c r="AF34" s="59"/>
-      <c r="AG34" s="60"/>
-      <c r="AH34" s="58"/>
-      <c r="AI34" s="59"/>
-      <c r="AJ34" s="59"/>
-      <c r="AK34" s="59"/>
-      <c r="AL34" s="59"/>
-      <c r="AM34" s="59"/>
-      <c r="AN34" s="59"/>
-      <c r="AO34" s="59"/>
-      <c r="AP34" s="59"/>
-      <c r="AQ34" s="59"/>
-      <c r="AR34" s="59"/>
-      <c r="AS34" s="59"/>
-      <c r="AT34" s="59"/>
-      <c r="AU34" s="60"/>
+      <c r="F34" s="123"/>
+      <c r="G34" s="92"/>
+      <c r="H34" s="92"/>
+      <c r="I34" s="92"/>
+      <c r="J34" s="92"/>
+      <c r="K34" s="92"/>
+      <c r="L34" s="92"/>
+      <c r="M34" s="92"/>
+      <c r="N34" s="92"/>
+      <c r="O34" s="92"/>
+      <c r="P34" s="92"/>
+      <c r="Q34" s="92"/>
+      <c r="R34" s="92"/>
+      <c r="S34" s="105"/>
+      <c r="T34" s="123"/>
+      <c r="U34" s="92"/>
+      <c r="V34" s="92"/>
+      <c r="W34" s="92"/>
+      <c r="X34" s="92"/>
+      <c r="Y34" s="92"/>
+      <c r="Z34" s="92"/>
+      <c r="AA34" s="92"/>
+      <c r="AB34" s="92"/>
+      <c r="AC34" s="92"/>
+      <c r="AD34" s="92"/>
+      <c r="AE34" s="92"/>
+      <c r="AF34" s="92"/>
+      <c r="AG34" s="105"/>
+      <c r="AH34" s="123"/>
+      <c r="AI34" s="92"/>
+      <c r="AJ34" s="92"/>
+      <c r="AK34" s="92"/>
+      <c r="AL34" s="92"/>
+      <c r="AM34" s="92"/>
+      <c r="AN34" s="92"/>
+      <c r="AO34" s="92"/>
+      <c r="AP34" s="92"/>
+      <c r="AQ34" s="92"/>
+      <c r="AR34" s="92"/>
+      <c r="AS34" s="92"/>
+      <c r="AT34" s="92"/>
+      <c r="AU34" s="105"/>
       <c r="AV34" s="20"/>
       <c r="AW34" s="20"/>
       <c r="AX34" s="20"/>
@@ -2942,48 +2854,48 @@
       <c r="C35" s="20"/>
       <c r="D35" s="20"/>
       <c r="E35" s="20"/>
-      <c r="F35" s="61"/>
-      <c r="G35" s="62"/>
-      <c r="H35" s="62"/>
-      <c r="I35" s="62"/>
-      <c r="J35" s="62"/>
-      <c r="K35" s="62"/>
-      <c r="L35" s="62"/>
-      <c r="M35" s="62"/>
-      <c r="N35" s="62"/>
-      <c r="O35" s="62"/>
-      <c r="P35" s="62"/>
-      <c r="Q35" s="62"/>
-      <c r="R35" s="62"/>
-      <c r="S35" s="63"/>
-      <c r="T35" s="61"/>
-      <c r="U35" s="62"/>
-      <c r="V35" s="62"/>
-      <c r="W35" s="62"/>
-      <c r="X35" s="62"/>
-      <c r="Y35" s="62"/>
-      <c r="Z35" s="62"/>
-      <c r="AA35" s="62"/>
-      <c r="AB35" s="62"/>
-      <c r="AC35" s="62"/>
-      <c r="AD35" s="62"/>
-      <c r="AE35" s="62"/>
-      <c r="AF35" s="62"/>
-      <c r="AG35" s="63"/>
-      <c r="AH35" s="61"/>
-      <c r="AI35" s="62"/>
-      <c r="AJ35" s="62"/>
-      <c r="AK35" s="62"/>
-      <c r="AL35" s="62"/>
-      <c r="AM35" s="62"/>
-      <c r="AN35" s="62"/>
-      <c r="AO35" s="62"/>
-      <c r="AP35" s="62"/>
-      <c r="AQ35" s="62"/>
-      <c r="AR35" s="62"/>
-      <c r="AS35" s="62"/>
-      <c r="AT35" s="62"/>
-      <c r="AU35" s="63"/>
+      <c r="F35" s="124"/>
+      <c r="G35" s="79"/>
+      <c r="H35" s="79"/>
+      <c r="I35" s="79"/>
+      <c r="J35" s="79"/>
+      <c r="K35" s="79"/>
+      <c r="L35" s="79"/>
+      <c r="M35" s="79"/>
+      <c r="N35" s="79"/>
+      <c r="O35" s="79"/>
+      <c r="P35" s="79"/>
+      <c r="Q35" s="79"/>
+      <c r="R35" s="79"/>
+      <c r="S35" s="80"/>
+      <c r="T35" s="124"/>
+      <c r="U35" s="79"/>
+      <c r="V35" s="79"/>
+      <c r="W35" s="79"/>
+      <c r="X35" s="79"/>
+      <c r="Y35" s="79"/>
+      <c r="Z35" s="79"/>
+      <c r="AA35" s="79"/>
+      <c r="AB35" s="79"/>
+      <c r="AC35" s="79"/>
+      <c r="AD35" s="79"/>
+      <c r="AE35" s="79"/>
+      <c r="AF35" s="79"/>
+      <c r="AG35" s="80"/>
+      <c r="AH35" s="124"/>
+      <c r="AI35" s="79"/>
+      <c r="AJ35" s="79"/>
+      <c r="AK35" s="79"/>
+      <c r="AL35" s="79"/>
+      <c r="AM35" s="79"/>
+      <c r="AN35" s="79"/>
+      <c r="AO35" s="79"/>
+      <c r="AP35" s="79"/>
+      <c r="AQ35" s="79"/>
+      <c r="AR35" s="79"/>
+      <c r="AS35" s="79"/>
+      <c r="AT35" s="79"/>
+      <c r="AU35" s="80"/>
       <c r="AV35" s="20"/>
       <c r="AW35" s="20"/>
       <c r="AX35" s="20"/>
@@ -2997,48 +2909,48 @@
       <c r="C36" s="20"/>
       <c r="D36" s="20"/>
       <c r="E36" s="20"/>
-      <c r="F36" s="64"/>
-      <c r="G36" s="65"/>
-      <c r="H36" s="65"/>
-      <c r="I36" s="65"/>
-      <c r="J36" s="65"/>
-      <c r="K36" s="65"/>
-      <c r="L36" s="65"/>
-      <c r="M36" s="65"/>
-      <c r="N36" s="65"/>
-      <c r="O36" s="65"/>
-      <c r="P36" s="65"/>
-      <c r="Q36" s="65"/>
-      <c r="R36" s="65"/>
-      <c r="S36" s="66"/>
-      <c r="T36" s="64"/>
-      <c r="U36" s="65"/>
-      <c r="V36" s="65"/>
-      <c r="W36" s="65"/>
-      <c r="X36" s="65"/>
-      <c r="Y36" s="65"/>
-      <c r="Z36" s="65"/>
-      <c r="AA36" s="65"/>
-      <c r="AB36" s="65"/>
-      <c r="AC36" s="65"/>
-      <c r="AD36" s="65"/>
-      <c r="AE36" s="65"/>
-      <c r="AF36" s="65"/>
-      <c r="AG36" s="66"/>
-      <c r="AH36" s="64"/>
-      <c r="AI36" s="65"/>
-      <c r="AJ36" s="65"/>
-      <c r="AK36" s="65"/>
-      <c r="AL36" s="65"/>
-      <c r="AM36" s="65"/>
-      <c r="AN36" s="65"/>
-      <c r="AO36" s="65"/>
-      <c r="AP36" s="65"/>
-      <c r="AQ36" s="65"/>
-      <c r="AR36" s="65"/>
-      <c r="AS36" s="65"/>
-      <c r="AT36" s="65"/>
-      <c r="AU36" s="66"/>
+      <c r="F36" s="125"/>
+      <c r="G36" s="111"/>
+      <c r="H36" s="111"/>
+      <c r="I36" s="111"/>
+      <c r="J36" s="111"/>
+      <c r="K36" s="111"/>
+      <c r="L36" s="111"/>
+      <c r="M36" s="111"/>
+      <c r="N36" s="111"/>
+      <c r="O36" s="111"/>
+      <c r="P36" s="111"/>
+      <c r="Q36" s="111"/>
+      <c r="R36" s="111"/>
+      <c r="S36" s="126"/>
+      <c r="T36" s="125"/>
+      <c r="U36" s="111"/>
+      <c r="V36" s="111"/>
+      <c r="W36" s="111"/>
+      <c r="X36" s="111"/>
+      <c r="Y36" s="111"/>
+      <c r="Z36" s="111"/>
+      <c r="AA36" s="111"/>
+      <c r="AB36" s="111"/>
+      <c r="AC36" s="111"/>
+      <c r="AD36" s="111"/>
+      <c r="AE36" s="111"/>
+      <c r="AF36" s="111"/>
+      <c r="AG36" s="126"/>
+      <c r="AH36" s="125"/>
+      <c r="AI36" s="111"/>
+      <c r="AJ36" s="111"/>
+      <c r="AK36" s="111"/>
+      <c r="AL36" s="111"/>
+      <c r="AM36" s="111"/>
+      <c r="AN36" s="111"/>
+      <c r="AO36" s="111"/>
+      <c r="AP36" s="111"/>
+      <c r="AQ36" s="111"/>
+      <c r="AR36" s="111"/>
+      <c r="AS36" s="111"/>
+      <c r="AT36" s="111"/>
+      <c r="AU36" s="126"/>
       <c r="AV36" s="20"/>
       <c r="AW36" s="20"/>
       <c r="AX36" s="20"/>
@@ -3052,48 +2964,48 @@
       <c r="C37" s="20"/>
       <c r="D37" s="20"/>
       <c r="E37" s="20"/>
-      <c r="F37" s="102"/>
-      <c r="G37" s="56"/>
-      <c r="H37" s="56"/>
-      <c r="I37" s="56"/>
-      <c r="J37" s="56"/>
-      <c r="K37" s="56"/>
-      <c r="L37" s="56"/>
-      <c r="M37" s="56"/>
-      <c r="N37" s="56"/>
-      <c r="O37" s="56"/>
-      <c r="P37" s="56"/>
-      <c r="Q37" s="56"/>
-      <c r="R37" s="56"/>
-      <c r="S37" s="57"/>
-      <c r="T37" s="55"/>
-      <c r="U37" s="56"/>
-      <c r="V37" s="56"/>
-      <c r="W37" s="56"/>
-      <c r="X37" s="56"/>
-      <c r="Y37" s="56"/>
-      <c r="Z37" s="56"/>
-      <c r="AA37" s="56"/>
-      <c r="AB37" s="56"/>
-      <c r="AC37" s="56"/>
-      <c r="AD37" s="56"/>
-      <c r="AE37" s="56"/>
-      <c r="AF37" s="56"/>
-      <c r="AG37" s="57"/>
-      <c r="AH37" s="102"/>
-      <c r="AI37" s="56"/>
-      <c r="AJ37" s="56"/>
-      <c r="AK37" s="56"/>
-      <c r="AL37" s="56"/>
-      <c r="AM37" s="56"/>
-      <c r="AN37" s="56"/>
-      <c r="AO37" s="56"/>
-      <c r="AP37" s="56"/>
-      <c r="AQ37" s="56"/>
-      <c r="AR37" s="56"/>
-      <c r="AS37" s="56"/>
-      <c r="AT37" s="56"/>
-      <c r="AU37" s="57"/>
+      <c r="F37" s="73"/>
+      <c r="G37" s="74"/>
+      <c r="H37" s="74"/>
+      <c r="I37" s="74"/>
+      <c r="J37" s="74"/>
+      <c r="K37" s="74"/>
+      <c r="L37" s="74"/>
+      <c r="M37" s="74"/>
+      <c r="N37" s="74"/>
+      <c r="O37" s="74"/>
+      <c r="P37" s="74"/>
+      <c r="Q37" s="74"/>
+      <c r="R37" s="74"/>
+      <c r="S37" s="75"/>
+      <c r="T37" s="77"/>
+      <c r="U37" s="74"/>
+      <c r="V37" s="74"/>
+      <c r="W37" s="74"/>
+      <c r="X37" s="74"/>
+      <c r="Y37" s="74"/>
+      <c r="Z37" s="74"/>
+      <c r="AA37" s="74"/>
+      <c r="AB37" s="74"/>
+      <c r="AC37" s="74"/>
+      <c r="AD37" s="74"/>
+      <c r="AE37" s="74"/>
+      <c r="AF37" s="74"/>
+      <c r="AG37" s="75"/>
+      <c r="AH37" s="73"/>
+      <c r="AI37" s="74"/>
+      <c r="AJ37" s="74"/>
+      <c r="AK37" s="74"/>
+      <c r="AL37" s="74"/>
+      <c r="AM37" s="74"/>
+      <c r="AN37" s="74"/>
+      <c r="AO37" s="74"/>
+      <c r="AP37" s="74"/>
+      <c r="AQ37" s="74"/>
+      <c r="AR37" s="74"/>
+      <c r="AS37" s="74"/>
+      <c r="AT37" s="74"/>
+      <c r="AU37" s="75"/>
       <c r="AV37" s="20"/>
       <c r="AW37" s="20"/>
       <c r="AX37" s="20"/>
@@ -3107,56 +3019,56 @@
       <c r="C38" s="20"/>
       <c r="D38" s="20"/>
       <c r="E38" s="20"/>
-      <c r="F38" s="102" t="s">
+      <c r="F38" s="73" t="s">
         <v>26</v>
       </c>
-      <c r="G38" s="56"/>
-      <c r="H38" s="56"/>
-      <c r="I38" s="103"/>
-      <c r="J38" s="56"/>
-      <c r="K38" s="56"/>
-      <c r="L38" s="56"/>
-      <c r="M38" s="56"/>
-      <c r="N38" s="56"/>
-      <c r="O38" s="56"/>
-      <c r="P38" s="56"/>
-      <c r="Q38" s="56"/>
-      <c r="R38" s="56"/>
-      <c r="S38" s="57"/>
+      <c r="G38" s="74"/>
+      <c r="H38" s="74"/>
+      <c r="I38" s="76"/>
+      <c r="J38" s="74"/>
+      <c r="K38" s="74"/>
+      <c r="L38" s="74"/>
+      <c r="M38" s="74"/>
+      <c r="N38" s="74"/>
+      <c r="O38" s="74"/>
+      <c r="P38" s="74"/>
+      <c r="Q38" s="74"/>
+      <c r="R38" s="74"/>
+      <c r="S38" s="75"/>
       <c r="T38" s="46" t="str">
         <f>F38</f>
         <v xml:space="preserve">Date : </v>
       </c>
-      <c r="U38" s="103"/>
-      <c r="V38" s="56"/>
-      <c r="W38" s="56"/>
-      <c r="X38" s="56"/>
-      <c r="Y38" s="56"/>
-      <c r="Z38" s="56"/>
-      <c r="AA38" s="56"/>
-      <c r="AB38" s="56"/>
-      <c r="AC38" s="56"/>
-      <c r="AD38" s="56"/>
-      <c r="AE38" s="56"/>
-      <c r="AF38" s="56"/>
-      <c r="AG38" s="57"/>
-      <c r="AH38" s="102" t="str">
+      <c r="U38" s="76"/>
+      <c r="V38" s="74"/>
+      <c r="W38" s="74"/>
+      <c r="X38" s="74"/>
+      <c r="Y38" s="74"/>
+      <c r="Z38" s="74"/>
+      <c r="AA38" s="74"/>
+      <c r="AB38" s="74"/>
+      <c r="AC38" s="74"/>
+      <c r="AD38" s="74"/>
+      <c r="AE38" s="74"/>
+      <c r="AF38" s="74"/>
+      <c r="AG38" s="75"/>
+      <c r="AH38" s="73" t="str">
         <f>F38</f>
         <v xml:space="preserve">Date : </v>
       </c>
-      <c r="AI38" s="56"/>
-      <c r="AJ38" s="103"/>
-      <c r="AK38" s="56"/>
-      <c r="AL38" s="56"/>
-      <c r="AM38" s="56"/>
-      <c r="AN38" s="56"/>
-      <c r="AO38" s="56"/>
-      <c r="AP38" s="56"/>
-      <c r="AQ38" s="56"/>
-      <c r="AR38" s="56"/>
-      <c r="AS38" s="56"/>
-      <c r="AT38" s="56"/>
-      <c r="AU38" s="57"/>
+      <c r="AI38" s="74"/>
+      <c r="AJ38" s="76"/>
+      <c r="AK38" s="74"/>
+      <c r="AL38" s="74"/>
+      <c r="AM38" s="74"/>
+      <c r="AN38" s="74"/>
+      <c r="AO38" s="74"/>
+      <c r="AP38" s="74"/>
+      <c r="AQ38" s="74"/>
+      <c r="AR38" s="74"/>
+      <c r="AS38" s="74"/>
+      <c r="AT38" s="74"/>
+      <c r="AU38" s="75"/>
       <c r="AV38" s="16"/>
       <c r="AW38" s="16"/>
       <c r="AX38" s="16"/>
@@ -56076,11 +55988,24 @@
     </row>
   </sheetData>
   <mergeCells count="50">
-    <mergeCell ref="AA4:AC4"/>
-    <mergeCell ref="F37:S37"/>
-    <mergeCell ref="F38:H38"/>
-    <mergeCell ref="I38:S38"/>
-    <mergeCell ref="T37:AG37"/>
+    <mergeCell ref="R19:T19"/>
+    <mergeCell ref="R23:T23"/>
+    <mergeCell ref="R26:T26"/>
+    <mergeCell ref="R27:T27"/>
+    <mergeCell ref="R20:T20"/>
+    <mergeCell ref="AV17:BA17"/>
+    <mergeCell ref="AV18:BA18"/>
+    <mergeCell ref="AV19:BA19"/>
+    <mergeCell ref="U12:AU12"/>
+    <mergeCell ref="AV12:BA13"/>
+    <mergeCell ref="U13:AH13"/>
+    <mergeCell ref="AI13:AU13"/>
+    <mergeCell ref="AV16:BA16"/>
+    <mergeCell ref="A1:BA1"/>
+    <mergeCell ref="A2:BA2"/>
+    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="A7:E7"/>
+    <mergeCell ref="A11:D11"/>
     <mergeCell ref="AH37:AU37"/>
     <mergeCell ref="U38:AG38"/>
     <mergeCell ref="AH38:AI38"/>
@@ -56090,35 +56015,6 @@
     <mergeCell ref="AV26:BA26"/>
     <mergeCell ref="AV29:BA29"/>
     <mergeCell ref="AV31:BA31"/>
-    <mergeCell ref="B14:Q14"/>
-    <mergeCell ref="B18:Q18"/>
-    <mergeCell ref="A12:Q13"/>
-    <mergeCell ref="R12:T13"/>
-    <mergeCell ref="R14:T14"/>
-    <mergeCell ref="R29:T29"/>
-    <mergeCell ref="A1:BA1"/>
-    <mergeCell ref="A2:BA2"/>
-    <mergeCell ref="A6:D6"/>
-    <mergeCell ref="A7:E7"/>
-    <mergeCell ref="A11:D11"/>
-    <mergeCell ref="AV17:BA17"/>
-    <mergeCell ref="AV18:BA18"/>
-    <mergeCell ref="AV19:BA19"/>
-    <mergeCell ref="U12:AU12"/>
-    <mergeCell ref="AV12:BA13"/>
-    <mergeCell ref="U13:AH13"/>
-    <mergeCell ref="AI13:AU13"/>
-    <mergeCell ref="AV16:BA16"/>
-    <mergeCell ref="B23:Q23"/>
-    <mergeCell ref="B27:Q27"/>
-    <mergeCell ref="R16:T16"/>
-    <mergeCell ref="R17:T17"/>
-    <mergeCell ref="R18:T18"/>
-    <mergeCell ref="R19:T19"/>
-    <mergeCell ref="R23:T23"/>
-    <mergeCell ref="R26:T26"/>
-    <mergeCell ref="R27:T27"/>
-    <mergeCell ref="R20:T20"/>
     <mergeCell ref="T33:AG33"/>
     <mergeCell ref="T34:AG36"/>
     <mergeCell ref="R31:T31"/>
@@ -56126,6 +56022,22 @@
     <mergeCell ref="AH34:AU36"/>
     <mergeCell ref="F33:S33"/>
     <mergeCell ref="F34:S36"/>
+    <mergeCell ref="AA4:AC4"/>
+    <mergeCell ref="F37:S37"/>
+    <mergeCell ref="F38:H38"/>
+    <mergeCell ref="I38:S38"/>
+    <mergeCell ref="T37:AG37"/>
+    <mergeCell ref="B14:Q14"/>
+    <mergeCell ref="B18:Q18"/>
+    <mergeCell ref="A12:Q13"/>
+    <mergeCell ref="R12:T13"/>
+    <mergeCell ref="R14:T14"/>
+    <mergeCell ref="R29:T29"/>
+    <mergeCell ref="B23:Q23"/>
+    <mergeCell ref="B27:Q27"/>
+    <mergeCell ref="R16:T16"/>
+    <mergeCell ref="R17:T17"/>
+    <mergeCell ref="R18:T18"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>

</xml_diff>

<commit_message>
feat: Enhance IPP export functionality and update Excel template
</commit_message>
<xml_diff>
--- a/public/assets/file/Template IPP.xlsx
+++ b/public/assets/file/Template IPP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\core\public\assets\file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73DFC3D9-D14E-46E1-884B-8665C0D4D4D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4BCD898-0997-413D-A3C4-76C4C8AA5E1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="30">
   <si>
     <t>PERSONAL &amp; CONFIDENTIAL</t>
   </si>
@@ -52,13 +52,7 @@
     <t>:</t>
   </si>
   <si>
-    <t xml:space="preserve">Date of review : </t>
-  </si>
-  <si>
     <t>DEPARTMENT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PIC  Review : </t>
   </si>
   <si>
     <t>SECTION / SUB</t>
@@ -126,12 +120,21 @@
   <si>
     <t xml:space="preserve">NO FORM : </t>
   </si>
+  <si>
+    <t>FRM-HRD-S3-012-00</t>
+  </si>
+  <si>
+    <t>PIC  Review</t>
+  </si>
+  <si>
+    <t>Date of review</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -177,6 +180,12 @@
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -692,7 +701,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="130">
+  <cellXfs count="131">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -857,51 +866,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="17" fontId="6" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="17" fontId="6" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -926,11 +892,68 @@
     <xf numFmtId="9" fontId="6" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="3" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="17" fontId="6" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="17" fontId="6" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -940,7 +963,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -956,21 +981,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="5" fillId="3" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1265,8 +1275,8 @@
   </sheetPr>
   <dimension ref="A1:BU1000"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="U9" sqref="U9"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AK8" sqref="AK8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1280,133 +1290,136 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:73" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="104" t="s">
+      <c r="A1" s="115" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="92"/>
-      <c r="C1" s="92"/>
-      <c r="D1" s="92"/>
-      <c r="E1" s="92"/>
-      <c r="F1" s="92"/>
-      <c r="G1" s="92"/>
-      <c r="H1" s="92"/>
-      <c r="I1" s="92"/>
-      <c r="J1" s="92"/>
-      <c r="K1" s="92"/>
-      <c r="L1" s="92"/>
-      <c r="M1" s="92"/>
-      <c r="N1" s="92"/>
-      <c r="O1" s="92"/>
-      <c r="P1" s="92"/>
-      <c r="Q1" s="92"/>
-      <c r="R1" s="92"/>
-      <c r="S1" s="92"/>
-      <c r="T1" s="92"/>
-      <c r="U1" s="92"/>
-      <c r="V1" s="92"/>
-      <c r="W1" s="92"/>
-      <c r="X1" s="92"/>
-      <c r="Y1" s="92"/>
-      <c r="Z1" s="92"/>
-      <c r="AA1" s="92"/>
-      <c r="AB1" s="92"/>
-      <c r="AC1" s="92"/>
-      <c r="AD1" s="92"/>
-      <c r="AE1" s="92"/>
-      <c r="AF1" s="92"/>
-      <c r="AG1" s="92"/>
-      <c r="AH1" s="92"/>
-      <c r="AI1" s="92"/>
-      <c r="AJ1" s="92"/>
-      <c r="AK1" s="92"/>
-      <c r="AL1" s="92"/>
-      <c r="AM1" s="92"/>
-      <c r="AN1" s="92"/>
-      <c r="AO1" s="92"/>
-      <c r="AP1" s="92"/>
-      <c r="AQ1" s="92"/>
-      <c r="AR1" s="92"/>
-      <c r="AS1" s="92"/>
-      <c r="AT1" s="92"/>
-      <c r="AU1" s="92"/>
-      <c r="AV1" s="92"/>
-      <c r="AW1" s="92"/>
-      <c r="AX1" s="92"/>
-      <c r="AY1" s="92"/>
-      <c r="AZ1" s="92"/>
-      <c r="BA1" s="105"/>
+      <c r="B1" s="75"/>
+      <c r="C1" s="75"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="75"/>
+      <c r="F1" s="75"/>
+      <c r="G1" s="75"/>
+      <c r="H1" s="75"/>
+      <c r="I1" s="75"/>
+      <c r="J1" s="75"/>
+      <c r="K1" s="75"/>
+      <c r="L1" s="75"/>
+      <c r="M1" s="75"/>
+      <c r="N1" s="75"/>
+      <c r="O1" s="75"/>
+      <c r="P1" s="75"/>
+      <c r="Q1" s="75"/>
+      <c r="R1" s="75"/>
+      <c r="S1" s="75"/>
+      <c r="T1" s="75"/>
+      <c r="U1" s="75"/>
+      <c r="V1" s="75"/>
+      <c r="W1" s="75"/>
+      <c r="X1" s="75"/>
+      <c r="Y1" s="75"/>
+      <c r="Z1" s="75"/>
+      <c r="AA1" s="75"/>
+      <c r="AB1" s="75"/>
+      <c r="AC1" s="75"/>
+      <c r="AD1" s="75"/>
+      <c r="AE1" s="75"/>
+      <c r="AF1" s="75"/>
+      <c r="AG1" s="75"/>
+      <c r="AH1" s="75"/>
+      <c r="AI1" s="75"/>
+      <c r="AJ1" s="75"/>
+      <c r="AK1" s="75"/>
+      <c r="AL1" s="75"/>
+      <c r="AM1" s="75"/>
+      <c r="AN1" s="75"/>
+      <c r="AO1" s="75"/>
+      <c r="AP1" s="75"/>
+      <c r="AQ1" s="75"/>
+      <c r="AR1" s="75"/>
+      <c r="AS1" s="75"/>
+      <c r="AT1" s="75"/>
+      <c r="AU1" s="75"/>
+      <c r="AV1" s="75"/>
+      <c r="AW1" s="75"/>
+      <c r="AX1" s="75"/>
+      <c r="AY1" s="75"/>
+      <c r="AZ1" s="75"/>
+      <c r="BA1" s="108"/>
     </row>
     <row r="2" spans="1:73" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="106" t="s">
+      <c r="A2" s="116" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="79"/>
-      <c r="C2" s="79"/>
-      <c r="D2" s="79"/>
-      <c r="E2" s="79"/>
-      <c r="F2" s="79"/>
-      <c r="G2" s="79"/>
-      <c r="H2" s="79"/>
-      <c r="I2" s="79"/>
-      <c r="J2" s="79"/>
-      <c r="K2" s="79"/>
-      <c r="L2" s="79"/>
-      <c r="M2" s="79"/>
-      <c r="N2" s="79"/>
-      <c r="O2" s="79"/>
-      <c r="P2" s="79"/>
-      <c r="Q2" s="79"/>
-      <c r="R2" s="79"/>
-      <c r="S2" s="79"/>
-      <c r="T2" s="79"/>
-      <c r="U2" s="79"/>
-      <c r="V2" s="79"/>
-      <c r="W2" s="79"/>
-      <c r="X2" s="79"/>
-      <c r="Y2" s="79"/>
-      <c r="Z2" s="79"/>
-      <c r="AA2" s="79"/>
-      <c r="AB2" s="79"/>
-      <c r="AC2" s="79"/>
-      <c r="AD2" s="79"/>
-      <c r="AE2" s="79"/>
-      <c r="AF2" s="79"/>
-      <c r="AG2" s="79"/>
-      <c r="AH2" s="79"/>
-      <c r="AI2" s="79"/>
-      <c r="AJ2" s="79"/>
-      <c r="AK2" s="79"/>
-      <c r="AL2" s="79"/>
-      <c r="AM2" s="79"/>
-      <c r="AN2" s="79"/>
-      <c r="AO2" s="79"/>
-      <c r="AP2" s="79"/>
-      <c r="AQ2" s="79"/>
-      <c r="AR2" s="79"/>
-      <c r="AS2" s="79"/>
-      <c r="AT2" s="79"/>
-      <c r="AU2" s="79"/>
-      <c r="AV2" s="79"/>
-      <c r="AW2" s="79"/>
-      <c r="AX2" s="79"/>
-      <c r="AY2" s="79"/>
-      <c r="AZ2" s="79"/>
-      <c r="BA2" s="80"/>
+      <c r="B2" s="86"/>
+      <c r="C2" s="86"/>
+      <c r="D2" s="86"/>
+      <c r="E2" s="86"/>
+      <c r="F2" s="86"/>
+      <c r="G2" s="86"/>
+      <c r="H2" s="86"/>
+      <c r="I2" s="86"/>
+      <c r="J2" s="86"/>
+      <c r="K2" s="86"/>
+      <c r="L2" s="86"/>
+      <c r="M2" s="86"/>
+      <c r="N2" s="86"/>
+      <c r="O2" s="86"/>
+      <c r="P2" s="86"/>
+      <c r="Q2" s="86"/>
+      <c r="R2" s="86"/>
+      <c r="S2" s="86"/>
+      <c r="T2" s="86"/>
+      <c r="U2" s="86"/>
+      <c r="V2" s="86"/>
+      <c r="W2" s="86"/>
+      <c r="X2" s="86"/>
+      <c r="Y2" s="86"/>
+      <c r="Z2" s="86"/>
+      <c r="AA2" s="86"/>
+      <c r="AB2" s="86"/>
+      <c r="AC2" s="86"/>
+      <c r="AD2" s="86"/>
+      <c r="AE2" s="86"/>
+      <c r="AF2" s="86"/>
+      <c r="AG2" s="86"/>
+      <c r="AH2" s="86"/>
+      <c r="AI2" s="86"/>
+      <c r="AJ2" s="86"/>
+      <c r="AK2" s="86"/>
+      <c r="AL2" s="86"/>
+      <c r="AM2" s="86"/>
+      <c r="AN2" s="86"/>
+      <c r="AO2" s="86"/>
+      <c r="AP2" s="86"/>
+      <c r="AQ2" s="86"/>
+      <c r="AR2" s="86"/>
+      <c r="AS2" s="86"/>
+      <c r="AT2" s="86"/>
+      <c r="AU2" s="86"/>
+      <c r="AV2" s="86"/>
+      <c r="AW2" s="86"/>
+      <c r="AX2" s="86"/>
+      <c r="AY2" s="86"/>
+      <c r="AZ2" s="86"/>
+      <c r="BA2" s="102"/>
     </row>
     <row r="3" spans="1:73" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="V3" s="71" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
-      <c r="BA3" s="129"/>
+      <c r="Y3" s="73" t="s">
+        <v>27</v>
+      </c>
+      <c r="BA3" s="72"/>
       <c r="BU3" s="55"/>
     </row>
     <row r="4" spans="1:73" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="W4" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
-      <c r="AA4" s="72"/>
-      <c r="AB4" s="72"/>
-      <c r="AC4" s="72"/>
+      <c r="AA4" s="121"/>
+      <c r="AB4" s="121"/>
+      <c r="AC4" s="121"/>
       <c r="BA4" s="55"/>
     </row>
     <row r="5" spans="1:73" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -1465,10 +1478,10 @@
       <c r="BA5" s="4"/>
     </row>
     <row r="6" spans="1:73" ht="6" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="107"/>
-      <c r="B6" s="108"/>
-      <c r="C6" s="108"/>
-      <c r="D6" s="108"/>
+      <c r="A6" s="117"/>
+      <c r="B6" s="118"/>
+      <c r="C6" s="118"/>
+      <c r="D6" s="118"/>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
@@ -1520,13 +1533,13 @@
       <c r="BA6" s="6"/>
     </row>
     <row r="7" spans="1:73" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="109" t="s">
+      <c r="A7" s="119" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="79"/>
-      <c r="C7" s="79"/>
-      <c r="D7" s="79"/>
-      <c r="E7" s="79"/>
+      <c r="B7" s="86"/>
+      <c r="C7" s="86"/>
+      <c r="D7" s="86"/>
+      <c r="E7" s="86"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
@@ -1566,13 +1579,15 @@
       <c r="AN7" s="2"/>
       <c r="AO7" s="2"/>
       <c r="AP7" s="8" t="s">
-        <v>4</v>
+        <v>29</v>
       </c>
       <c r="AQ7" s="2"/>
       <c r="AR7" s="2"/>
       <c r="AS7" s="2"/>
       <c r="AT7" s="2"/>
-      <c r="AU7" s="2"/>
+      <c r="AU7" s="7" t="s">
+        <v>3</v>
+      </c>
       <c r="AV7" s="2"/>
       <c r="AW7" s="2"/>
       <c r="AX7" s="2"/>
@@ -1582,7 +1597,7 @@
     </row>
     <row r="8" spans="1:73" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
@@ -1627,13 +1642,15 @@
       <c r="AN8" s="2"/>
       <c r="AO8" s="2"/>
       <c r="AP8" s="3" t="s">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="AQ8" s="2"/>
       <c r="AR8" s="2"/>
       <c r="AS8" s="2"/>
       <c r="AT8" s="2"/>
-      <c r="AU8" s="2"/>
+      <c r="AU8" s="7" t="s">
+        <v>3</v>
+      </c>
       <c r="AV8" s="2"/>
       <c r="AW8" s="2"/>
       <c r="AX8" s="2"/>
@@ -1643,7 +1660,7 @@
     </row>
     <row r="9" spans="1:73" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="10" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -1702,7 +1719,7 @@
     </row>
     <row r="10" spans="1:73" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="10" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -1760,7 +1777,7 @@
       <c r="BA10" s="9"/>
     </row>
     <row r="11" spans="1:73" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="110"/>
+      <c r="A11" s="120"/>
       <c r="B11" s="111"/>
       <c r="C11" s="111"/>
       <c r="D11" s="111"/>
@@ -1815,154 +1832,154 @@
       <c r="BA11" s="13"/>
     </row>
     <row r="12" spans="1:73" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="91" t="s">
+      <c r="A12" s="74" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="75"/>
+      <c r="C12" s="75"/>
+      <c r="D12" s="75"/>
+      <c r="E12" s="75"/>
+      <c r="F12" s="75"/>
+      <c r="G12" s="75"/>
+      <c r="H12" s="75"/>
+      <c r="I12" s="75"/>
+      <c r="J12" s="75"/>
+      <c r="K12" s="75"/>
+      <c r="L12" s="75"/>
+      <c r="M12" s="75"/>
+      <c r="N12" s="75"/>
+      <c r="O12" s="75"/>
+      <c r="P12" s="75"/>
+      <c r="Q12" s="76"/>
+      <c r="R12" s="80" t="s">
+        <v>8</v>
+      </c>
+      <c r="S12" s="75"/>
+      <c r="T12" s="76"/>
+      <c r="U12" s="122" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="92"/>
-      <c r="C12" s="92"/>
-      <c r="D12" s="92"/>
-      <c r="E12" s="92"/>
-      <c r="F12" s="92"/>
-      <c r="G12" s="92"/>
-      <c r="H12" s="92"/>
-      <c r="I12" s="92"/>
-      <c r="J12" s="92"/>
-      <c r="K12" s="92"/>
-      <c r="L12" s="92"/>
-      <c r="M12" s="92"/>
-      <c r="N12" s="92"/>
-      <c r="O12" s="92"/>
-      <c r="P12" s="92"/>
-      <c r="Q12" s="93"/>
-      <c r="R12" s="97" t="s">
+      <c r="V12" s="123"/>
+      <c r="W12" s="123"/>
+      <c r="X12" s="123"/>
+      <c r="Y12" s="123"/>
+      <c r="Z12" s="123"/>
+      <c r="AA12" s="123"/>
+      <c r="AB12" s="123"/>
+      <c r="AC12" s="123"/>
+      <c r="AD12" s="123"/>
+      <c r="AE12" s="123"/>
+      <c r="AF12" s="123"/>
+      <c r="AG12" s="123"/>
+      <c r="AH12" s="123"/>
+      <c r="AI12" s="123"/>
+      <c r="AJ12" s="123"/>
+      <c r="AK12" s="123"/>
+      <c r="AL12" s="123"/>
+      <c r="AM12" s="123"/>
+      <c r="AN12" s="123"/>
+      <c r="AO12" s="123"/>
+      <c r="AP12" s="123"/>
+      <c r="AQ12" s="123"/>
+      <c r="AR12" s="123"/>
+      <c r="AS12" s="123"/>
+      <c r="AT12" s="123"/>
+      <c r="AU12" s="124"/>
+      <c r="AV12" s="125" t="s">
         <v>10</v>
       </c>
-      <c r="S12" s="92"/>
-      <c r="T12" s="93"/>
-      <c r="U12" s="112" t="s">
+      <c r="AW12" s="75"/>
+      <c r="AX12" s="75"/>
+      <c r="AY12" s="75"/>
+      <c r="AZ12" s="75"/>
+      <c r="BA12" s="108"/>
+    </row>
+    <row r="13" spans="1:73" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="77"/>
+      <c r="B13" s="78"/>
+      <c r="C13" s="78"/>
+      <c r="D13" s="78"/>
+      <c r="E13" s="78"/>
+      <c r="F13" s="78"/>
+      <c r="G13" s="78"/>
+      <c r="H13" s="78"/>
+      <c r="I13" s="78"/>
+      <c r="J13" s="78"/>
+      <c r="K13" s="78"/>
+      <c r="L13" s="78"/>
+      <c r="M13" s="78"/>
+      <c r="N13" s="78"/>
+      <c r="O13" s="78"/>
+      <c r="P13" s="78"/>
+      <c r="Q13" s="79"/>
+      <c r="R13" s="81"/>
+      <c r="S13" s="78"/>
+      <c r="T13" s="79"/>
+      <c r="U13" s="127" t="s">
         <v>11</v>
       </c>
-      <c r="V12" s="113"/>
-      <c r="W12" s="113"/>
-      <c r="X12" s="113"/>
-      <c r="Y12" s="113"/>
-      <c r="Z12" s="113"/>
-      <c r="AA12" s="113"/>
-      <c r="AB12" s="113"/>
-      <c r="AC12" s="113"/>
-      <c r="AD12" s="113"/>
-      <c r="AE12" s="113"/>
-      <c r="AF12" s="113"/>
-      <c r="AG12" s="113"/>
-      <c r="AH12" s="113"/>
-      <c r="AI12" s="113"/>
-      <c r="AJ12" s="113"/>
-      <c r="AK12" s="113"/>
-      <c r="AL12" s="113"/>
-      <c r="AM12" s="113"/>
-      <c r="AN12" s="113"/>
-      <c r="AO12" s="113"/>
-      <c r="AP12" s="113"/>
-      <c r="AQ12" s="113"/>
-      <c r="AR12" s="113"/>
-      <c r="AS12" s="113"/>
-      <c r="AT12" s="113"/>
-      <c r="AU12" s="114"/>
-      <c r="AV12" s="115" t="s">
+      <c r="V13" s="128"/>
+      <c r="W13" s="128"/>
+      <c r="X13" s="128"/>
+      <c r="Y13" s="128"/>
+      <c r="Z13" s="128"/>
+      <c r="AA13" s="128"/>
+      <c r="AB13" s="128"/>
+      <c r="AC13" s="128"/>
+      <c r="AD13" s="128"/>
+      <c r="AE13" s="128"/>
+      <c r="AF13" s="128"/>
+      <c r="AG13" s="128"/>
+      <c r="AH13" s="129"/>
+      <c r="AI13" s="127" t="s">
         <v>12</v>
       </c>
-      <c r="AW12" s="92"/>
-      <c r="AX12" s="92"/>
-      <c r="AY12" s="92"/>
-      <c r="AZ12" s="92"/>
-      <c r="BA12" s="105"/>
-    </row>
-    <row r="13" spans="1:73" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="94"/>
-      <c r="B13" s="95"/>
-      <c r="C13" s="95"/>
-      <c r="D13" s="95"/>
-      <c r="E13" s="95"/>
-      <c r="F13" s="95"/>
-      <c r="G13" s="95"/>
-      <c r="H13" s="95"/>
-      <c r="I13" s="95"/>
-      <c r="J13" s="95"/>
-      <c r="K13" s="95"/>
-      <c r="L13" s="95"/>
-      <c r="M13" s="95"/>
-      <c r="N13" s="95"/>
-      <c r="O13" s="95"/>
-      <c r="P13" s="95"/>
-      <c r="Q13" s="96"/>
-      <c r="R13" s="98"/>
-      <c r="S13" s="95"/>
-      <c r="T13" s="96"/>
-      <c r="U13" s="117" t="s">
+      <c r="AJ13" s="128"/>
+      <c r="AK13" s="128"/>
+      <c r="AL13" s="128"/>
+      <c r="AM13" s="128"/>
+      <c r="AN13" s="128"/>
+      <c r="AO13" s="128"/>
+      <c r="AP13" s="128"/>
+      <c r="AQ13" s="128"/>
+      <c r="AR13" s="128"/>
+      <c r="AS13" s="128"/>
+      <c r="AT13" s="128"/>
+      <c r="AU13" s="130"/>
+      <c r="AV13" s="78"/>
+      <c r="AW13" s="78"/>
+      <c r="AX13" s="78"/>
+      <c r="AY13" s="78"/>
+      <c r="AZ13" s="78"/>
+      <c r="BA13" s="126"/>
+    </row>
+    <row r="14" spans="1:73" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="V13" s="118"/>
-      <c r="W13" s="118"/>
-      <c r="X13" s="118"/>
-      <c r="Y13" s="118"/>
-      <c r="Z13" s="118"/>
-      <c r="AA13" s="118"/>
-      <c r="AB13" s="118"/>
-      <c r="AC13" s="118"/>
-      <c r="AD13" s="118"/>
-      <c r="AE13" s="118"/>
-      <c r="AF13" s="118"/>
-      <c r="AG13" s="118"/>
-      <c r="AH13" s="119"/>
-      <c r="AI13" s="117" t="s">
+      <c r="B14" s="98" t="s">
         <v>14</v>
       </c>
-      <c r="AJ13" s="118"/>
-      <c r="AK13" s="118"/>
-      <c r="AL13" s="118"/>
-      <c r="AM13" s="118"/>
-      <c r="AN13" s="118"/>
-      <c r="AO13" s="118"/>
-      <c r="AP13" s="118"/>
-      <c r="AQ13" s="118"/>
-      <c r="AR13" s="118"/>
-      <c r="AS13" s="118"/>
-      <c r="AT13" s="118"/>
-      <c r="AU13" s="120"/>
-      <c r="AV13" s="95"/>
-      <c r="AW13" s="95"/>
-      <c r="AX13" s="95"/>
-      <c r="AY13" s="95"/>
-      <c r="AZ13" s="95"/>
-      <c r="BA13" s="116"/>
-    </row>
-    <row r="14" spans="1:73" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" s="85" t="s">
-        <v>16</v>
-      </c>
-      <c r="C14" s="86"/>
-      <c r="D14" s="86"/>
-      <c r="E14" s="86"/>
-      <c r="F14" s="86"/>
-      <c r="G14" s="86"/>
-      <c r="H14" s="86"/>
-      <c r="I14" s="86"/>
-      <c r="J14" s="86"/>
-      <c r="K14" s="86"/>
-      <c r="L14" s="86"/>
-      <c r="M14" s="86"/>
-      <c r="N14" s="86"/>
-      <c r="O14" s="86"/>
-      <c r="P14" s="86"/>
-      <c r="Q14" s="87"/>
-      <c r="R14" s="99">
+      <c r="C14" s="99"/>
+      <c r="D14" s="99"/>
+      <c r="E14" s="99"/>
+      <c r="F14" s="99"/>
+      <c r="G14" s="99"/>
+      <c r="H14" s="99"/>
+      <c r="I14" s="99"/>
+      <c r="J14" s="99"/>
+      <c r="K14" s="99"/>
+      <c r="L14" s="99"/>
+      <c r="M14" s="99"/>
+      <c r="N14" s="99"/>
+      <c r="O14" s="99"/>
+      <c r="P14" s="99"/>
+      <c r="Q14" s="100"/>
+      <c r="R14" s="82">
         <v>0.7</v>
       </c>
-      <c r="S14" s="100"/>
-      <c r="T14" s="101"/>
+      <c r="S14" s="83"/>
+      <c r="T14" s="84"/>
       <c r="U14" s="58"/>
       <c r="V14" s="59"/>
       <c r="W14" s="59"/>
@@ -2047,19 +2064,19 @@
       <c r="O16" s="45"/>
       <c r="P16" s="45"/>
       <c r="Q16" s="45"/>
-      <c r="R16" s="102"/>
-      <c r="S16" s="79"/>
-      <c r="T16" s="103"/>
+      <c r="R16" s="85"/>
+      <c r="S16" s="86"/>
+      <c r="T16" s="87"/>
       <c r="U16" s="49"/>
       <c r="AH16" s="47"/>
       <c r="AI16" s="49"/>
       <c r="AU16" s="56"/>
-      <c r="AV16" s="78"/>
-      <c r="AW16" s="79"/>
-      <c r="AX16" s="79"/>
-      <c r="AY16" s="79"/>
-      <c r="AZ16" s="79"/>
-      <c r="BA16" s="80"/>
+      <c r="AV16" s="101"/>
+      <c r="AW16" s="86"/>
+      <c r="AX16" s="86"/>
+      <c r="AY16" s="86"/>
+      <c r="AZ16" s="86"/>
+      <c r="BA16" s="102"/>
     </row>
     <row r="17" spans="1:53" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="15"/>
@@ -2079,26 +2096,26 @@
       <c r="O17" s="45"/>
       <c r="P17" s="45"/>
       <c r="Q17" s="45"/>
-      <c r="R17" s="102"/>
-      <c r="S17" s="79"/>
-      <c r="T17" s="103"/>
+      <c r="R17" s="85"/>
+      <c r="S17" s="86"/>
+      <c r="T17" s="87"/>
       <c r="U17" s="49"/>
       <c r="AH17" s="47"/>
       <c r="AI17" s="49"/>
       <c r="AU17" s="56"/>
-      <c r="AV17" s="78"/>
-      <c r="AW17" s="79"/>
-      <c r="AX17" s="79"/>
-      <c r="AY17" s="79"/>
-      <c r="AZ17" s="79"/>
-      <c r="BA17" s="80"/>
+      <c r="AV17" s="101"/>
+      <c r="AW17" s="86"/>
+      <c r="AX17" s="86"/>
+      <c r="AY17" s="86"/>
+      <c r="AZ17" s="86"/>
+      <c r="BA17" s="102"/>
     </row>
     <row r="18" spans="1:53" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="22" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B18" s="88" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C18" s="89"/>
       <c r="D18" s="89"/>
@@ -2115,11 +2132,11 @@
       <c r="O18" s="89"/>
       <c r="P18" s="89"/>
       <c r="Q18" s="90"/>
-      <c r="R18" s="121">
+      <c r="R18" s="91">
         <v>0.1</v>
       </c>
-      <c r="S18" s="122"/>
-      <c r="T18" s="103"/>
+      <c r="S18" s="92"/>
+      <c r="T18" s="87"/>
       <c r="U18" s="65"/>
       <c r="V18" s="66"/>
       <c r="W18" s="66"/>
@@ -2147,12 +2164,12 @@
       <c r="AS18" s="66"/>
       <c r="AT18" s="66"/>
       <c r="AU18" s="68"/>
-      <c r="AV18" s="81"/>
-      <c r="AW18" s="82"/>
-      <c r="AX18" s="82"/>
-      <c r="AY18" s="82"/>
-      <c r="AZ18" s="82"/>
-      <c r="BA18" s="83"/>
+      <c r="AV18" s="103"/>
+      <c r="AW18" s="104"/>
+      <c r="AX18" s="104"/>
+      <c r="AY18" s="104"/>
+      <c r="AZ18" s="104"/>
+      <c r="BA18" s="105"/>
     </row>
     <row r="19" spans="1:53" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="15"/>
@@ -2172,19 +2189,19 @@
       <c r="O19" s="45"/>
       <c r="P19" s="45"/>
       <c r="Q19" s="45"/>
-      <c r="R19" s="102"/>
-      <c r="S19" s="79"/>
-      <c r="T19" s="103"/>
+      <c r="R19" s="85"/>
+      <c r="S19" s="86"/>
+      <c r="T19" s="87"/>
       <c r="U19" s="49"/>
       <c r="AH19" s="47"/>
       <c r="AI19" s="49"/>
       <c r="AU19" s="56"/>
-      <c r="AV19" s="78"/>
-      <c r="AW19" s="79"/>
-      <c r="AX19" s="79"/>
-      <c r="AY19" s="79"/>
-      <c r="AZ19" s="79"/>
-      <c r="BA19" s="80"/>
+      <c r="AV19" s="101"/>
+      <c r="AW19" s="86"/>
+      <c r="AX19" s="86"/>
+      <c r="AY19" s="86"/>
+      <c r="AZ19" s="86"/>
+      <c r="BA19" s="102"/>
     </row>
     <row r="20" spans="1:53" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="15"/>
@@ -2204,19 +2221,19 @@
       <c r="O20" s="45"/>
       <c r="P20" s="45"/>
       <c r="Q20" s="45"/>
-      <c r="R20" s="102"/>
-      <c r="S20" s="79"/>
-      <c r="T20" s="103"/>
+      <c r="R20" s="85"/>
+      <c r="S20" s="86"/>
+      <c r="T20" s="87"/>
       <c r="U20" s="49"/>
       <c r="AH20" s="47"/>
       <c r="AI20" s="49"/>
       <c r="AU20" s="56"/>
-      <c r="AV20" s="78"/>
-      <c r="AW20" s="79"/>
-      <c r="AX20" s="79"/>
-      <c r="AY20" s="79"/>
-      <c r="AZ20" s="79"/>
-      <c r="BA20" s="80"/>
+      <c r="AV20" s="101"/>
+      <c r="AW20" s="86"/>
+      <c r="AX20" s="86"/>
+      <c r="AY20" s="86"/>
+      <c r="AZ20" s="86"/>
+      <c r="BA20" s="102"/>
     </row>
     <row r="21" spans="1:53" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="15"/>
@@ -2284,10 +2301,10 @@
     </row>
     <row r="23" spans="1:53" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="22" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B23" s="88" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C23" s="89"/>
       <c r="D23" s="89"/>
@@ -2304,11 +2321,11 @@
       <c r="O23" s="89"/>
       <c r="P23" s="89"/>
       <c r="Q23" s="90"/>
-      <c r="R23" s="121">
+      <c r="R23" s="91">
         <v>0.1</v>
       </c>
-      <c r="S23" s="122"/>
-      <c r="T23" s="103"/>
+      <c r="S23" s="92"/>
+      <c r="T23" s="87"/>
       <c r="U23" s="65"/>
       <c r="V23" s="66"/>
       <c r="W23" s="66"/>
@@ -2336,12 +2353,12 @@
       <c r="AS23" s="66"/>
       <c r="AT23" s="66"/>
       <c r="AU23" s="68"/>
-      <c r="AV23" s="81"/>
-      <c r="AW23" s="82"/>
-      <c r="AX23" s="82"/>
-      <c r="AY23" s="82"/>
-      <c r="AZ23" s="82"/>
-      <c r="BA23" s="83"/>
+      <c r="AV23" s="103"/>
+      <c r="AW23" s="104"/>
+      <c r="AX23" s="104"/>
+      <c r="AY23" s="104"/>
+      <c r="AZ23" s="104"/>
+      <c r="BA23" s="105"/>
     </row>
     <row r="24" spans="1:53" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="15"/>
@@ -2425,26 +2442,26 @@
       <c r="O26" s="20"/>
       <c r="P26" s="20"/>
       <c r="Q26" s="53"/>
-      <c r="R26" s="102"/>
-      <c r="S26" s="79"/>
-      <c r="T26" s="103"/>
+      <c r="R26" s="85"/>
+      <c r="S26" s="86"/>
+      <c r="T26" s="87"/>
       <c r="U26" s="49"/>
       <c r="AH26" s="47"/>
       <c r="AI26" s="49"/>
       <c r="AU26" s="56"/>
-      <c r="AV26" s="78"/>
-      <c r="AW26" s="79"/>
-      <c r="AX26" s="79"/>
-      <c r="AY26" s="79"/>
-      <c r="AZ26" s="79"/>
-      <c r="BA26" s="80"/>
+      <c r="AV26" s="101"/>
+      <c r="AW26" s="86"/>
+      <c r="AX26" s="86"/>
+      <c r="AY26" s="86"/>
+      <c r="AZ26" s="86"/>
+      <c r="BA26" s="102"/>
     </row>
     <row r="27" spans="1:53" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="22" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B27" s="88" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C27" s="89"/>
       <c r="D27" s="89"/>
@@ -2461,11 +2478,11 @@
       <c r="O27" s="89"/>
       <c r="P27" s="89"/>
       <c r="Q27" s="90"/>
-      <c r="R27" s="121">
+      <c r="R27" s="91">
         <v>0.1</v>
       </c>
-      <c r="S27" s="122"/>
-      <c r="T27" s="103"/>
+      <c r="S27" s="92"/>
+      <c r="T27" s="87"/>
       <c r="U27" s="65"/>
       <c r="V27" s="66"/>
       <c r="W27" s="66"/>
@@ -2550,19 +2567,19 @@
       <c r="O29" s="20"/>
       <c r="P29" s="20"/>
       <c r="Q29" s="53"/>
-      <c r="R29" s="102"/>
-      <c r="S29" s="79"/>
-      <c r="T29" s="103"/>
+      <c r="R29" s="85"/>
+      <c r="S29" s="86"/>
+      <c r="T29" s="87"/>
       <c r="U29" s="49"/>
       <c r="AH29" s="47"/>
       <c r="AI29" s="49"/>
       <c r="AU29" s="56"/>
-      <c r="AV29" s="78"/>
-      <c r="AW29" s="79"/>
-      <c r="AX29" s="79"/>
-      <c r="AY29" s="79"/>
-      <c r="AZ29" s="79"/>
-      <c r="BA29" s="80"/>
+      <c r="AV29" s="101"/>
+      <c r="AW29" s="86"/>
+      <c r="AX29" s="86"/>
+      <c r="AY29" s="86"/>
+      <c r="AZ29" s="86"/>
+      <c r="BA29" s="102"/>
     </row>
     <row r="30" spans="1:53" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="29"/>
@@ -2637,12 +2654,12 @@
       <c r="O31" s="30"/>
       <c r="P31" s="30"/>
       <c r="Q31" s="31"/>
-      <c r="R31" s="127">
+      <c r="R31" s="113">
         <f>+R14+R18+R23+R27</f>
         <v>0.99999999999999989</v>
       </c>
-      <c r="S31" s="74"/>
-      <c r="T31" s="128"/>
+      <c r="S31" s="94"/>
+      <c r="T31" s="114"/>
       <c r="U31" s="38"/>
       <c r="V31" s="36"/>
       <c r="W31" s="36"/>
@@ -2670,12 +2687,12 @@
       <c r="AS31" s="30"/>
       <c r="AT31" s="30"/>
       <c r="AU31" s="39"/>
-      <c r="AV31" s="84"/>
-      <c r="AW31" s="74"/>
-      <c r="AX31" s="74"/>
-      <c r="AY31" s="74"/>
-      <c r="AZ31" s="74"/>
-      <c r="BA31" s="75"/>
+      <c r="AV31" s="106"/>
+      <c r="AW31" s="94"/>
+      <c r="AX31" s="94"/>
+      <c r="AY31" s="94"/>
+      <c r="AZ31" s="94"/>
+      <c r="BA31" s="95"/>
     </row>
     <row r="32" spans="1:53" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A32" s="40"/>
@@ -2738,54 +2755,54 @@
       <c r="C33" s="45"/>
       <c r="D33" s="45"/>
       <c r="E33" s="45"/>
-      <c r="F33" s="77" t="s">
+      <c r="F33" s="97" t="s">
+        <v>21</v>
+      </c>
+      <c r="G33" s="94"/>
+      <c r="H33" s="94"/>
+      <c r="I33" s="94"/>
+      <c r="J33" s="94"/>
+      <c r="K33" s="94"/>
+      <c r="L33" s="94"/>
+      <c r="M33" s="94"/>
+      <c r="N33" s="94"/>
+      <c r="O33" s="94"/>
+      <c r="P33" s="94"/>
+      <c r="Q33" s="94"/>
+      <c r="R33" s="94"/>
+      <c r="S33" s="95"/>
+      <c r="T33" s="97" t="s">
+        <v>22</v>
+      </c>
+      <c r="U33" s="94"/>
+      <c r="V33" s="94"/>
+      <c r="W33" s="94"/>
+      <c r="X33" s="94"/>
+      <c r="Y33" s="94"/>
+      <c r="Z33" s="94"/>
+      <c r="AA33" s="94"/>
+      <c r="AB33" s="94"/>
+      <c r="AC33" s="94"/>
+      <c r="AD33" s="94"/>
+      <c r="AE33" s="94"/>
+      <c r="AF33" s="94"/>
+      <c r="AG33" s="95"/>
+      <c r="AH33" s="97" t="s">
         <v>23</v>
       </c>
-      <c r="G33" s="74"/>
-      <c r="H33" s="74"/>
-      <c r="I33" s="74"/>
-      <c r="J33" s="74"/>
-      <c r="K33" s="74"/>
-      <c r="L33" s="74"/>
-      <c r="M33" s="74"/>
-      <c r="N33" s="74"/>
-      <c r="O33" s="74"/>
-      <c r="P33" s="74"/>
-      <c r="Q33" s="74"/>
-      <c r="R33" s="74"/>
-      <c r="S33" s="75"/>
-      <c r="T33" s="77" t="s">
-        <v>24</v>
-      </c>
-      <c r="U33" s="74"/>
-      <c r="V33" s="74"/>
-      <c r="W33" s="74"/>
-      <c r="X33" s="74"/>
-      <c r="Y33" s="74"/>
-      <c r="Z33" s="74"/>
-      <c r="AA33" s="74"/>
-      <c r="AB33" s="74"/>
-      <c r="AC33" s="74"/>
-      <c r="AD33" s="74"/>
-      <c r="AE33" s="74"/>
-      <c r="AF33" s="74"/>
-      <c r="AG33" s="75"/>
-      <c r="AH33" s="77" t="s">
-        <v>25</v>
-      </c>
-      <c r="AI33" s="74"/>
-      <c r="AJ33" s="74"/>
-      <c r="AK33" s="74"/>
-      <c r="AL33" s="74"/>
-      <c r="AM33" s="74"/>
-      <c r="AN33" s="74"/>
-      <c r="AO33" s="74"/>
-      <c r="AP33" s="74"/>
-      <c r="AQ33" s="74"/>
-      <c r="AR33" s="74"/>
-      <c r="AS33" s="74"/>
-      <c r="AT33" s="74"/>
-      <c r="AU33" s="75"/>
+      <c r="AI33" s="94"/>
+      <c r="AJ33" s="94"/>
+      <c r="AK33" s="94"/>
+      <c r="AL33" s="94"/>
+      <c r="AM33" s="94"/>
+      <c r="AN33" s="94"/>
+      <c r="AO33" s="94"/>
+      <c r="AP33" s="94"/>
+      <c r="AQ33" s="94"/>
+      <c r="AR33" s="94"/>
+      <c r="AS33" s="94"/>
+      <c r="AT33" s="94"/>
+      <c r="AU33" s="95"/>
       <c r="AV33" s="45"/>
       <c r="AW33" s="45"/>
       <c r="AX33" s="45"/>
@@ -2799,48 +2816,48 @@
       <c r="C34" s="20"/>
       <c r="D34" s="20"/>
       <c r="E34" s="20"/>
-      <c r="F34" s="123"/>
-      <c r="G34" s="92"/>
-      <c r="H34" s="92"/>
-      <c r="I34" s="92"/>
-      <c r="J34" s="92"/>
-      <c r="K34" s="92"/>
-      <c r="L34" s="92"/>
-      <c r="M34" s="92"/>
-      <c r="N34" s="92"/>
-      <c r="O34" s="92"/>
-      <c r="P34" s="92"/>
-      <c r="Q34" s="92"/>
-      <c r="R34" s="92"/>
-      <c r="S34" s="105"/>
-      <c r="T34" s="123"/>
-      <c r="U34" s="92"/>
-      <c r="V34" s="92"/>
-      <c r="W34" s="92"/>
-      <c r="X34" s="92"/>
-      <c r="Y34" s="92"/>
-      <c r="Z34" s="92"/>
-      <c r="AA34" s="92"/>
-      <c r="AB34" s="92"/>
-      <c r="AC34" s="92"/>
-      <c r="AD34" s="92"/>
-      <c r="AE34" s="92"/>
-      <c r="AF34" s="92"/>
-      <c r="AG34" s="105"/>
-      <c r="AH34" s="123"/>
-      <c r="AI34" s="92"/>
-      <c r="AJ34" s="92"/>
-      <c r="AK34" s="92"/>
-      <c r="AL34" s="92"/>
-      <c r="AM34" s="92"/>
-      <c r="AN34" s="92"/>
-      <c r="AO34" s="92"/>
-      <c r="AP34" s="92"/>
-      <c r="AQ34" s="92"/>
-      <c r="AR34" s="92"/>
-      <c r="AS34" s="92"/>
-      <c r="AT34" s="92"/>
-      <c r="AU34" s="105"/>
+      <c r="F34" s="107"/>
+      <c r="G34" s="75"/>
+      <c r="H34" s="75"/>
+      <c r="I34" s="75"/>
+      <c r="J34" s="75"/>
+      <c r="K34" s="75"/>
+      <c r="L34" s="75"/>
+      <c r="M34" s="75"/>
+      <c r="N34" s="75"/>
+      <c r="O34" s="75"/>
+      <c r="P34" s="75"/>
+      <c r="Q34" s="75"/>
+      <c r="R34" s="75"/>
+      <c r="S34" s="108"/>
+      <c r="T34" s="107"/>
+      <c r="U34" s="75"/>
+      <c r="V34" s="75"/>
+      <c r="W34" s="75"/>
+      <c r="X34" s="75"/>
+      <c r="Y34" s="75"/>
+      <c r="Z34" s="75"/>
+      <c r="AA34" s="75"/>
+      <c r="AB34" s="75"/>
+      <c r="AC34" s="75"/>
+      <c r="AD34" s="75"/>
+      <c r="AE34" s="75"/>
+      <c r="AF34" s="75"/>
+      <c r="AG34" s="108"/>
+      <c r="AH34" s="107"/>
+      <c r="AI34" s="75"/>
+      <c r="AJ34" s="75"/>
+      <c r="AK34" s="75"/>
+      <c r="AL34" s="75"/>
+      <c r="AM34" s="75"/>
+      <c r="AN34" s="75"/>
+      <c r="AO34" s="75"/>
+      <c r="AP34" s="75"/>
+      <c r="AQ34" s="75"/>
+      <c r="AR34" s="75"/>
+      <c r="AS34" s="75"/>
+      <c r="AT34" s="75"/>
+      <c r="AU34" s="108"/>
       <c r="AV34" s="20"/>
       <c r="AW34" s="20"/>
       <c r="AX34" s="20"/>
@@ -2854,48 +2871,48 @@
       <c r="C35" s="20"/>
       <c r="D35" s="20"/>
       <c r="E35" s="20"/>
-      <c r="F35" s="124"/>
-      <c r="G35" s="79"/>
-      <c r="H35" s="79"/>
-      <c r="I35" s="79"/>
-      <c r="J35" s="79"/>
-      <c r="K35" s="79"/>
-      <c r="L35" s="79"/>
-      <c r="M35" s="79"/>
-      <c r="N35" s="79"/>
-      <c r="O35" s="79"/>
-      <c r="P35" s="79"/>
-      <c r="Q35" s="79"/>
-      <c r="R35" s="79"/>
-      <c r="S35" s="80"/>
-      <c r="T35" s="124"/>
-      <c r="U35" s="79"/>
-      <c r="V35" s="79"/>
-      <c r="W35" s="79"/>
-      <c r="X35" s="79"/>
-      <c r="Y35" s="79"/>
-      <c r="Z35" s="79"/>
-      <c r="AA35" s="79"/>
-      <c r="AB35" s="79"/>
-      <c r="AC35" s="79"/>
-      <c r="AD35" s="79"/>
-      <c r="AE35" s="79"/>
-      <c r="AF35" s="79"/>
-      <c r="AG35" s="80"/>
-      <c r="AH35" s="124"/>
-      <c r="AI35" s="79"/>
-      <c r="AJ35" s="79"/>
-      <c r="AK35" s="79"/>
-      <c r="AL35" s="79"/>
-      <c r="AM35" s="79"/>
-      <c r="AN35" s="79"/>
-      <c r="AO35" s="79"/>
-      <c r="AP35" s="79"/>
-      <c r="AQ35" s="79"/>
-      <c r="AR35" s="79"/>
-      <c r="AS35" s="79"/>
-      <c r="AT35" s="79"/>
-      <c r="AU35" s="80"/>
+      <c r="F35" s="109"/>
+      <c r="G35" s="86"/>
+      <c r="H35" s="86"/>
+      <c r="I35" s="86"/>
+      <c r="J35" s="86"/>
+      <c r="K35" s="86"/>
+      <c r="L35" s="86"/>
+      <c r="M35" s="86"/>
+      <c r="N35" s="86"/>
+      <c r="O35" s="86"/>
+      <c r="P35" s="86"/>
+      <c r="Q35" s="86"/>
+      <c r="R35" s="86"/>
+      <c r="S35" s="102"/>
+      <c r="T35" s="109"/>
+      <c r="U35" s="86"/>
+      <c r="V35" s="86"/>
+      <c r="W35" s="86"/>
+      <c r="X35" s="86"/>
+      <c r="Y35" s="86"/>
+      <c r="Z35" s="86"/>
+      <c r="AA35" s="86"/>
+      <c r="AB35" s="86"/>
+      <c r="AC35" s="86"/>
+      <c r="AD35" s="86"/>
+      <c r="AE35" s="86"/>
+      <c r="AF35" s="86"/>
+      <c r="AG35" s="102"/>
+      <c r="AH35" s="109"/>
+      <c r="AI35" s="86"/>
+      <c r="AJ35" s="86"/>
+      <c r="AK35" s="86"/>
+      <c r="AL35" s="86"/>
+      <c r="AM35" s="86"/>
+      <c r="AN35" s="86"/>
+      <c r="AO35" s="86"/>
+      <c r="AP35" s="86"/>
+      <c r="AQ35" s="86"/>
+      <c r="AR35" s="86"/>
+      <c r="AS35" s="86"/>
+      <c r="AT35" s="86"/>
+      <c r="AU35" s="102"/>
       <c r="AV35" s="20"/>
       <c r="AW35" s="20"/>
       <c r="AX35" s="20"/>
@@ -2909,7 +2926,7 @@
       <c r="C36" s="20"/>
       <c r="D36" s="20"/>
       <c r="E36" s="20"/>
-      <c r="F36" s="125"/>
+      <c r="F36" s="110"/>
       <c r="G36" s="111"/>
       <c r="H36" s="111"/>
       <c r="I36" s="111"/>
@@ -2922,8 +2939,8 @@
       <c r="P36" s="111"/>
       <c r="Q36" s="111"/>
       <c r="R36" s="111"/>
-      <c r="S36" s="126"/>
-      <c r="T36" s="125"/>
+      <c r="S36" s="112"/>
+      <c r="T36" s="110"/>
       <c r="U36" s="111"/>
       <c r="V36" s="111"/>
       <c r="W36" s="111"/>
@@ -2936,8 +2953,8 @@
       <c r="AD36" s="111"/>
       <c r="AE36" s="111"/>
       <c r="AF36" s="111"/>
-      <c r="AG36" s="126"/>
-      <c r="AH36" s="125"/>
+      <c r="AG36" s="112"/>
+      <c r="AH36" s="110"/>
       <c r="AI36" s="111"/>
       <c r="AJ36" s="111"/>
       <c r="AK36" s="111"/>
@@ -2950,7 +2967,7 @@
       <c r="AR36" s="111"/>
       <c r="AS36" s="111"/>
       <c r="AT36" s="111"/>
-      <c r="AU36" s="126"/>
+      <c r="AU36" s="112"/>
       <c r="AV36" s="20"/>
       <c r="AW36" s="20"/>
       <c r="AX36" s="20"/>
@@ -2964,48 +2981,48 @@
       <c r="C37" s="20"/>
       <c r="D37" s="20"/>
       <c r="E37" s="20"/>
-      <c r="F37" s="73"/>
-      <c r="G37" s="74"/>
-      <c r="H37" s="74"/>
-      <c r="I37" s="74"/>
-      <c r="J37" s="74"/>
-      <c r="K37" s="74"/>
-      <c r="L37" s="74"/>
-      <c r="M37" s="74"/>
-      <c r="N37" s="74"/>
-      <c r="O37" s="74"/>
-      <c r="P37" s="74"/>
-      <c r="Q37" s="74"/>
-      <c r="R37" s="74"/>
-      <c r="S37" s="75"/>
-      <c r="T37" s="77"/>
-      <c r="U37" s="74"/>
-      <c r="V37" s="74"/>
-      <c r="W37" s="74"/>
-      <c r="X37" s="74"/>
-      <c r="Y37" s="74"/>
-      <c r="Z37" s="74"/>
-      <c r="AA37" s="74"/>
-      <c r="AB37" s="74"/>
-      <c r="AC37" s="74"/>
-      <c r="AD37" s="74"/>
-      <c r="AE37" s="74"/>
-      <c r="AF37" s="74"/>
-      <c r="AG37" s="75"/>
-      <c r="AH37" s="73"/>
-      <c r="AI37" s="74"/>
-      <c r="AJ37" s="74"/>
-      <c r="AK37" s="74"/>
-      <c r="AL37" s="74"/>
-      <c r="AM37" s="74"/>
-      <c r="AN37" s="74"/>
-      <c r="AO37" s="74"/>
-      <c r="AP37" s="74"/>
-      <c r="AQ37" s="74"/>
-      <c r="AR37" s="74"/>
-      <c r="AS37" s="74"/>
-      <c r="AT37" s="74"/>
-      <c r="AU37" s="75"/>
+      <c r="F37" s="93"/>
+      <c r="G37" s="94"/>
+      <c r="H37" s="94"/>
+      <c r="I37" s="94"/>
+      <c r="J37" s="94"/>
+      <c r="K37" s="94"/>
+      <c r="L37" s="94"/>
+      <c r="M37" s="94"/>
+      <c r="N37" s="94"/>
+      <c r="O37" s="94"/>
+      <c r="P37" s="94"/>
+      <c r="Q37" s="94"/>
+      <c r="R37" s="94"/>
+      <c r="S37" s="95"/>
+      <c r="T37" s="97"/>
+      <c r="U37" s="94"/>
+      <c r="V37" s="94"/>
+      <c r="W37" s="94"/>
+      <c r="X37" s="94"/>
+      <c r="Y37" s="94"/>
+      <c r="Z37" s="94"/>
+      <c r="AA37" s="94"/>
+      <c r="AB37" s="94"/>
+      <c r="AC37" s="94"/>
+      <c r="AD37" s="94"/>
+      <c r="AE37" s="94"/>
+      <c r="AF37" s="94"/>
+      <c r="AG37" s="95"/>
+      <c r="AH37" s="93"/>
+      <c r="AI37" s="94"/>
+      <c r="AJ37" s="94"/>
+      <c r="AK37" s="94"/>
+      <c r="AL37" s="94"/>
+      <c r="AM37" s="94"/>
+      <c r="AN37" s="94"/>
+      <c r="AO37" s="94"/>
+      <c r="AP37" s="94"/>
+      <c r="AQ37" s="94"/>
+      <c r="AR37" s="94"/>
+      <c r="AS37" s="94"/>
+      <c r="AT37" s="94"/>
+      <c r="AU37" s="95"/>
       <c r="AV37" s="20"/>
       <c r="AW37" s="20"/>
       <c r="AX37" s="20"/>
@@ -3019,56 +3036,56 @@
       <c r="C38" s="20"/>
       <c r="D38" s="20"/>
       <c r="E38" s="20"/>
-      <c r="F38" s="73" t="s">
-        <v>26</v>
+      <c r="F38" s="93" t="s">
+        <v>24</v>
       </c>
-      <c r="G38" s="74"/>
-      <c r="H38" s="74"/>
-      <c r="I38" s="76"/>
-      <c r="J38" s="74"/>
-      <c r="K38" s="74"/>
-      <c r="L38" s="74"/>
-      <c r="M38" s="74"/>
-      <c r="N38" s="74"/>
-      <c r="O38" s="74"/>
-      <c r="P38" s="74"/>
-      <c r="Q38" s="74"/>
-      <c r="R38" s="74"/>
-      <c r="S38" s="75"/>
+      <c r="G38" s="94"/>
+      <c r="H38" s="94"/>
+      <c r="I38" s="96"/>
+      <c r="J38" s="94"/>
+      <c r="K38" s="94"/>
+      <c r="L38" s="94"/>
+      <c r="M38" s="94"/>
+      <c r="N38" s="94"/>
+      <c r="O38" s="94"/>
+      <c r="P38" s="94"/>
+      <c r="Q38" s="94"/>
+      <c r="R38" s="94"/>
+      <c r="S38" s="95"/>
       <c r="T38" s="46" t="str">
         <f>F38</f>
         <v xml:space="preserve">Date : </v>
       </c>
-      <c r="U38" s="76"/>
-      <c r="V38" s="74"/>
-      <c r="W38" s="74"/>
-      <c r="X38" s="74"/>
-      <c r="Y38" s="74"/>
-      <c r="Z38" s="74"/>
-      <c r="AA38" s="74"/>
-      <c r="AB38" s="74"/>
-      <c r="AC38" s="74"/>
-      <c r="AD38" s="74"/>
-      <c r="AE38" s="74"/>
-      <c r="AF38" s="74"/>
-      <c r="AG38" s="75"/>
-      <c r="AH38" s="73" t="str">
+      <c r="U38" s="96"/>
+      <c r="V38" s="94"/>
+      <c r="W38" s="94"/>
+      <c r="X38" s="94"/>
+      <c r="Y38" s="94"/>
+      <c r="Z38" s="94"/>
+      <c r="AA38" s="94"/>
+      <c r="AB38" s="94"/>
+      <c r="AC38" s="94"/>
+      <c r="AD38" s="94"/>
+      <c r="AE38" s="94"/>
+      <c r="AF38" s="94"/>
+      <c r="AG38" s="95"/>
+      <c r="AH38" s="93" t="str">
         <f>F38</f>
         <v xml:space="preserve">Date : </v>
       </c>
-      <c r="AI38" s="74"/>
-      <c r="AJ38" s="76"/>
-      <c r="AK38" s="74"/>
-      <c r="AL38" s="74"/>
-      <c r="AM38" s="74"/>
-      <c r="AN38" s="74"/>
-      <c r="AO38" s="74"/>
-      <c r="AP38" s="74"/>
-      <c r="AQ38" s="74"/>
-      <c r="AR38" s="74"/>
-      <c r="AS38" s="74"/>
-      <c r="AT38" s="74"/>
-      <c r="AU38" s="75"/>
+      <c r="AI38" s="94"/>
+      <c r="AJ38" s="96"/>
+      <c r="AK38" s="94"/>
+      <c r="AL38" s="94"/>
+      <c r="AM38" s="94"/>
+      <c r="AN38" s="94"/>
+      <c r="AO38" s="94"/>
+      <c r="AP38" s="94"/>
+      <c r="AQ38" s="94"/>
+      <c r="AR38" s="94"/>
+      <c r="AS38" s="94"/>
+      <c r="AT38" s="94"/>
+      <c r="AU38" s="95"/>
       <c r="AV38" s="16"/>
       <c r="AW38" s="16"/>
       <c r="AX38" s="16"/>
@@ -55988,11 +56005,6 @@
     </row>
   </sheetData>
   <mergeCells count="50">
-    <mergeCell ref="R19:T19"/>
-    <mergeCell ref="R23:T23"/>
-    <mergeCell ref="R26:T26"/>
-    <mergeCell ref="R27:T27"/>
-    <mergeCell ref="R20:T20"/>
     <mergeCell ref="AV17:BA17"/>
     <mergeCell ref="AV18:BA18"/>
     <mergeCell ref="AV19:BA19"/>
@@ -56006,6 +56018,7 @@
     <mergeCell ref="A6:D6"/>
     <mergeCell ref="A7:E7"/>
     <mergeCell ref="A11:D11"/>
+    <mergeCell ref="AA4:AC4"/>
     <mergeCell ref="AH37:AU37"/>
     <mergeCell ref="U38:AG38"/>
     <mergeCell ref="AH38:AI38"/>
@@ -56022,13 +56035,17 @@
     <mergeCell ref="AH34:AU36"/>
     <mergeCell ref="F33:S33"/>
     <mergeCell ref="F34:S36"/>
-    <mergeCell ref="AA4:AC4"/>
     <mergeCell ref="F37:S37"/>
     <mergeCell ref="F38:H38"/>
     <mergeCell ref="I38:S38"/>
     <mergeCell ref="T37:AG37"/>
     <mergeCell ref="B14:Q14"/>
     <mergeCell ref="B18:Q18"/>
+    <mergeCell ref="R19:T19"/>
+    <mergeCell ref="R23:T23"/>
+    <mergeCell ref="R26:T26"/>
+    <mergeCell ref="R27:T27"/>
+    <mergeCell ref="R20:T20"/>
     <mergeCell ref="A12:Q13"/>
     <mergeCell ref="R12:T13"/>
     <mergeCell ref="R14:T14"/>

</xml_diff>

<commit_message>
feat: Add author for checked or approved to export excel IPP
</commit_message>
<xml_diff>
--- a/public/assets/file/Template IPP.xlsx
+++ b/public/assets/file/Template IPP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\core\public\assets\file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4BCD898-0997-413D-A3C4-76C4C8AA5E1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEC0E75B-7789-4809-8885-E39B715AD50D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="31">
   <si>
     <t>PERSONAL &amp; CONFIDENTIAL</t>
   </si>
@@ -129,11 +129,17 @@
   <si>
     <t>Date of review</t>
   </si>
+  <si>
+    <t>Date :</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
+  </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -214,7 +220,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="44">
+  <borders count="51">
     <border>
       <left/>
       <right/>
@@ -697,11 +703,82 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="131">
+  <cellXfs count="143">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -816,9 +893,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
@@ -868,13 +942,93 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="17" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="17" fontId="6" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="17" fontId="6" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="5" fillId="3" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -889,98 +1043,55 @@
     <xf numFmtId="9" fontId="5" fillId="3" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="5" fillId="3" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="17" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="17" fontId="6" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="17" fontId="6" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1275,8 +1386,8 @@
   </sheetPr>
   <dimension ref="A1:BU1000"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AK8" sqref="AK8"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A29" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AU42" sqref="AU42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1290,137 +1401,137 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:73" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="115" t="s">
+      <c r="A1" s="91" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="75"/>
-      <c r="C1" s="75"/>
-      <c r="D1" s="75"/>
-      <c r="E1" s="75"/>
-      <c r="F1" s="75"/>
-      <c r="G1" s="75"/>
-      <c r="H1" s="75"/>
-      <c r="I1" s="75"/>
-      <c r="J1" s="75"/>
-      <c r="K1" s="75"/>
-      <c r="L1" s="75"/>
-      <c r="M1" s="75"/>
-      <c r="N1" s="75"/>
-      <c r="O1" s="75"/>
-      <c r="P1" s="75"/>
-      <c r="Q1" s="75"/>
-      <c r="R1" s="75"/>
-      <c r="S1" s="75"/>
-      <c r="T1" s="75"/>
-      <c r="U1" s="75"/>
-      <c r="V1" s="75"/>
-      <c r="W1" s="75"/>
-      <c r="X1" s="75"/>
-      <c r="Y1" s="75"/>
-      <c r="Z1" s="75"/>
-      <c r="AA1" s="75"/>
-      <c r="AB1" s="75"/>
-      <c r="AC1" s="75"/>
-      <c r="AD1" s="75"/>
-      <c r="AE1" s="75"/>
-      <c r="AF1" s="75"/>
-      <c r="AG1" s="75"/>
-      <c r="AH1" s="75"/>
-      <c r="AI1" s="75"/>
-      <c r="AJ1" s="75"/>
-      <c r="AK1" s="75"/>
-      <c r="AL1" s="75"/>
-      <c r="AM1" s="75"/>
-      <c r="AN1" s="75"/>
-      <c r="AO1" s="75"/>
-      <c r="AP1" s="75"/>
-      <c r="AQ1" s="75"/>
-      <c r="AR1" s="75"/>
-      <c r="AS1" s="75"/>
-      <c r="AT1" s="75"/>
-      <c r="AU1" s="75"/>
-      <c r="AV1" s="75"/>
-      <c r="AW1" s="75"/>
-      <c r="AX1" s="75"/>
-      <c r="AY1" s="75"/>
-      <c r="AZ1" s="75"/>
-      <c r="BA1" s="108"/>
+      <c r="B1" s="83"/>
+      <c r="C1" s="83"/>
+      <c r="D1" s="83"/>
+      <c r="E1" s="83"/>
+      <c r="F1" s="83"/>
+      <c r="G1" s="83"/>
+      <c r="H1" s="83"/>
+      <c r="I1" s="83"/>
+      <c r="J1" s="83"/>
+      <c r="K1" s="83"/>
+      <c r="L1" s="83"/>
+      <c r="M1" s="83"/>
+      <c r="N1" s="83"/>
+      <c r="O1" s="83"/>
+      <c r="P1" s="83"/>
+      <c r="Q1" s="83"/>
+      <c r="R1" s="83"/>
+      <c r="S1" s="83"/>
+      <c r="T1" s="83"/>
+      <c r="U1" s="83"/>
+      <c r="V1" s="83"/>
+      <c r="W1" s="83"/>
+      <c r="X1" s="83"/>
+      <c r="Y1" s="83"/>
+      <c r="Z1" s="83"/>
+      <c r="AA1" s="83"/>
+      <c r="AB1" s="83"/>
+      <c r="AC1" s="83"/>
+      <c r="AD1" s="83"/>
+      <c r="AE1" s="83"/>
+      <c r="AF1" s="83"/>
+      <c r="AG1" s="83"/>
+      <c r="AH1" s="83"/>
+      <c r="AI1" s="83"/>
+      <c r="AJ1" s="83"/>
+      <c r="AK1" s="83"/>
+      <c r="AL1" s="83"/>
+      <c r="AM1" s="83"/>
+      <c r="AN1" s="83"/>
+      <c r="AO1" s="83"/>
+      <c r="AP1" s="83"/>
+      <c r="AQ1" s="83"/>
+      <c r="AR1" s="83"/>
+      <c r="AS1" s="83"/>
+      <c r="AT1" s="83"/>
+      <c r="AU1" s="83"/>
+      <c r="AV1" s="83"/>
+      <c r="AW1" s="83"/>
+      <c r="AX1" s="83"/>
+      <c r="AY1" s="83"/>
+      <c r="AZ1" s="83"/>
+      <c r="BA1" s="84"/>
     </row>
     <row r="2" spans="1:73" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="116" t="s">
+      <c r="A2" s="92" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="86"/>
-      <c r="C2" s="86"/>
-      <c r="D2" s="86"/>
-      <c r="E2" s="86"/>
-      <c r="F2" s="86"/>
-      <c r="G2" s="86"/>
-      <c r="H2" s="86"/>
-      <c r="I2" s="86"/>
-      <c r="J2" s="86"/>
-      <c r="K2" s="86"/>
-      <c r="L2" s="86"/>
-      <c r="M2" s="86"/>
-      <c r="N2" s="86"/>
-      <c r="O2" s="86"/>
-      <c r="P2" s="86"/>
-      <c r="Q2" s="86"/>
-      <c r="R2" s="86"/>
-      <c r="S2" s="86"/>
-      <c r="T2" s="86"/>
-      <c r="U2" s="86"/>
-      <c r="V2" s="86"/>
-      <c r="W2" s="86"/>
-      <c r="X2" s="86"/>
-      <c r="Y2" s="86"/>
-      <c r="Z2" s="86"/>
-      <c r="AA2" s="86"/>
-      <c r="AB2" s="86"/>
-      <c r="AC2" s="86"/>
-      <c r="AD2" s="86"/>
-      <c r="AE2" s="86"/>
-      <c r="AF2" s="86"/>
-      <c r="AG2" s="86"/>
-      <c r="AH2" s="86"/>
-      <c r="AI2" s="86"/>
-      <c r="AJ2" s="86"/>
-      <c r="AK2" s="86"/>
-      <c r="AL2" s="86"/>
-      <c r="AM2" s="86"/>
-      <c r="AN2" s="86"/>
-      <c r="AO2" s="86"/>
-      <c r="AP2" s="86"/>
-      <c r="AQ2" s="86"/>
-      <c r="AR2" s="86"/>
-      <c r="AS2" s="86"/>
-      <c r="AT2" s="86"/>
-      <c r="AU2" s="86"/>
-      <c r="AV2" s="86"/>
-      <c r="AW2" s="86"/>
-      <c r="AX2" s="86"/>
-      <c r="AY2" s="86"/>
-      <c r="AZ2" s="86"/>
-      <c r="BA2" s="102"/>
+      <c r="B2" s="74"/>
+      <c r="C2" s="74"/>
+      <c r="D2" s="74"/>
+      <c r="E2" s="74"/>
+      <c r="F2" s="74"/>
+      <c r="G2" s="74"/>
+      <c r="H2" s="74"/>
+      <c r="I2" s="74"/>
+      <c r="J2" s="74"/>
+      <c r="K2" s="74"/>
+      <c r="L2" s="74"/>
+      <c r="M2" s="74"/>
+      <c r="N2" s="74"/>
+      <c r="O2" s="74"/>
+      <c r="P2" s="74"/>
+      <c r="Q2" s="74"/>
+      <c r="R2" s="74"/>
+      <c r="S2" s="74"/>
+      <c r="T2" s="74"/>
+      <c r="U2" s="74"/>
+      <c r="V2" s="74"/>
+      <c r="W2" s="74"/>
+      <c r="X2" s="74"/>
+      <c r="Y2" s="74"/>
+      <c r="Z2" s="74"/>
+      <c r="AA2" s="74"/>
+      <c r="AB2" s="74"/>
+      <c r="AC2" s="74"/>
+      <c r="AD2" s="74"/>
+      <c r="AE2" s="74"/>
+      <c r="AF2" s="74"/>
+      <c r="AG2" s="74"/>
+      <c r="AH2" s="74"/>
+      <c r="AI2" s="74"/>
+      <c r="AJ2" s="74"/>
+      <c r="AK2" s="74"/>
+      <c r="AL2" s="74"/>
+      <c r="AM2" s="74"/>
+      <c r="AN2" s="74"/>
+      <c r="AO2" s="74"/>
+      <c r="AP2" s="74"/>
+      <c r="AQ2" s="74"/>
+      <c r="AR2" s="74"/>
+      <c r="AS2" s="74"/>
+      <c r="AT2" s="74"/>
+      <c r="AU2" s="74"/>
+      <c r="AV2" s="74"/>
+      <c r="AW2" s="74"/>
+      <c r="AX2" s="74"/>
+      <c r="AY2" s="74"/>
+      <c r="AZ2" s="74"/>
+      <c r="BA2" s="75"/>
     </row>
     <row r="3" spans="1:73" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="V3" s="71" t="s">
+      <c r="V3" s="70" t="s">
         <v>26</v>
       </c>
-      <c r="Y3" s="73" t="s">
+      <c r="Y3" s="72" t="s">
         <v>27</v>
       </c>
-      <c r="BA3" s="72"/>
-      <c r="BU3" s="55"/>
+      <c r="BA3" s="71"/>
+      <c r="BU3" s="54"/>
     </row>
     <row r="4" spans="1:73" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="W4" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="AA4" s="121"/>
-      <c r="AB4" s="121"/>
-      <c r="AC4" s="121"/>
-      <c r="BA4" s="55"/>
+      <c r="AA4" s="98"/>
+      <c r="AB4" s="98"/>
+      <c r="AC4" s="98"/>
+      <c r="BA4" s="54"/>
     </row>
     <row r="5" spans="1:73" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1"/>
@@ -1478,10 +1589,10 @@
       <c r="BA5" s="4"/>
     </row>
     <row r="6" spans="1:73" ht="6" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="117"/>
-      <c r="B6" s="118"/>
-      <c r="C6" s="118"/>
-      <c r="D6" s="118"/>
+      <c r="A6" s="93"/>
+      <c r="B6" s="94"/>
+      <c r="C6" s="94"/>
+      <c r="D6" s="94"/>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
@@ -1533,13 +1644,13 @@
       <c r="BA6" s="6"/>
     </row>
     <row r="7" spans="1:73" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="119" t="s">
+      <c r="A7" s="95" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="86"/>
-      <c r="C7" s="86"/>
-      <c r="D7" s="86"/>
-      <c r="E7" s="86"/>
+      <c r="B7" s="74"/>
+      <c r="C7" s="74"/>
+      <c r="D7" s="74"/>
+      <c r="E7" s="74"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
@@ -1777,10 +1888,10 @@
       <c r="BA10" s="9"/>
     </row>
     <row r="11" spans="1:73" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="120"/>
-      <c r="B11" s="111"/>
-      <c r="C11" s="111"/>
-      <c r="D11" s="111"/>
+      <c r="A11" s="96"/>
+      <c r="B11" s="97"/>
+      <c r="C11" s="97"/>
+      <c r="D11" s="97"/>
       <c r="E11" s="12"/>
       <c r="F11" s="12"/>
       <c r="G11" s="12"/>
@@ -1832,191 +1943,191 @@
       <c r="BA11" s="13"/>
     </row>
     <row r="12" spans="1:73" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="74" t="s">
+      <c r="A12" s="115" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="75"/>
-      <c r="C12" s="75"/>
-      <c r="D12" s="75"/>
-      <c r="E12" s="75"/>
-      <c r="F12" s="75"/>
-      <c r="G12" s="75"/>
-      <c r="H12" s="75"/>
-      <c r="I12" s="75"/>
-      <c r="J12" s="75"/>
-      <c r="K12" s="75"/>
-      <c r="L12" s="75"/>
-      <c r="M12" s="75"/>
-      <c r="N12" s="75"/>
-      <c r="O12" s="75"/>
-      <c r="P12" s="75"/>
-      <c r="Q12" s="76"/>
-      <c r="R12" s="80" t="s">
+      <c r="B12" s="83"/>
+      <c r="C12" s="83"/>
+      <c r="D12" s="83"/>
+      <c r="E12" s="83"/>
+      <c r="F12" s="83"/>
+      <c r="G12" s="83"/>
+      <c r="H12" s="83"/>
+      <c r="I12" s="83"/>
+      <c r="J12" s="83"/>
+      <c r="K12" s="83"/>
+      <c r="L12" s="83"/>
+      <c r="M12" s="83"/>
+      <c r="N12" s="83"/>
+      <c r="O12" s="83"/>
+      <c r="P12" s="83"/>
+      <c r="Q12" s="116"/>
+      <c r="R12" s="119" t="s">
         <v>8</v>
       </c>
-      <c r="S12" s="75"/>
-      <c r="T12" s="76"/>
-      <c r="U12" s="122" t="s">
+      <c r="S12" s="83"/>
+      <c r="T12" s="116"/>
+      <c r="U12" s="79" t="s">
         <v>9</v>
       </c>
-      <c r="V12" s="123"/>
-      <c r="W12" s="123"/>
-      <c r="X12" s="123"/>
-      <c r="Y12" s="123"/>
-      <c r="Z12" s="123"/>
-      <c r="AA12" s="123"/>
-      <c r="AB12" s="123"/>
-      <c r="AC12" s="123"/>
-      <c r="AD12" s="123"/>
-      <c r="AE12" s="123"/>
-      <c r="AF12" s="123"/>
-      <c r="AG12" s="123"/>
-      <c r="AH12" s="123"/>
-      <c r="AI12" s="123"/>
-      <c r="AJ12" s="123"/>
-      <c r="AK12" s="123"/>
-      <c r="AL12" s="123"/>
-      <c r="AM12" s="123"/>
-      <c r="AN12" s="123"/>
-      <c r="AO12" s="123"/>
-      <c r="AP12" s="123"/>
-      <c r="AQ12" s="123"/>
-      <c r="AR12" s="123"/>
-      <c r="AS12" s="123"/>
-      <c r="AT12" s="123"/>
-      <c r="AU12" s="124"/>
-      <c r="AV12" s="125" t="s">
+      <c r="V12" s="80"/>
+      <c r="W12" s="80"/>
+      <c r="X12" s="80"/>
+      <c r="Y12" s="80"/>
+      <c r="Z12" s="80"/>
+      <c r="AA12" s="80"/>
+      <c r="AB12" s="80"/>
+      <c r="AC12" s="80"/>
+      <c r="AD12" s="80"/>
+      <c r="AE12" s="80"/>
+      <c r="AF12" s="80"/>
+      <c r="AG12" s="80"/>
+      <c r="AH12" s="80"/>
+      <c r="AI12" s="80"/>
+      <c r="AJ12" s="80"/>
+      <c r="AK12" s="80"/>
+      <c r="AL12" s="80"/>
+      <c r="AM12" s="80"/>
+      <c r="AN12" s="80"/>
+      <c r="AO12" s="80"/>
+      <c r="AP12" s="80"/>
+      <c r="AQ12" s="80"/>
+      <c r="AR12" s="80"/>
+      <c r="AS12" s="80"/>
+      <c r="AT12" s="80"/>
+      <c r="AU12" s="81"/>
+      <c r="AV12" s="82" t="s">
         <v>10</v>
       </c>
-      <c r="AW12" s="75"/>
-      <c r="AX12" s="75"/>
-      <c r="AY12" s="75"/>
-      <c r="AZ12" s="75"/>
-      <c r="BA12" s="108"/>
+      <c r="AW12" s="83"/>
+      <c r="AX12" s="83"/>
+      <c r="AY12" s="83"/>
+      <c r="AZ12" s="83"/>
+      <c r="BA12" s="84"/>
     </row>
     <row r="13" spans="1:73" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="77"/>
-      <c r="B13" s="78"/>
-      <c r="C13" s="78"/>
-      <c r="D13" s="78"/>
-      <c r="E13" s="78"/>
-      <c r="F13" s="78"/>
-      <c r="G13" s="78"/>
-      <c r="H13" s="78"/>
-      <c r="I13" s="78"/>
-      <c r="J13" s="78"/>
-      <c r="K13" s="78"/>
-      <c r="L13" s="78"/>
-      <c r="M13" s="78"/>
-      <c r="N13" s="78"/>
-      <c r="O13" s="78"/>
-      <c r="P13" s="78"/>
-      <c r="Q13" s="79"/>
-      <c r="R13" s="81"/>
-      <c r="S13" s="78"/>
-      <c r="T13" s="79"/>
-      <c r="U13" s="127" t="s">
+      <c r="A13" s="117"/>
+      <c r="B13" s="85"/>
+      <c r="C13" s="85"/>
+      <c r="D13" s="85"/>
+      <c r="E13" s="85"/>
+      <c r="F13" s="85"/>
+      <c r="G13" s="85"/>
+      <c r="H13" s="85"/>
+      <c r="I13" s="85"/>
+      <c r="J13" s="85"/>
+      <c r="K13" s="85"/>
+      <c r="L13" s="85"/>
+      <c r="M13" s="85"/>
+      <c r="N13" s="85"/>
+      <c r="O13" s="85"/>
+      <c r="P13" s="85"/>
+      <c r="Q13" s="118"/>
+      <c r="R13" s="120"/>
+      <c r="S13" s="85"/>
+      <c r="T13" s="118"/>
+      <c r="U13" s="87" t="s">
         <v>11</v>
       </c>
-      <c r="V13" s="128"/>
-      <c r="W13" s="128"/>
-      <c r="X13" s="128"/>
-      <c r="Y13" s="128"/>
-      <c r="Z13" s="128"/>
-      <c r="AA13" s="128"/>
-      <c r="AB13" s="128"/>
-      <c r="AC13" s="128"/>
-      <c r="AD13" s="128"/>
-      <c r="AE13" s="128"/>
-      <c r="AF13" s="128"/>
-      <c r="AG13" s="128"/>
-      <c r="AH13" s="129"/>
-      <c r="AI13" s="127" t="s">
+      <c r="V13" s="88"/>
+      <c r="W13" s="88"/>
+      <c r="X13" s="88"/>
+      <c r="Y13" s="88"/>
+      <c r="Z13" s="88"/>
+      <c r="AA13" s="88"/>
+      <c r="AB13" s="88"/>
+      <c r="AC13" s="88"/>
+      <c r="AD13" s="88"/>
+      <c r="AE13" s="88"/>
+      <c r="AF13" s="88"/>
+      <c r="AG13" s="88"/>
+      <c r="AH13" s="89"/>
+      <c r="AI13" s="87" t="s">
         <v>12</v>
       </c>
-      <c r="AJ13" s="128"/>
-      <c r="AK13" s="128"/>
-      <c r="AL13" s="128"/>
-      <c r="AM13" s="128"/>
-      <c r="AN13" s="128"/>
-      <c r="AO13" s="128"/>
-      <c r="AP13" s="128"/>
-      <c r="AQ13" s="128"/>
-      <c r="AR13" s="128"/>
-      <c r="AS13" s="128"/>
-      <c r="AT13" s="128"/>
-      <c r="AU13" s="130"/>
-      <c r="AV13" s="78"/>
-      <c r="AW13" s="78"/>
-      <c r="AX13" s="78"/>
-      <c r="AY13" s="78"/>
-      <c r="AZ13" s="78"/>
-      <c r="BA13" s="126"/>
+      <c r="AJ13" s="88"/>
+      <c r="AK13" s="88"/>
+      <c r="AL13" s="88"/>
+      <c r="AM13" s="88"/>
+      <c r="AN13" s="88"/>
+      <c r="AO13" s="88"/>
+      <c r="AP13" s="88"/>
+      <c r="AQ13" s="88"/>
+      <c r="AR13" s="88"/>
+      <c r="AS13" s="88"/>
+      <c r="AT13" s="88"/>
+      <c r="AU13" s="90"/>
+      <c r="AV13" s="85"/>
+      <c r="AW13" s="85"/>
+      <c r="AX13" s="85"/>
+      <c r="AY13" s="85"/>
+      <c r="AZ13" s="85"/>
+      <c r="BA13" s="86"/>
     </row>
     <row r="14" spans="1:73" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="98" t="s">
+      <c r="B14" s="105" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="99"/>
-      <c r="D14" s="99"/>
-      <c r="E14" s="99"/>
-      <c r="F14" s="99"/>
-      <c r="G14" s="99"/>
-      <c r="H14" s="99"/>
-      <c r="I14" s="99"/>
-      <c r="J14" s="99"/>
-      <c r="K14" s="99"/>
-      <c r="L14" s="99"/>
-      <c r="M14" s="99"/>
-      <c r="N14" s="99"/>
-      <c r="O14" s="99"/>
-      <c r="P14" s="99"/>
-      <c r="Q14" s="100"/>
-      <c r="R14" s="82">
+      <c r="C14" s="106"/>
+      <c r="D14" s="106"/>
+      <c r="E14" s="106"/>
+      <c r="F14" s="106"/>
+      <c r="G14" s="106"/>
+      <c r="H14" s="106"/>
+      <c r="I14" s="106"/>
+      <c r="J14" s="106"/>
+      <c r="K14" s="106"/>
+      <c r="L14" s="106"/>
+      <c r="M14" s="106"/>
+      <c r="N14" s="106"/>
+      <c r="O14" s="106"/>
+      <c r="P14" s="106"/>
+      <c r="Q14" s="107"/>
+      <c r="R14" s="121">
         <v>0.7</v>
       </c>
-      <c r="S14" s="83"/>
-      <c r="T14" s="84"/>
-      <c r="U14" s="58"/>
-      <c r="V14" s="59"/>
-      <c r="W14" s="59"/>
-      <c r="X14" s="59"/>
-      <c r="Y14" s="59"/>
-      <c r="Z14" s="59"/>
-      <c r="AA14" s="59"/>
-      <c r="AB14" s="59"/>
-      <c r="AC14" s="59"/>
-      <c r="AD14" s="59"/>
-      <c r="AE14" s="59"/>
-      <c r="AF14" s="59"/>
-      <c r="AG14" s="59"/>
-      <c r="AH14" s="60"/>
-      <c r="AI14" s="58"/>
-      <c r="AJ14" s="59"/>
-      <c r="AK14" s="59"/>
-      <c r="AL14" s="59"/>
-      <c r="AM14" s="59"/>
-      <c r="AN14" s="59"/>
-      <c r="AO14" s="59"/>
-      <c r="AP14" s="59"/>
-      <c r="AQ14" s="59"/>
-      <c r="AR14" s="59"/>
-      <c r="AS14" s="59"/>
-      <c r="AT14" s="59"/>
-      <c r="AU14" s="61"/>
-      <c r="AV14" s="62"/>
-      <c r="AW14" s="63"/>
-      <c r="AX14" s="63"/>
-      <c r="AY14" s="63"/>
-      <c r="AZ14" s="63"/>
-      <c r="BA14" s="64"/>
+      <c r="S14" s="122"/>
+      <c r="T14" s="123"/>
+      <c r="U14" s="57"/>
+      <c r="V14" s="58"/>
+      <c r="W14" s="58"/>
+      <c r="X14" s="58"/>
+      <c r="Y14" s="58"/>
+      <c r="Z14" s="58"/>
+      <c r="AA14" s="58"/>
+      <c r="AB14" s="58"/>
+      <c r="AC14" s="58"/>
+      <c r="AD14" s="58"/>
+      <c r="AE14" s="58"/>
+      <c r="AF14" s="58"/>
+      <c r="AG14" s="58"/>
+      <c r="AH14" s="59"/>
+      <c r="AI14" s="57"/>
+      <c r="AJ14" s="58"/>
+      <c r="AK14" s="58"/>
+      <c r="AL14" s="58"/>
+      <c r="AM14" s="58"/>
+      <c r="AN14" s="58"/>
+      <c r="AO14" s="58"/>
+      <c r="AP14" s="58"/>
+      <c r="AQ14" s="58"/>
+      <c r="AR14" s="58"/>
+      <c r="AS14" s="58"/>
+      <c r="AT14" s="58"/>
+      <c r="AU14" s="60"/>
+      <c r="AV14" s="61"/>
+      <c r="AW14" s="62"/>
+      <c r="AX14" s="62"/>
+      <c r="AY14" s="62"/>
+      <c r="AZ14" s="62"/>
+      <c r="BA14" s="63"/>
     </row>
     <row r="15" spans="1:73" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="15"/>
-      <c r="B15" s="50"/>
+      <c r="B15" s="49"/>
       <c r="C15" s="45"/>
       <c r="D15" s="20"/>
       <c r="E15" s="20"/>
@@ -2035,10 +2146,10 @@
       <c r="R15" s="17"/>
       <c r="S15" s="18"/>
       <c r="T15" s="19"/>
-      <c r="U15" s="49"/>
-      <c r="AH15" s="47"/>
-      <c r="AI15" s="49"/>
-      <c r="AU15" s="56"/>
+      <c r="U15" s="48"/>
+      <c r="AH15" s="46"/>
+      <c r="AI15" s="48"/>
+      <c r="AU15" s="55"/>
       <c r="AV15" s="20"/>
       <c r="AW15" s="20"/>
       <c r="AX15" s="20"/>
@@ -2064,19 +2175,19 @@
       <c r="O16" s="45"/>
       <c r="P16" s="45"/>
       <c r="Q16" s="45"/>
-      <c r="R16" s="85"/>
-      <c r="S16" s="86"/>
-      <c r="T16" s="87"/>
-      <c r="U16" s="49"/>
-      <c r="AH16" s="47"/>
-      <c r="AI16" s="49"/>
-      <c r="AU16" s="56"/>
-      <c r="AV16" s="101"/>
-      <c r="AW16" s="86"/>
-      <c r="AX16" s="86"/>
-      <c r="AY16" s="86"/>
-      <c r="AZ16" s="86"/>
-      <c r="BA16" s="102"/>
+      <c r="R16" s="111"/>
+      <c r="S16" s="74"/>
+      <c r="T16" s="112"/>
+      <c r="U16" s="48"/>
+      <c r="AH16" s="46"/>
+      <c r="AI16" s="48"/>
+      <c r="AU16" s="55"/>
+      <c r="AV16" s="73"/>
+      <c r="AW16" s="74"/>
+      <c r="AX16" s="74"/>
+      <c r="AY16" s="74"/>
+      <c r="AZ16" s="74"/>
+      <c r="BA16" s="75"/>
     </row>
     <row r="17" spans="1:53" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="15"/>
@@ -2096,80 +2207,80 @@
       <c r="O17" s="45"/>
       <c r="P17" s="45"/>
       <c r="Q17" s="45"/>
-      <c r="R17" s="85"/>
-      <c r="S17" s="86"/>
-      <c r="T17" s="87"/>
-      <c r="U17" s="49"/>
-      <c r="AH17" s="47"/>
-      <c r="AI17" s="49"/>
-      <c r="AU17" s="56"/>
-      <c r="AV17" s="101"/>
-      <c r="AW17" s="86"/>
-      <c r="AX17" s="86"/>
-      <c r="AY17" s="86"/>
-      <c r="AZ17" s="86"/>
-      <c r="BA17" s="102"/>
+      <c r="R17" s="111"/>
+      <c r="S17" s="74"/>
+      <c r="T17" s="112"/>
+      <c r="U17" s="48"/>
+      <c r="AH17" s="46"/>
+      <c r="AI17" s="48"/>
+      <c r="AU17" s="55"/>
+      <c r="AV17" s="73"/>
+      <c r="AW17" s="74"/>
+      <c r="AX17" s="74"/>
+      <c r="AY17" s="74"/>
+      <c r="AZ17" s="74"/>
+      <c r="BA17" s="75"/>
     </row>
     <row r="18" spans="1:53" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="88" t="s">
+      <c r="B18" s="108" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="89"/>
-      <c r="D18" s="89"/>
-      <c r="E18" s="89"/>
-      <c r="F18" s="89"/>
-      <c r="G18" s="89"/>
-      <c r="H18" s="89"/>
-      <c r="I18" s="89"/>
-      <c r="J18" s="89"/>
-      <c r="K18" s="89"/>
-      <c r="L18" s="89"/>
-      <c r="M18" s="89"/>
-      <c r="N18" s="89"/>
-      <c r="O18" s="89"/>
-      <c r="P18" s="89"/>
-      <c r="Q18" s="90"/>
-      <c r="R18" s="91">
+      <c r="C18" s="109"/>
+      <c r="D18" s="109"/>
+      <c r="E18" s="109"/>
+      <c r="F18" s="109"/>
+      <c r="G18" s="109"/>
+      <c r="H18" s="109"/>
+      <c r="I18" s="109"/>
+      <c r="J18" s="109"/>
+      <c r="K18" s="109"/>
+      <c r="L18" s="109"/>
+      <c r="M18" s="109"/>
+      <c r="N18" s="109"/>
+      <c r="O18" s="109"/>
+      <c r="P18" s="109"/>
+      <c r="Q18" s="110"/>
+      <c r="R18" s="113">
         <v>0.1</v>
       </c>
-      <c r="S18" s="92"/>
-      <c r="T18" s="87"/>
-      <c r="U18" s="65"/>
-      <c r="V18" s="66"/>
-      <c r="W18" s="66"/>
-      <c r="X18" s="66"/>
-      <c r="Y18" s="66"/>
-      <c r="Z18" s="66"/>
-      <c r="AA18" s="66"/>
-      <c r="AB18" s="66"/>
-      <c r="AC18" s="66"/>
-      <c r="AD18" s="66"/>
-      <c r="AE18" s="66"/>
-      <c r="AF18" s="66"/>
-      <c r="AG18" s="66"/>
-      <c r="AH18" s="67"/>
-      <c r="AI18" s="65"/>
-      <c r="AJ18" s="66"/>
-      <c r="AK18" s="66"/>
-      <c r="AL18" s="66"/>
-      <c r="AM18" s="66"/>
-      <c r="AN18" s="66"/>
-      <c r="AO18" s="66"/>
-      <c r="AP18" s="66"/>
-      <c r="AQ18" s="66"/>
-      <c r="AR18" s="66"/>
-      <c r="AS18" s="66"/>
-      <c r="AT18" s="66"/>
-      <c r="AU18" s="68"/>
-      <c r="AV18" s="103"/>
-      <c r="AW18" s="104"/>
-      <c r="AX18" s="104"/>
-      <c r="AY18" s="104"/>
-      <c r="AZ18" s="104"/>
-      <c r="BA18" s="105"/>
+      <c r="S18" s="114"/>
+      <c r="T18" s="112"/>
+      <c r="U18" s="64"/>
+      <c r="V18" s="65"/>
+      <c r="W18" s="65"/>
+      <c r="X18" s="65"/>
+      <c r="Y18" s="65"/>
+      <c r="Z18" s="65"/>
+      <c r="AA18" s="65"/>
+      <c r="AB18" s="65"/>
+      <c r="AC18" s="65"/>
+      <c r="AD18" s="65"/>
+      <c r="AE18" s="65"/>
+      <c r="AF18" s="65"/>
+      <c r="AG18" s="65"/>
+      <c r="AH18" s="66"/>
+      <c r="AI18" s="64"/>
+      <c r="AJ18" s="65"/>
+      <c r="AK18" s="65"/>
+      <c r="AL18" s="65"/>
+      <c r="AM18" s="65"/>
+      <c r="AN18" s="65"/>
+      <c r="AO18" s="65"/>
+      <c r="AP18" s="65"/>
+      <c r="AQ18" s="65"/>
+      <c r="AR18" s="65"/>
+      <c r="AS18" s="65"/>
+      <c r="AT18" s="65"/>
+      <c r="AU18" s="67"/>
+      <c r="AV18" s="76"/>
+      <c r="AW18" s="77"/>
+      <c r="AX18" s="77"/>
+      <c r="AY18" s="77"/>
+      <c r="AZ18" s="77"/>
+      <c r="BA18" s="78"/>
     </row>
     <row r="19" spans="1:53" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="15"/>
@@ -2189,19 +2300,19 @@
       <c r="O19" s="45"/>
       <c r="P19" s="45"/>
       <c r="Q19" s="45"/>
-      <c r="R19" s="85"/>
-      <c r="S19" s="86"/>
-      <c r="T19" s="87"/>
-      <c r="U19" s="49"/>
-      <c r="AH19" s="47"/>
-      <c r="AI19" s="49"/>
-      <c r="AU19" s="56"/>
-      <c r="AV19" s="101"/>
-      <c r="AW19" s="86"/>
-      <c r="AX19" s="86"/>
-      <c r="AY19" s="86"/>
-      <c r="AZ19" s="86"/>
-      <c r="BA19" s="102"/>
+      <c r="R19" s="111"/>
+      <c r="S19" s="74"/>
+      <c r="T19" s="112"/>
+      <c r="U19" s="48"/>
+      <c r="AH19" s="46"/>
+      <c r="AI19" s="48"/>
+      <c r="AU19" s="55"/>
+      <c r="AV19" s="73"/>
+      <c r="AW19" s="74"/>
+      <c r="AX19" s="74"/>
+      <c r="AY19" s="74"/>
+      <c r="AZ19" s="74"/>
+      <c r="BA19" s="75"/>
     </row>
     <row r="20" spans="1:53" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="15"/>
@@ -2221,19 +2332,19 @@
       <c r="O20" s="45"/>
       <c r="P20" s="45"/>
       <c r="Q20" s="45"/>
-      <c r="R20" s="85"/>
-      <c r="S20" s="86"/>
-      <c r="T20" s="87"/>
-      <c r="U20" s="49"/>
-      <c r="AH20" s="47"/>
-      <c r="AI20" s="49"/>
-      <c r="AU20" s="56"/>
-      <c r="AV20" s="101"/>
-      <c r="AW20" s="86"/>
-      <c r="AX20" s="86"/>
-      <c r="AY20" s="86"/>
-      <c r="AZ20" s="86"/>
-      <c r="BA20" s="102"/>
+      <c r="R20" s="111"/>
+      <c r="S20" s="74"/>
+      <c r="T20" s="112"/>
+      <c r="U20" s="48"/>
+      <c r="AH20" s="46"/>
+      <c r="AI20" s="48"/>
+      <c r="AU20" s="55"/>
+      <c r="AV20" s="73"/>
+      <c r="AW20" s="74"/>
+      <c r="AX20" s="74"/>
+      <c r="AY20" s="74"/>
+      <c r="AZ20" s="74"/>
+      <c r="BA20" s="75"/>
     </row>
     <row r="21" spans="1:53" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="15"/>
@@ -2256,10 +2367,10 @@
       <c r="R21" s="17"/>
       <c r="S21" s="23"/>
       <c r="T21" s="24"/>
-      <c r="U21" s="49"/>
-      <c r="AH21" s="47"/>
-      <c r="AI21" s="49"/>
-      <c r="AU21" s="56"/>
+      <c r="U21" s="48"/>
+      <c r="AH21" s="46"/>
+      <c r="AI21" s="48"/>
+      <c r="AU21" s="55"/>
       <c r="AV21" s="25"/>
       <c r="AW21" s="18"/>
       <c r="AX21" s="18"/>
@@ -2288,10 +2399,10 @@
       <c r="R22" s="17"/>
       <c r="S22" s="23"/>
       <c r="T22" s="24"/>
-      <c r="U22" s="49"/>
-      <c r="AH22" s="47"/>
-      <c r="AI22" s="49"/>
-      <c r="AU22" s="56"/>
+      <c r="U22" s="48"/>
+      <c r="AH22" s="46"/>
+      <c r="AI22" s="48"/>
+      <c r="AU22" s="55"/>
       <c r="AV22" s="25"/>
       <c r="AW22" s="18"/>
       <c r="AX22" s="18"/>
@@ -2303,62 +2414,62 @@
       <c r="A23" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="B23" s="88" t="s">
+      <c r="B23" s="108" t="s">
         <v>18</v>
       </c>
-      <c r="C23" s="89"/>
-      <c r="D23" s="89"/>
-      <c r="E23" s="89"/>
-      <c r="F23" s="89"/>
-      <c r="G23" s="89"/>
-      <c r="H23" s="89"/>
-      <c r="I23" s="89"/>
-      <c r="J23" s="89"/>
-      <c r="K23" s="89"/>
-      <c r="L23" s="89"/>
-      <c r="M23" s="89"/>
-      <c r="N23" s="89"/>
-      <c r="O23" s="89"/>
-      <c r="P23" s="89"/>
-      <c r="Q23" s="90"/>
-      <c r="R23" s="91">
+      <c r="C23" s="109"/>
+      <c r="D23" s="109"/>
+      <c r="E23" s="109"/>
+      <c r="F23" s="109"/>
+      <c r="G23" s="109"/>
+      <c r="H23" s="109"/>
+      <c r="I23" s="109"/>
+      <c r="J23" s="109"/>
+      <c r="K23" s="109"/>
+      <c r="L23" s="109"/>
+      <c r="M23" s="109"/>
+      <c r="N23" s="109"/>
+      <c r="O23" s="109"/>
+      <c r="P23" s="109"/>
+      <c r="Q23" s="110"/>
+      <c r="R23" s="113">
         <v>0.1</v>
       </c>
-      <c r="S23" s="92"/>
-      <c r="T23" s="87"/>
-      <c r="U23" s="65"/>
-      <c r="V23" s="66"/>
-      <c r="W23" s="66"/>
-      <c r="X23" s="66"/>
-      <c r="Y23" s="66"/>
-      <c r="Z23" s="66"/>
-      <c r="AA23" s="66"/>
-      <c r="AB23" s="66"/>
-      <c r="AC23" s="66"/>
-      <c r="AD23" s="66"/>
-      <c r="AE23" s="66"/>
-      <c r="AF23" s="66"/>
-      <c r="AG23" s="66"/>
-      <c r="AH23" s="67"/>
-      <c r="AI23" s="65"/>
-      <c r="AJ23" s="66"/>
-      <c r="AK23" s="66"/>
-      <c r="AL23" s="66"/>
-      <c r="AM23" s="66"/>
-      <c r="AN23" s="66"/>
-      <c r="AO23" s="66"/>
-      <c r="AP23" s="66"/>
-      <c r="AQ23" s="66"/>
-      <c r="AR23" s="66"/>
-      <c r="AS23" s="66"/>
-      <c r="AT23" s="66"/>
-      <c r="AU23" s="68"/>
-      <c r="AV23" s="103"/>
-      <c r="AW23" s="104"/>
-      <c r="AX23" s="104"/>
-      <c r="AY23" s="104"/>
-      <c r="AZ23" s="104"/>
-      <c r="BA23" s="105"/>
+      <c r="S23" s="114"/>
+      <c r="T23" s="112"/>
+      <c r="U23" s="64"/>
+      <c r="V23" s="65"/>
+      <c r="W23" s="65"/>
+      <c r="X23" s="65"/>
+      <c r="Y23" s="65"/>
+      <c r="Z23" s="65"/>
+      <c r="AA23" s="65"/>
+      <c r="AB23" s="65"/>
+      <c r="AC23" s="65"/>
+      <c r="AD23" s="65"/>
+      <c r="AE23" s="65"/>
+      <c r="AF23" s="65"/>
+      <c r="AG23" s="65"/>
+      <c r="AH23" s="66"/>
+      <c r="AI23" s="64"/>
+      <c r="AJ23" s="65"/>
+      <c r="AK23" s="65"/>
+      <c r="AL23" s="65"/>
+      <c r="AM23" s="65"/>
+      <c r="AN23" s="65"/>
+      <c r="AO23" s="65"/>
+      <c r="AP23" s="65"/>
+      <c r="AQ23" s="65"/>
+      <c r="AR23" s="65"/>
+      <c r="AS23" s="65"/>
+      <c r="AT23" s="65"/>
+      <c r="AU23" s="67"/>
+      <c r="AV23" s="76"/>
+      <c r="AW23" s="77"/>
+      <c r="AX23" s="77"/>
+      <c r="AY23" s="77"/>
+      <c r="AZ23" s="77"/>
+      <c r="BA23" s="78"/>
     </row>
     <row r="24" spans="1:53" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="15"/>
@@ -2377,14 +2488,14 @@
       <c r="N24" s="20"/>
       <c r="O24" s="20"/>
       <c r="P24" s="20"/>
-      <c r="Q24" s="53"/>
+      <c r="Q24" s="52"/>
       <c r="R24" s="17"/>
       <c r="S24" s="18"/>
       <c r="T24" s="19"/>
-      <c r="U24" s="49"/>
-      <c r="AH24" s="47"/>
-      <c r="AI24" s="49"/>
-      <c r="AU24" s="56"/>
+      <c r="U24" s="48"/>
+      <c r="AH24" s="46"/>
+      <c r="AI24" s="48"/>
+      <c r="AU24" s="55"/>
       <c r="AV24" s="27"/>
       <c r="AW24" s="20"/>
       <c r="AX24" s="20"/>
@@ -2409,14 +2520,14 @@
       <c r="N25" s="20"/>
       <c r="O25" s="20"/>
       <c r="P25" s="20"/>
-      <c r="Q25" s="53"/>
+      <c r="Q25" s="52"/>
       <c r="R25" s="17"/>
       <c r="S25" s="18"/>
       <c r="T25" s="19"/>
-      <c r="U25" s="49"/>
-      <c r="AH25" s="47"/>
-      <c r="AI25" s="49"/>
-      <c r="AU25" s="56"/>
+      <c r="U25" s="48"/>
+      <c r="AH25" s="46"/>
+      <c r="AI25" s="48"/>
+      <c r="AU25" s="55"/>
       <c r="AV25" s="27"/>
       <c r="AW25" s="27"/>
       <c r="AX25" s="20"/>
@@ -2441,85 +2552,85 @@
       <c r="N26" s="20"/>
       <c r="O26" s="20"/>
       <c r="P26" s="20"/>
-      <c r="Q26" s="53"/>
-      <c r="R26" s="85"/>
-      <c r="S26" s="86"/>
-      <c r="T26" s="87"/>
-      <c r="U26" s="49"/>
-      <c r="AH26" s="47"/>
-      <c r="AI26" s="49"/>
-      <c r="AU26" s="56"/>
-      <c r="AV26" s="101"/>
-      <c r="AW26" s="86"/>
-      <c r="AX26" s="86"/>
-      <c r="AY26" s="86"/>
-      <c r="AZ26" s="86"/>
-      <c r="BA26" s="102"/>
+      <c r="Q26" s="52"/>
+      <c r="R26" s="111"/>
+      <c r="S26" s="74"/>
+      <c r="T26" s="112"/>
+      <c r="U26" s="48"/>
+      <c r="AH26" s="46"/>
+      <c r="AI26" s="48"/>
+      <c r="AU26" s="55"/>
+      <c r="AV26" s="73"/>
+      <c r="AW26" s="74"/>
+      <c r="AX26" s="74"/>
+      <c r="AY26" s="74"/>
+      <c r="AZ26" s="74"/>
+      <c r="BA26" s="75"/>
     </row>
     <row r="27" spans="1:53" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="B27" s="88" t="s">
+      <c r="B27" s="108" t="s">
         <v>20</v>
       </c>
-      <c r="C27" s="89"/>
-      <c r="D27" s="89"/>
-      <c r="E27" s="89"/>
-      <c r="F27" s="89"/>
-      <c r="G27" s="89"/>
-      <c r="H27" s="89"/>
-      <c r="I27" s="89"/>
-      <c r="J27" s="89"/>
-      <c r="K27" s="89"/>
-      <c r="L27" s="89"/>
-      <c r="M27" s="89"/>
-      <c r="N27" s="89"/>
-      <c r="O27" s="89"/>
-      <c r="P27" s="89"/>
-      <c r="Q27" s="90"/>
-      <c r="R27" s="91">
+      <c r="C27" s="109"/>
+      <c r="D27" s="109"/>
+      <c r="E27" s="109"/>
+      <c r="F27" s="109"/>
+      <c r="G27" s="109"/>
+      <c r="H27" s="109"/>
+      <c r="I27" s="109"/>
+      <c r="J27" s="109"/>
+      <c r="K27" s="109"/>
+      <c r="L27" s="109"/>
+      <c r="M27" s="109"/>
+      <c r="N27" s="109"/>
+      <c r="O27" s="109"/>
+      <c r="P27" s="109"/>
+      <c r="Q27" s="110"/>
+      <c r="R27" s="113">
         <v>0.1</v>
       </c>
-      <c r="S27" s="92"/>
-      <c r="T27" s="87"/>
-      <c r="U27" s="65"/>
-      <c r="V27" s="66"/>
-      <c r="W27" s="66"/>
-      <c r="X27" s="66"/>
-      <c r="Y27" s="66"/>
-      <c r="Z27" s="66"/>
-      <c r="AA27" s="66"/>
-      <c r="AB27" s="66"/>
-      <c r="AC27" s="66"/>
-      <c r="AD27" s="66"/>
-      <c r="AE27" s="66"/>
-      <c r="AF27" s="66"/>
-      <c r="AG27" s="66"/>
-      <c r="AH27" s="67"/>
-      <c r="AI27" s="65"/>
-      <c r="AJ27" s="66"/>
-      <c r="AK27" s="66"/>
-      <c r="AL27" s="66"/>
-      <c r="AM27" s="66"/>
-      <c r="AN27" s="66"/>
-      <c r="AO27" s="66"/>
-      <c r="AP27" s="66"/>
-      <c r="AQ27" s="66"/>
-      <c r="AR27" s="66"/>
-      <c r="AS27" s="66"/>
-      <c r="AT27" s="66"/>
-      <c r="AU27" s="68"/>
-      <c r="AV27" s="69"/>
-      <c r="AW27" s="69"/>
-      <c r="AX27" s="69"/>
-      <c r="AY27" s="69"/>
-      <c r="AZ27" s="69"/>
-      <c r="BA27" s="70"/>
+      <c r="S27" s="114"/>
+      <c r="T27" s="112"/>
+      <c r="U27" s="64"/>
+      <c r="V27" s="65"/>
+      <c r="W27" s="65"/>
+      <c r="X27" s="65"/>
+      <c r="Y27" s="65"/>
+      <c r="Z27" s="65"/>
+      <c r="AA27" s="65"/>
+      <c r="AB27" s="65"/>
+      <c r="AC27" s="65"/>
+      <c r="AD27" s="65"/>
+      <c r="AE27" s="65"/>
+      <c r="AF27" s="65"/>
+      <c r="AG27" s="65"/>
+      <c r="AH27" s="66"/>
+      <c r="AI27" s="64"/>
+      <c r="AJ27" s="65"/>
+      <c r="AK27" s="65"/>
+      <c r="AL27" s="65"/>
+      <c r="AM27" s="65"/>
+      <c r="AN27" s="65"/>
+      <c r="AO27" s="65"/>
+      <c r="AP27" s="65"/>
+      <c r="AQ27" s="65"/>
+      <c r="AR27" s="65"/>
+      <c r="AS27" s="65"/>
+      <c r="AT27" s="65"/>
+      <c r="AU27" s="67"/>
+      <c r="AV27" s="68"/>
+      <c r="AW27" s="68"/>
+      <c r="AX27" s="68"/>
+      <c r="AY27" s="68"/>
+      <c r="AZ27" s="68"/>
+      <c r="BA27" s="69"/>
     </row>
     <row r="28" spans="1:53" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="15"/>
-      <c r="B28" s="50"/>
+      <c r="B28" s="49"/>
       <c r="C28" s="20"/>
       <c r="D28" s="20"/>
       <c r="E28" s="20"/>
@@ -2534,14 +2645,14 @@
       <c r="N28" s="20"/>
       <c r="O28" s="20"/>
       <c r="P28" s="20"/>
-      <c r="Q28" s="53"/>
+      <c r="Q28" s="52"/>
       <c r="R28" s="17"/>
       <c r="S28" s="18"/>
       <c r="T28" s="19"/>
-      <c r="U28" s="49"/>
-      <c r="AH28" s="47"/>
-      <c r="AI28" s="49"/>
-      <c r="AU28" s="56"/>
+      <c r="U28" s="48"/>
+      <c r="AH28" s="46"/>
+      <c r="AI28" s="48"/>
+      <c r="AU28" s="55"/>
       <c r="AV28" s="28"/>
       <c r="AW28" s="27"/>
       <c r="AX28" s="20"/>
@@ -2566,20 +2677,20 @@
       <c r="N29" s="20"/>
       <c r="O29" s="20"/>
       <c r="P29" s="20"/>
-      <c r="Q29" s="53"/>
-      <c r="R29" s="85"/>
-      <c r="S29" s="86"/>
-      <c r="T29" s="87"/>
-      <c r="U29" s="49"/>
-      <c r="AH29" s="47"/>
-      <c r="AI29" s="49"/>
-      <c r="AU29" s="56"/>
-      <c r="AV29" s="101"/>
-      <c r="AW29" s="86"/>
-      <c r="AX29" s="86"/>
-      <c r="AY29" s="86"/>
-      <c r="AZ29" s="86"/>
-      <c r="BA29" s="102"/>
+      <c r="Q29" s="52"/>
+      <c r="R29" s="111"/>
+      <c r="S29" s="74"/>
+      <c r="T29" s="112"/>
+      <c r="U29" s="48"/>
+      <c r="AH29" s="46"/>
+      <c r="AI29" s="48"/>
+      <c r="AU29" s="55"/>
+      <c r="AV29" s="73"/>
+      <c r="AW29" s="74"/>
+      <c r="AX29" s="74"/>
+      <c r="AY29" s="74"/>
+      <c r="AZ29" s="74"/>
+      <c r="BA29" s="75"/>
     </row>
     <row r="30" spans="1:53" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="29"/>
@@ -2598,37 +2709,37 @@
       <c r="N30" s="36"/>
       <c r="O30" s="36"/>
       <c r="P30" s="36"/>
-      <c r="Q30" s="54"/>
+      <c r="Q30" s="53"/>
       <c r="R30" s="32"/>
       <c r="S30" s="33"/>
       <c r="T30" s="34"/>
-      <c r="U30" s="51"/>
-      <c r="V30" s="48"/>
-      <c r="W30" s="48"/>
-      <c r="X30" s="48"/>
-      <c r="Y30" s="48"/>
-      <c r="Z30" s="48"/>
-      <c r="AA30" s="48"/>
-      <c r="AB30" s="48"/>
-      <c r="AC30" s="48"/>
-      <c r="AD30" s="48"/>
-      <c r="AE30" s="48"/>
-      <c r="AF30" s="48"/>
-      <c r="AG30" s="48"/>
-      <c r="AH30" s="52"/>
-      <c r="AI30" s="51"/>
-      <c r="AJ30" s="48"/>
-      <c r="AK30" s="48"/>
-      <c r="AL30" s="48"/>
-      <c r="AM30" s="48"/>
-      <c r="AN30" s="48"/>
-      <c r="AO30" s="48"/>
-      <c r="AP30" s="48"/>
-      <c r="AQ30" s="48"/>
-      <c r="AR30" s="48"/>
-      <c r="AS30" s="48"/>
-      <c r="AT30" s="48"/>
-      <c r="AU30" s="57"/>
+      <c r="U30" s="50"/>
+      <c r="V30" s="47"/>
+      <c r="W30" s="47"/>
+      <c r="X30" s="47"/>
+      <c r="Y30" s="47"/>
+      <c r="Z30" s="47"/>
+      <c r="AA30" s="47"/>
+      <c r="AB30" s="47"/>
+      <c r="AC30" s="47"/>
+      <c r="AD30" s="47"/>
+      <c r="AE30" s="47"/>
+      <c r="AF30" s="47"/>
+      <c r="AG30" s="47"/>
+      <c r="AH30" s="51"/>
+      <c r="AI30" s="50"/>
+      <c r="AJ30" s="47"/>
+      <c r="AK30" s="47"/>
+      <c r="AL30" s="47"/>
+      <c r="AM30" s="47"/>
+      <c r="AN30" s="47"/>
+      <c r="AO30" s="47"/>
+      <c r="AP30" s="47"/>
+      <c r="AQ30" s="47"/>
+      <c r="AR30" s="47"/>
+      <c r="AS30" s="47"/>
+      <c r="AT30" s="47"/>
+      <c r="AU30" s="56"/>
       <c r="AV30" s="30"/>
       <c r="AW30" s="35"/>
       <c r="AX30" s="36"/>
@@ -2654,12 +2765,12 @@
       <c r="O31" s="30"/>
       <c r="P31" s="30"/>
       <c r="Q31" s="31"/>
-      <c r="R31" s="113">
+      <c r="R31" s="103">
         <f>+R14+R18+R23+R27</f>
         <v>0.99999999999999989</v>
       </c>
-      <c r="S31" s="94"/>
-      <c r="T31" s="114"/>
+      <c r="S31" s="100"/>
+      <c r="T31" s="104"/>
       <c r="U31" s="38"/>
       <c r="V31" s="36"/>
       <c r="W31" s="36"/>
@@ -2687,12 +2798,12 @@
       <c r="AS31" s="30"/>
       <c r="AT31" s="30"/>
       <c r="AU31" s="39"/>
-      <c r="AV31" s="106"/>
-      <c r="AW31" s="94"/>
-      <c r="AX31" s="94"/>
-      <c r="AY31" s="94"/>
-      <c r="AZ31" s="94"/>
-      <c r="BA31" s="95"/>
+      <c r="AV31" s="102"/>
+      <c r="AW31" s="100"/>
+      <c r="AX31" s="100"/>
+      <c r="AY31" s="100"/>
+      <c r="AZ31" s="100"/>
+      <c r="BA31" s="101"/>
     </row>
     <row r="32" spans="1:53" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A32" s="40"/>
@@ -2755,54 +2866,54 @@
       <c r="C33" s="45"/>
       <c r="D33" s="45"/>
       <c r="E33" s="45"/>
-      <c r="F33" s="97" t="s">
+      <c r="F33" s="124" t="s">
         <v>21</v>
       </c>
-      <c r="G33" s="94"/>
-      <c r="H33" s="94"/>
-      <c r="I33" s="94"/>
-      <c r="J33" s="94"/>
-      <c r="K33" s="94"/>
-      <c r="L33" s="94"/>
-      <c r="M33" s="94"/>
-      <c r="N33" s="94"/>
-      <c r="O33" s="94"/>
-      <c r="P33" s="94"/>
-      <c r="Q33" s="94"/>
-      <c r="R33" s="94"/>
-      <c r="S33" s="95"/>
-      <c r="T33" s="97" t="s">
+      <c r="G33" s="83"/>
+      <c r="H33" s="83"/>
+      <c r="I33" s="83"/>
+      <c r="J33" s="83"/>
+      <c r="K33" s="83"/>
+      <c r="L33" s="83"/>
+      <c r="M33" s="83"/>
+      <c r="N33" s="83"/>
+      <c r="O33" s="83"/>
+      <c r="P33" s="83"/>
+      <c r="Q33" s="83"/>
+      <c r="R33" s="83"/>
+      <c r="S33" s="84"/>
+      <c r="T33" s="124" t="s">
         <v>22</v>
       </c>
-      <c r="U33" s="94"/>
-      <c r="V33" s="94"/>
-      <c r="W33" s="94"/>
-      <c r="X33" s="94"/>
-      <c r="Y33" s="94"/>
-      <c r="Z33" s="94"/>
-      <c r="AA33" s="94"/>
-      <c r="AB33" s="94"/>
-      <c r="AC33" s="94"/>
-      <c r="AD33" s="94"/>
-      <c r="AE33" s="94"/>
-      <c r="AF33" s="94"/>
-      <c r="AG33" s="95"/>
-      <c r="AH33" s="97" t="s">
+      <c r="U33" s="83"/>
+      <c r="V33" s="83"/>
+      <c r="W33" s="83"/>
+      <c r="X33" s="83"/>
+      <c r="Y33" s="83"/>
+      <c r="Z33" s="83"/>
+      <c r="AA33" s="83"/>
+      <c r="AB33" s="83"/>
+      <c r="AC33" s="83"/>
+      <c r="AD33" s="83"/>
+      <c r="AE33" s="83"/>
+      <c r="AF33" s="83"/>
+      <c r="AG33" s="84"/>
+      <c r="AH33" s="124" t="s">
         <v>23</v>
       </c>
-      <c r="AI33" s="94"/>
-      <c r="AJ33" s="94"/>
-      <c r="AK33" s="94"/>
-      <c r="AL33" s="94"/>
-      <c r="AM33" s="94"/>
-      <c r="AN33" s="94"/>
-      <c r="AO33" s="94"/>
-      <c r="AP33" s="94"/>
-      <c r="AQ33" s="94"/>
-      <c r="AR33" s="94"/>
-      <c r="AS33" s="94"/>
-      <c r="AT33" s="94"/>
-      <c r="AU33" s="95"/>
+      <c r="AI33" s="83"/>
+      <c r="AJ33" s="83"/>
+      <c r="AK33" s="83"/>
+      <c r="AL33" s="83"/>
+      <c r="AM33" s="83"/>
+      <c r="AN33" s="83"/>
+      <c r="AO33" s="83"/>
+      <c r="AP33" s="83"/>
+      <c r="AQ33" s="83"/>
+      <c r="AR33" s="83"/>
+      <c r="AS33" s="83"/>
+      <c r="AT33" s="83"/>
+      <c r="AU33" s="84"/>
       <c r="AV33" s="45"/>
       <c r="AW33" s="45"/>
       <c r="AX33" s="45"/>
@@ -2816,48 +2927,48 @@
       <c r="C34" s="20"/>
       <c r="D34" s="20"/>
       <c r="E34" s="20"/>
-      <c r="F34" s="107"/>
-      <c r="G34" s="75"/>
-      <c r="H34" s="75"/>
-      <c r="I34" s="75"/>
-      <c r="J34" s="75"/>
-      <c r="K34" s="75"/>
-      <c r="L34" s="75"/>
-      <c r="M34" s="75"/>
-      <c r="N34" s="75"/>
-      <c r="O34" s="75"/>
-      <c r="P34" s="75"/>
-      <c r="Q34" s="75"/>
-      <c r="R34" s="75"/>
-      <c r="S34" s="108"/>
-      <c r="T34" s="107"/>
-      <c r="U34" s="75"/>
-      <c r="V34" s="75"/>
-      <c r="W34" s="75"/>
-      <c r="X34" s="75"/>
-      <c r="Y34" s="75"/>
-      <c r="Z34" s="75"/>
-      <c r="AA34" s="75"/>
-      <c r="AB34" s="75"/>
-      <c r="AC34" s="75"/>
-      <c r="AD34" s="75"/>
-      <c r="AE34" s="75"/>
-      <c r="AF34" s="75"/>
-      <c r="AG34" s="108"/>
-      <c r="AH34" s="107"/>
-      <c r="AI34" s="75"/>
-      <c r="AJ34" s="75"/>
-      <c r="AK34" s="75"/>
-      <c r="AL34" s="75"/>
-      <c r="AM34" s="75"/>
-      <c r="AN34" s="75"/>
-      <c r="AO34" s="75"/>
-      <c r="AP34" s="75"/>
-      <c r="AQ34" s="75"/>
-      <c r="AR34" s="75"/>
-      <c r="AS34" s="75"/>
-      <c r="AT34" s="75"/>
-      <c r="AU34" s="108"/>
+      <c r="F34" s="127"/>
+      <c r="G34" s="128"/>
+      <c r="H34" s="128"/>
+      <c r="I34" s="128"/>
+      <c r="J34" s="128"/>
+      <c r="K34" s="128"/>
+      <c r="L34" s="128"/>
+      <c r="M34" s="128"/>
+      <c r="N34" s="128"/>
+      <c r="O34" s="128"/>
+      <c r="P34" s="128"/>
+      <c r="Q34" s="128"/>
+      <c r="R34" s="128"/>
+      <c r="S34" s="129"/>
+      <c r="T34" s="127"/>
+      <c r="U34" s="128"/>
+      <c r="V34" s="128"/>
+      <c r="W34" s="128"/>
+      <c r="X34" s="128"/>
+      <c r="Y34" s="128"/>
+      <c r="Z34" s="128"/>
+      <c r="AA34" s="128"/>
+      <c r="AB34" s="128"/>
+      <c r="AC34" s="128"/>
+      <c r="AD34" s="128"/>
+      <c r="AE34" s="128"/>
+      <c r="AF34" s="128"/>
+      <c r="AG34" s="129"/>
+      <c r="AH34" s="127"/>
+      <c r="AI34" s="128"/>
+      <c r="AJ34" s="128"/>
+      <c r="AK34" s="128"/>
+      <c r="AL34" s="128"/>
+      <c r="AM34" s="128"/>
+      <c r="AN34" s="128"/>
+      <c r="AO34" s="128"/>
+      <c r="AP34" s="128"/>
+      <c r="AQ34" s="128"/>
+      <c r="AR34" s="128"/>
+      <c r="AS34" s="128"/>
+      <c r="AT34" s="128"/>
+      <c r="AU34" s="129"/>
       <c r="AV34" s="20"/>
       <c r="AW34" s="20"/>
       <c r="AX34" s="20"/>
@@ -2871,48 +2982,48 @@
       <c r="C35" s="20"/>
       <c r="D35" s="20"/>
       <c r="E35" s="20"/>
-      <c r="F35" s="109"/>
-      <c r="G35" s="86"/>
-      <c r="H35" s="86"/>
-      <c r="I35" s="86"/>
-      <c r="J35" s="86"/>
-      <c r="K35" s="86"/>
-      <c r="L35" s="86"/>
-      <c r="M35" s="86"/>
-      <c r="N35" s="86"/>
-      <c r="O35" s="86"/>
-      <c r="P35" s="86"/>
-      <c r="Q35" s="86"/>
-      <c r="R35" s="86"/>
-      <c r="S35" s="102"/>
-      <c r="T35" s="109"/>
-      <c r="U35" s="86"/>
-      <c r="V35" s="86"/>
-      <c r="W35" s="86"/>
-      <c r="X35" s="86"/>
-      <c r="Y35" s="86"/>
-      <c r="Z35" s="86"/>
-      <c r="AA35" s="86"/>
-      <c r="AB35" s="86"/>
-      <c r="AC35" s="86"/>
-      <c r="AD35" s="86"/>
-      <c r="AE35" s="86"/>
-      <c r="AF35" s="86"/>
-      <c r="AG35" s="102"/>
-      <c r="AH35" s="109"/>
-      <c r="AI35" s="86"/>
-      <c r="AJ35" s="86"/>
-      <c r="AK35" s="86"/>
-      <c r="AL35" s="86"/>
-      <c r="AM35" s="86"/>
-      <c r="AN35" s="86"/>
-      <c r="AO35" s="86"/>
-      <c r="AP35" s="86"/>
-      <c r="AQ35" s="86"/>
-      <c r="AR35" s="86"/>
-      <c r="AS35" s="86"/>
-      <c r="AT35" s="86"/>
-      <c r="AU35" s="102"/>
+      <c r="F35" s="130"/>
+      <c r="G35" s="20"/>
+      <c r="H35" s="20"/>
+      <c r="I35" s="20"/>
+      <c r="J35" s="20"/>
+      <c r="K35" s="20"/>
+      <c r="L35" s="20"/>
+      <c r="M35" s="20"/>
+      <c r="N35" s="20"/>
+      <c r="O35" s="20"/>
+      <c r="P35" s="20"/>
+      <c r="Q35" s="20"/>
+      <c r="R35" s="20"/>
+      <c r="S35" s="131"/>
+      <c r="T35" s="130"/>
+      <c r="U35" s="20"/>
+      <c r="V35" s="20"/>
+      <c r="W35" s="20"/>
+      <c r="X35" s="20"/>
+      <c r="Y35" s="20"/>
+      <c r="Z35" s="20"/>
+      <c r="AA35" s="20"/>
+      <c r="AB35" s="20"/>
+      <c r="AC35" s="20"/>
+      <c r="AD35" s="20"/>
+      <c r="AE35" s="20"/>
+      <c r="AF35" s="20"/>
+      <c r="AG35" s="131"/>
+      <c r="AH35" s="130"/>
+      <c r="AI35" s="20"/>
+      <c r="AJ35" s="20"/>
+      <c r="AK35" s="20"/>
+      <c r="AL35" s="20"/>
+      <c r="AM35" s="20"/>
+      <c r="AN35" s="20"/>
+      <c r="AO35" s="20"/>
+      <c r="AP35" s="20"/>
+      <c r="AQ35" s="20"/>
+      <c r="AR35" s="20"/>
+      <c r="AS35" s="20"/>
+      <c r="AT35" s="20"/>
+      <c r="AU35" s="131"/>
       <c r="AV35" s="20"/>
       <c r="AW35" s="20"/>
       <c r="AX35" s="20"/>
@@ -2920,54 +3031,54 @@
       <c r="AZ35" s="20"/>
       <c r="BA35" s="20"/>
     </row>
-    <row r="36" spans="1:53" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:53" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="20"/>
       <c r="B36" s="20"/>
       <c r="C36" s="20"/>
       <c r="D36" s="20"/>
       <c r="E36" s="20"/>
-      <c r="F36" s="110"/>
-      <c r="G36" s="111"/>
-      <c r="H36" s="111"/>
-      <c r="I36" s="111"/>
-      <c r="J36" s="111"/>
-      <c r="K36" s="111"/>
-      <c r="L36" s="111"/>
-      <c r="M36" s="111"/>
-      <c r="N36" s="111"/>
-      <c r="O36" s="111"/>
-      <c r="P36" s="111"/>
-      <c r="Q36" s="111"/>
-      <c r="R36" s="111"/>
-      <c r="S36" s="112"/>
-      <c r="T36" s="110"/>
-      <c r="U36" s="111"/>
-      <c r="V36" s="111"/>
-      <c r="W36" s="111"/>
-      <c r="X36" s="111"/>
-      <c r="Y36" s="111"/>
-      <c r="Z36" s="111"/>
-      <c r="AA36" s="111"/>
-      <c r="AB36" s="111"/>
-      <c r="AC36" s="111"/>
-      <c r="AD36" s="111"/>
-      <c r="AE36" s="111"/>
-      <c r="AF36" s="111"/>
-      <c r="AG36" s="112"/>
-      <c r="AH36" s="110"/>
-      <c r="AI36" s="111"/>
-      <c r="AJ36" s="111"/>
-      <c r="AK36" s="111"/>
-      <c r="AL36" s="111"/>
-      <c r="AM36" s="111"/>
-      <c r="AN36" s="111"/>
-      <c r="AO36" s="111"/>
-      <c r="AP36" s="111"/>
-      <c r="AQ36" s="111"/>
-      <c r="AR36" s="111"/>
-      <c r="AS36" s="111"/>
-      <c r="AT36" s="111"/>
-      <c r="AU36" s="112"/>
+      <c r="F36" s="130"/>
+      <c r="G36" s="20"/>
+      <c r="H36" s="20"/>
+      <c r="I36" s="20"/>
+      <c r="J36" s="20"/>
+      <c r="K36" s="20"/>
+      <c r="L36" s="20"/>
+      <c r="M36" s="20"/>
+      <c r="N36" s="20"/>
+      <c r="O36" s="20"/>
+      <c r="P36" s="20"/>
+      <c r="Q36" s="20"/>
+      <c r="R36" s="20"/>
+      <c r="S36" s="131"/>
+      <c r="T36" s="130"/>
+      <c r="U36" s="20"/>
+      <c r="V36" s="20"/>
+      <c r="W36" s="20"/>
+      <c r="X36" s="20"/>
+      <c r="Y36" s="20"/>
+      <c r="Z36" s="20"/>
+      <c r="AA36" s="20"/>
+      <c r="AB36" s="20"/>
+      <c r="AC36" s="20"/>
+      <c r="AD36" s="20"/>
+      <c r="AE36" s="20"/>
+      <c r="AF36" s="20"/>
+      <c r="AG36" s="131"/>
+      <c r="AH36" s="130"/>
+      <c r="AI36" s="20"/>
+      <c r="AJ36" s="20"/>
+      <c r="AK36" s="20"/>
+      <c r="AL36" s="20"/>
+      <c r="AM36" s="20"/>
+      <c r="AN36" s="20"/>
+      <c r="AO36" s="20"/>
+      <c r="AP36" s="20"/>
+      <c r="AQ36" s="20"/>
+      <c r="AR36" s="20"/>
+      <c r="AS36" s="20"/>
+      <c r="AT36" s="20"/>
+      <c r="AU36" s="131"/>
       <c r="AV36" s="20"/>
       <c r="AW36" s="20"/>
       <c r="AX36" s="20"/>
@@ -2975,54 +3086,54 @@
       <c r="AZ36" s="20"/>
       <c r="BA36" s="20"/>
     </row>
-    <row r="37" spans="1:53" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:53" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="20"/>
       <c r="B37" s="20"/>
       <c r="C37" s="20"/>
       <c r="D37" s="20"/>
       <c r="E37" s="20"/>
-      <c r="F37" s="93"/>
-      <c r="G37" s="94"/>
-      <c r="H37" s="94"/>
-      <c r="I37" s="94"/>
-      <c r="J37" s="94"/>
-      <c r="K37" s="94"/>
-      <c r="L37" s="94"/>
-      <c r="M37" s="94"/>
-      <c r="N37" s="94"/>
-      <c r="O37" s="94"/>
-      <c r="P37" s="94"/>
-      <c r="Q37" s="94"/>
-      <c r="R37" s="94"/>
-      <c r="S37" s="95"/>
-      <c r="T37" s="97"/>
-      <c r="U37" s="94"/>
-      <c r="V37" s="94"/>
-      <c r="W37" s="94"/>
-      <c r="X37" s="94"/>
-      <c r="Y37" s="94"/>
-      <c r="Z37" s="94"/>
-      <c r="AA37" s="94"/>
-      <c r="AB37" s="94"/>
-      <c r="AC37" s="94"/>
-      <c r="AD37" s="94"/>
-      <c r="AE37" s="94"/>
-      <c r="AF37" s="94"/>
-      <c r="AG37" s="95"/>
-      <c r="AH37" s="93"/>
-      <c r="AI37" s="94"/>
-      <c r="AJ37" s="94"/>
-      <c r="AK37" s="94"/>
-      <c r="AL37" s="94"/>
-      <c r="AM37" s="94"/>
-      <c r="AN37" s="94"/>
-      <c r="AO37" s="94"/>
-      <c r="AP37" s="94"/>
-      <c r="AQ37" s="94"/>
-      <c r="AR37" s="94"/>
-      <c r="AS37" s="94"/>
-      <c r="AT37" s="94"/>
-      <c r="AU37" s="95"/>
+      <c r="F37" s="130"/>
+      <c r="G37" s="20"/>
+      <c r="H37" s="20"/>
+      <c r="I37" s="20"/>
+      <c r="J37" s="20"/>
+      <c r="K37" s="20"/>
+      <c r="L37" s="20"/>
+      <c r="M37" s="20"/>
+      <c r="N37" s="20"/>
+      <c r="O37" s="20"/>
+      <c r="P37" s="20"/>
+      <c r="Q37" s="20"/>
+      <c r="R37" s="20"/>
+      <c r="S37" s="131"/>
+      <c r="T37" s="130"/>
+      <c r="U37" s="20"/>
+      <c r="V37" s="20"/>
+      <c r="W37" s="20"/>
+      <c r="X37" s="20"/>
+      <c r="Y37" s="20"/>
+      <c r="Z37" s="20"/>
+      <c r="AA37" s="20"/>
+      <c r="AB37" s="20"/>
+      <c r="AC37" s="20"/>
+      <c r="AD37" s="20"/>
+      <c r="AE37" s="20"/>
+      <c r="AF37" s="20"/>
+      <c r="AG37" s="131"/>
+      <c r="AH37" s="130"/>
+      <c r="AI37" s="20"/>
+      <c r="AJ37" s="20"/>
+      <c r="AK37" s="20"/>
+      <c r="AL37" s="20"/>
+      <c r="AM37" s="20"/>
+      <c r="AN37" s="20"/>
+      <c r="AO37" s="20"/>
+      <c r="AP37" s="20"/>
+      <c r="AQ37" s="20"/>
+      <c r="AR37" s="20"/>
+      <c r="AS37" s="20"/>
+      <c r="AT37" s="20"/>
+      <c r="AU37" s="131"/>
       <c r="AV37" s="20"/>
       <c r="AW37" s="20"/>
       <c r="AX37" s="20"/>
@@ -3030,62 +3141,54 @@
       <c r="AZ37" s="20"/>
       <c r="BA37" s="20"/>
     </row>
-    <row r="38" spans="1:53" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:53" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="20"/>
       <c r="B38" s="20"/>
       <c r="C38" s="20"/>
       <c r="D38" s="20"/>
       <c r="E38" s="20"/>
-      <c r="F38" s="93" t="s">
-        <v>24</v>
-      </c>
-      <c r="G38" s="94"/>
-      <c r="H38" s="94"/>
-      <c r="I38" s="96"/>
-      <c r="J38" s="94"/>
-      <c r="K38" s="94"/>
-      <c r="L38" s="94"/>
-      <c r="M38" s="94"/>
-      <c r="N38" s="94"/>
-      <c r="O38" s="94"/>
-      <c r="P38" s="94"/>
-      <c r="Q38" s="94"/>
-      <c r="R38" s="94"/>
-      <c r="S38" s="95"/>
-      <c r="T38" s="46" t="str">
-        <f>F38</f>
-        <v xml:space="preserve">Date : </v>
-      </c>
-      <c r="U38" s="96"/>
-      <c r="V38" s="94"/>
-      <c r="W38" s="94"/>
-      <c r="X38" s="94"/>
-      <c r="Y38" s="94"/>
-      <c r="Z38" s="94"/>
-      <c r="AA38" s="94"/>
-      <c r="AB38" s="94"/>
-      <c r="AC38" s="94"/>
-      <c r="AD38" s="94"/>
-      <c r="AE38" s="94"/>
-      <c r="AF38" s="94"/>
-      <c r="AG38" s="95"/>
-      <c r="AH38" s="93" t="str">
-        <f>F38</f>
-        <v xml:space="preserve">Date : </v>
-      </c>
-      <c r="AI38" s="94"/>
-      <c r="AJ38" s="96"/>
-      <c r="AK38" s="94"/>
-      <c r="AL38" s="94"/>
-      <c r="AM38" s="94"/>
-      <c r="AN38" s="94"/>
-      <c r="AO38" s="94"/>
-      <c r="AP38" s="94"/>
-      <c r="AQ38" s="94"/>
-      <c r="AR38" s="94"/>
-      <c r="AS38" s="94"/>
-      <c r="AT38" s="94"/>
-      <c r="AU38" s="95"/>
+      <c r="F38" s="130"/>
+      <c r="G38" s="20"/>
+      <c r="H38" s="20"/>
+      <c r="I38" s="20"/>
+      <c r="J38" s="20"/>
+      <c r="K38" s="20"/>
+      <c r="L38" s="20"/>
+      <c r="M38" s="20"/>
+      <c r="N38" s="20"/>
+      <c r="O38" s="20"/>
+      <c r="P38" s="20"/>
+      <c r="Q38" s="20"/>
+      <c r="R38" s="20"/>
+      <c r="S38" s="131"/>
+      <c r="T38" s="130"/>
+      <c r="U38" s="20"/>
+      <c r="V38" s="20"/>
+      <c r="W38" s="20"/>
+      <c r="X38" s="20"/>
+      <c r="Y38" s="20"/>
+      <c r="Z38" s="20"/>
+      <c r="AA38" s="20"/>
+      <c r="AB38" s="20"/>
+      <c r="AC38" s="20"/>
+      <c r="AD38" s="20"/>
+      <c r="AE38" s="20"/>
+      <c r="AF38" s="20"/>
+      <c r="AG38" s="131"/>
+      <c r="AH38" s="130"/>
+      <c r="AI38" s="20"/>
+      <c r="AJ38" s="20"/>
+      <c r="AK38" s="20"/>
+      <c r="AL38" s="20"/>
+      <c r="AM38" s="20"/>
+      <c r="AN38" s="20"/>
+      <c r="AO38" s="20"/>
+      <c r="AP38" s="20"/>
+      <c r="AQ38" s="20"/>
+      <c r="AR38" s="20"/>
+      <c r="AS38" s="20"/>
+      <c r="AT38" s="20"/>
+      <c r="AU38" s="131"/>
       <c r="AV38" s="16"/>
       <c r="AW38" s="16"/>
       <c r="AX38" s="16"/>
@@ -3099,48 +3202,48 @@
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
-      <c r="F39" s="2"/>
-      <c r="G39" s="2"/>
-      <c r="H39" s="2"/>
-      <c r="I39" s="2"/>
-      <c r="J39" s="2"/>
-      <c r="K39" s="2"/>
-      <c r="L39" s="2"/>
-      <c r="M39" s="2"/>
-      <c r="N39" s="2"/>
-      <c r="O39" s="2"/>
-      <c r="P39" s="2"/>
-      <c r="Q39" s="2"/>
-      <c r="R39" s="2"/>
-      <c r="S39" s="2"/>
-      <c r="T39" s="2"/>
-      <c r="U39" s="2"/>
-      <c r="V39" s="2"/>
-      <c r="W39" s="2"/>
-      <c r="X39" s="2"/>
-      <c r="Y39" s="2"/>
-      <c r="Z39" s="2"/>
-      <c r="AA39" s="2"/>
-      <c r="AB39" s="2"/>
-      <c r="AC39" s="2"/>
-      <c r="AD39" s="2"/>
-      <c r="AE39" s="2"/>
-      <c r="AF39" s="2"/>
-      <c r="AG39" s="2"/>
-      <c r="AH39" s="2"/>
-      <c r="AI39" s="2"/>
-      <c r="AJ39" s="2"/>
-      <c r="AK39" s="2"/>
-      <c r="AL39" s="2"/>
-      <c r="AM39" s="2"/>
-      <c r="AN39" s="2"/>
-      <c r="AO39" s="2"/>
-      <c r="AP39" s="2"/>
-      <c r="AQ39" s="2"/>
-      <c r="AR39" s="2"/>
-      <c r="AS39" s="2"/>
-      <c r="AT39" s="2"/>
-      <c r="AU39" s="2"/>
+      <c r="F39" s="130"/>
+      <c r="G39" s="20"/>
+      <c r="H39" s="20"/>
+      <c r="I39" s="20"/>
+      <c r="J39" s="20"/>
+      <c r="K39" s="20"/>
+      <c r="L39" s="20"/>
+      <c r="M39" s="20"/>
+      <c r="N39" s="20"/>
+      <c r="O39" s="20"/>
+      <c r="P39" s="20"/>
+      <c r="Q39" s="20"/>
+      <c r="R39" s="20"/>
+      <c r="S39" s="131"/>
+      <c r="T39" s="130"/>
+      <c r="U39" s="20"/>
+      <c r="V39" s="20"/>
+      <c r="W39" s="20"/>
+      <c r="X39" s="20"/>
+      <c r="Y39" s="20"/>
+      <c r="Z39" s="20"/>
+      <c r="AA39" s="20"/>
+      <c r="AB39" s="20"/>
+      <c r="AC39" s="20"/>
+      <c r="AD39" s="20"/>
+      <c r="AE39" s="20"/>
+      <c r="AF39" s="20"/>
+      <c r="AG39" s="131"/>
+      <c r="AH39" s="130"/>
+      <c r="AI39" s="20"/>
+      <c r="AJ39" s="20"/>
+      <c r="AK39" s="20"/>
+      <c r="AL39" s="20"/>
+      <c r="AM39" s="20"/>
+      <c r="AN39" s="20"/>
+      <c r="AO39" s="20"/>
+      <c r="AP39" s="20"/>
+      <c r="AQ39" s="20"/>
+      <c r="AR39" s="20"/>
+      <c r="AS39" s="20"/>
+      <c r="AT39" s="20"/>
+      <c r="AU39" s="131"/>
       <c r="AV39" s="2"/>
       <c r="AW39" s="2"/>
       <c r="AX39" s="2"/>
@@ -3148,54 +3251,54 @@
       <c r="AZ39" s="2"/>
       <c r="BA39" s="2"/>
     </row>
-    <row r="40" spans="1:53" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:53" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
       <c r="E40" s="2"/>
-      <c r="F40" s="2"/>
-      <c r="G40" s="2"/>
-      <c r="H40" s="2"/>
-      <c r="I40" s="2"/>
-      <c r="J40" s="2"/>
-      <c r="K40" s="2"/>
-      <c r="L40" s="2"/>
-      <c r="M40" s="2"/>
-      <c r="N40" s="2"/>
-      <c r="O40" s="2"/>
-      <c r="P40" s="2"/>
-      <c r="Q40" s="2"/>
-      <c r="R40" s="2"/>
-      <c r="S40" s="2"/>
-      <c r="T40" s="2"/>
-      <c r="U40" s="2"/>
-      <c r="V40" s="2"/>
-      <c r="W40" s="2"/>
-      <c r="X40" s="2"/>
-      <c r="Y40" s="2"/>
-      <c r="Z40" s="2"/>
-      <c r="AA40" s="2"/>
-      <c r="AB40" s="2"/>
-      <c r="AC40" s="2"/>
-      <c r="AD40" s="2"/>
-      <c r="AE40" s="2"/>
-      <c r="AF40" s="2"/>
-      <c r="AG40" s="2"/>
-      <c r="AH40" s="2"/>
-      <c r="AI40" s="2"/>
-      <c r="AJ40" s="2"/>
-      <c r="AK40" s="2"/>
-      <c r="AL40" s="2"/>
-      <c r="AM40" s="2"/>
-      <c r="AN40" s="2"/>
-      <c r="AO40" s="2"/>
-      <c r="AP40" s="2"/>
-      <c r="AQ40" s="2"/>
-      <c r="AR40" s="2"/>
-      <c r="AS40" s="2"/>
-      <c r="AT40" s="2"/>
-      <c r="AU40" s="2"/>
+      <c r="F40" s="132"/>
+      <c r="G40" s="133"/>
+      <c r="H40" s="133"/>
+      <c r="I40" s="133"/>
+      <c r="J40" s="133"/>
+      <c r="K40" s="133"/>
+      <c r="L40" s="133"/>
+      <c r="M40" s="133"/>
+      <c r="N40" s="133"/>
+      <c r="O40" s="133"/>
+      <c r="P40" s="133"/>
+      <c r="Q40" s="133"/>
+      <c r="R40" s="133"/>
+      <c r="S40" s="134"/>
+      <c r="T40" s="132"/>
+      <c r="U40" s="133"/>
+      <c r="V40" s="133"/>
+      <c r="W40" s="133"/>
+      <c r="X40" s="133"/>
+      <c r="Y40" s="133"/>
+      <c r="Z40" s="133"/>
+      <c r="AA40" s="133"/>
+      <c r="AB40" s="133"/>
+      <c r="AC40" s="133"/>
+      <c r="AD40" s="133"/>
+      <c r="AE40" s="133"/>
+      <c r="AF40" s="133"/>
+      <c r="AG40" s="134"/>
+      <c r="AH40" s="132"/>
+      <c r="AI40" s="133"/>
+      <c r="AJ40" s="133"/>
+      <c r="AK40" s="133"/>
+      <c r="AL40" s="133"/>
+      <c r="AM40" s="133"/>
+      <c r="AN40" s="133"/>
+      <c r="AO40" s="133"/>
+      <c r="AP40" s="133"/>
+      <c r="AQ40" s="133"/>
+      <c r="AR40" s="133"/>
+      <c r="AS40" s="133"/>
+      <c r="AT40" s="133"/>
+      <c r="AU40" s="134"/>
       <c r="AV40" s="2"/>
       <c r="AW40" s="2"/>
       <c r="AX40" s="2"/>
@@ -3203,54 +3306,54 @@
       <c r="AZ40" s="2"/>
       <c r="BA40" s="2"/>
     </row>
-    <row r="41" spans="1:53" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:53" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
       <c r="E41" s="2"/>
-      <c r="F41" s="2"/>
-      <c r="G41" s="2"/>
-      <c r="H41" s="2"/>
-      <c r="I41" s="2"/>
-      <c r="J41" s="2"/>
-      <c r="K41" s="2"/>
-      <c r="L41" s="2"/>
-      <c r="M41" s="2"/>
-      <c r="N41" s="2"/>
-      <c r="O41" s="2"/>
-      <c r="P41" s="2"/>
-      <c r="Q41" s="2"/>
-      <c r="R41" s="2"/>
-      <c r="S41" s="2"/>
-      <c r="T41" s="2"/>
-      <c r="U41" s="2"/>
-      <c r="V41" s="2"/>
-      <c r="W41" s="2"/>
-      <c r="X41" s="2"/>
-      <c r="Y41" s="2"/>
-      <c r="Z41" s="2"/>
-      <c r="AA41" s="2"/>
-      <c r="AB41" s="2"/>
-      <c r="AC41" s="2"/>
-      <c r="AD41" s="2"/>
-      <c r="AE41" s="2"/>
-      <c r="AF41" s="2"/>
-      <c r="AG41" s="2"/>
-      <c r="AH41" s="2"/>
-      <c r="AI41" s="2"/>
-      <c r="AJ41" s="2"/>
-      <c r="AK41" s="2"/>
-      <c r="AL41" s="2"/>
-      <c r="AM41" s="2"/>
-      <c r="AN41" s="2"/>
-      <c r="AO41" s="2"/>
-      <c r="AP41" s="2"/>
-      <c r="AQ41" s="2"/>
-      <c r="AR41" s="2"/>
-      <c r="AS41" s="2"/>
-      <c r="AT41" s="2"/>
-      <c r="AU41" s="2"/>
+      <c r="F41" s="135"/>
+      <c r="G41" s="136"/>
+      <c r="H41" s="136"/>
+      <c r="I41" s="136"/>
+      <c r="J41" s="136"/>
+      <c r="K41" s="136"/>
+      <c r="L41" s="136"/>
+      <c r="M41" s="136"/>
+      <c r="N41" s="136"/>
+      <c r="O41" s="136"/>
+      <c r="P41" s="136"/>
+      <c r="Q41" s="136"/>
+      <c r="R41" s="136"/>
+      <c r="S41" s="137"/>
+      <c r="T41" s="138"/>
+      <c r="U41" s="136"/>
+      <c r="V41" s="136"/>
+      <c r="W41" s="136"/>
+      <c r="X41" s="136"/>
+      <c r="Y41" s="136"/>
+      <c r="Z41" s="136"/>
+      <c r="AA41" s="136"/>
+      <c r="AB41" s="136"/>
+      <c r="AC41" s="136"/>
+      <c r="AD41" s="136"/>
+      <c r="AE41" s="136"/>
+      <c r="AF41" s="136"/>
+      <c r="AG41" s="137"/>
+      <c r="AH41" s="135"/>
+      <c r="AI41" s="136"/>
+      <c r="AJ41" s="136"/>
+      <c r="AK41" s="136"/>
+      <c r="AL41" s="136"/>
+      <c r="AM41" s="136"/>
+      <c r="AN41" s="136"/>
+      <c r="AO41" s="136"/>
+      <c r="AP41" s="136"/>
+      <c r="AQ41" s="136"/>
+      <c r="AR41" s="136"/>
+      <c r="AS41" s="136"/>
+      <c r="AT41" s="136"/>
+      <c r="AU41" s="137"/>
       <c r="AV41" s="2"/>
       <c r="AW41" s="2"/>
       <c r="AX41" s="2"/>
@@ -3258,54 +3361,61 @@
       <c r="AZ41" s="2"/>
       <c r="BA41" s="2"/>
     </row>
-    <row r="42" spans="1:53" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:53" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>
-      <c r="F42" s="2"/>
-      <c r="G42" s="2"/>
-      <c r="H42" s="2"/>
-      <c r="I42" s="2"/>
-      <c r="J42" s="2"/>
-      <c r="K42" s="2"/>
-      <c r="L42" s="2"/>
-      <c r="M42" s="2"/>
-      <c r="N42" s="2"/>
-      <c r="O42" s="2"/>
-      <c r="P42" s="2"/>
-      <c r="Q42" s="2"/>
-      <c r="R42" s="2"/>
-      <c r="S42" s="2"/>
-      <c r="T42" s="2"/>
-      <c r="U42" s="2"/>
-      <c r="V42" s="2"/>
-      <c r="W42" s="2"/>
-      <c r="X42" s="2"/>
-      <c r="Y42" s="2"/>
-      <c r="Z42" s="2"/>
-      <c r="AA42" s="2"/>
-      <c r="AB42" s="2"/>
-      <c r="AC42" s="2"/>
-      <c r="AD42" s="2"/>
-      <c r="AE42" s="2"/>
-      <c r="AF42" s="2"/>
-      <c r="AG42" s="2"/>
-      <c r="AH42" s="2"/>
-      <c r="AI42" s="2"/>
-      <c r="AJ42" s="2"/>
-      <c r="AK42" s="2"/>
-      <c r="AL42" s="2"/>
-      <c r="AM42" s="2"/>
-      <c r="AN42" s="2"/>
-      <c r="AO42" s="2"/>
-      <c r="AP42" s="2"/>
-      <c r="AQ42" s="2"/>
-      <c r="AR42" s="2"/>
-      <c r="AS42" s="2"/>
-      <c r="AT42" s="2"/>
-      <c r="AU42" s="2"/>
+      <c r="F42" s="99" t="s">
+        <v>24</v>
+      </c>
+      <c r="G42" s="100"/>
+      <c r="H42" s="100"/>
+      <c r="I42" s="139"/>
+      <c r="J42" s="140"/>
+      <c r="K42" s="140"/>
+      <c r="L42" s="140"/>
+      <c r="M42" s="140"/>
+      <c r="N42" s="140"/>
+      <c r="O42" s="140"/>
+      <c r="P42" s="140"/>
+      <c r="Q42" s="140"/>
+      <c r="R42" s="141"/>
+      <c r="S42" s="142"/>
+      <c r="T42" s="125" t="str">
+        <f>AH42</f>
+        <v>Date :</v>
+      </c>
+      <c r="U42" s="139"/>
+      <c r="V42" s="140"/>
+      <c r="W42" s="140"/>
+      <c r="X42" s="140"/>
+      <c r="Y42" s="140"/>
+      <c r="Z42" s="140"/>
+      <c r="AA42" s="140"/>
+      <c r="AB42" s="140"/>
+      <c r="AC42" s="140"/>
+      <c r="AD42" s="140"/>
+      <c r="AE42" s="140"/>
+      <c r="AF42" s="140"/>
+      <c r="AG42" s="142"/>
+      <c r="AH42" s="126" t="s">
+        <v>30</v>
+      </c>
+      <c r="AI42" s="100"/>
+      <c r="AJ42" s="139"/>
+      <c r="AK42" s="140"/>
+      <c r="AL42" s="140"/>
+      <c r="AM42" s="140"/>
+      <c r="AN42" s="140"/>
+      <c r="AO42" s="140"/>
+      <c r="AP42" s="140"/>
+      <c r="AQ42" s="140"/>
+      <c r="AR42" s="140"/>
+      <c r="AS42" s="140"/>
+      <c r="AT42" s="140"/>
+      <c r="AU42" s="142"/>
       <c r="AV42" s="2"/>
       <c r="AW42" s="2"/>
       <c r="AX42" s="2"/>
@@ -56004,48 +56114,9 @@
       <c r="BA1000" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="50">
-    <mergeCell ref="AV17:BA17"/>
-    <mergeCell ref="AV18:BA18"/>
-    <mergeCell ref="AV19:BA19"/>
-    <mergeCell ref="U12:AU12"/>
-    <mergeCell ref="AV12:BA13"/>
-    <mergeCell ref="U13:AH13"/>
-    <mergeCell ref="AI13:AU13"/>
-    <mergeCell ref="AV16:BA16"/>
-    <mergeCell ref="A1:BA1"/>
-    <mergeCell ref="A2:BA2"/>
-    <mergeCell ref="A6:D6"/>
-    <mergeCell ref="A7:E7"/>
-    <mergeCell ref="A11:D11"/>
-    <mergeCell ref="AA4:AC4"/>
-    <mergeCell ref="AH37:AU37"/>
-    <mergeCell ref="U38:AG38"/>
-    <mergeCell ref="AH38:AI38"/>
-    <mergeCell ref="AJ38:AU38"/>
-    <mergeCell ref="AV20:BA20"/>
-    <mergeCell ref="AV23:BA23"/>
-    <mergeCell ref="AV26:BA26"/>
-    <mergeCell ref="AV29:BA29"/>
-    <mergeCell ref="AV31:BA31"/>
-    <mergeCell ref="T33:AG33"/>
-    <mergeCell ref="T34:AG36"/>
-    <mergeCell ref="R31:T31"/>
-    <mergeCell ref="AH33:AU33"/>
-    <mergeCell ref="AH34:AU36"/>
-    <mergeCell ref="F33:S33"/>
-    <mergeCell ref="F34:S36"/>
-    <mergeCell ref="F37:S37"/>
-    <mergeCell ref="F38:H38"/>
-    <mergeCell ref="I38:S38"/>
-    <mergeCell ref="T37:AG37"/>
-    <mergeCell ref="B14:Q14"/>
-    <mergeCell ref="B18:Q18"/>
-    <mergeCell ref="R19:T19"/>
-    <mergeCell ref="R23:T23"/>
-    <mergeCell ref="R26:T26"/>
-    <mergeCell ref="R27:T27"/>
-    <mergeCell ref="R20:T20"/>
+  <mergeCells count="41">
+    <mergeCell ref="F42:H42"/>
+    <mergeCell ref="AH42:AI42"/>
     <mergeCell ref="A12:Q13"/>
     <mergeCell ref="R12:T13"/>
     <mergeCell ref="R14:T14"/>
@@ -56055,6 +56126,36 @@
     <mergeCell ref="R16:T16"/>
     <mergeCell ref="R17:T17"/>
     <mergeCell ref="R18:T18"/>
+    <mergeCell ref="B14:Q14"/>
+    <mergeCell ref="B18:Q18"/>
+    <mergeCell ref="R19:T19"/>
+    <mergeCell ref="R23:T23"/>
+    <mergeCell ref="R26:T26"/>
+    <mergeCell ref="R27:T27"/>
+    <mergeCell ref="R20:T20"/>
+    <mergeCell ref="AV20:BA20"/>
+    <mergeCell ref="AV23:BA23"/>
+    <mergeCell ref="AV26:BA26"/>
+    <mergeCell ref="AV29:BA29"/>
+    <mergeCell ref="AV31:BA31"/>
+    <mergeCell ref="T33:AG33"/>
+    <mergeCell ref="R31:T31"/>
+    <mergeCell ref="AH33:AU33"/>
+    <mergeCell ref="F33:S33"/>
+    <mergeCell ref="A1:BA1"/>
+    <mergeCell ref="A2:BA2"/>
+    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="A7:E7"/>
+    <mergeCell ref="A11:D11"/>
+    <mergeCell ref="AA4:AC4"/>
+    <mergeCell ref="AV17:BA17"/>
+    <mergeCell ref="AV18:BA18"/>
+    <mergeCell ref="AV19:BA19"/>
+    <mergeCell ref="U12:AU12"/>
+    <mergeCell ref="AV12:BA13"/>
+    <mergeCell ref="U13:AH13"/>
+    <mergeCell ref="AI13:AU13"/>
+    <mergeCell ref="AV16:BA16"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>

</xml_diff>